<commit_message>
added new class ResultsExtractor(). processing the text extracted from the txt-file
</commit_message>
<xml_diff>
--- a/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
+++ b/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
@@ -14,7 +14,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+  <si>
+    <t>1 результат</t>
+  </si>
+  <si>
+    <t>2 результат</t>
+  </si>
+  <si>
+    <t>3 результат</t>
+  </si>
+  <si>
+    <t>4 результат</t>
+  </si>
+  <si>
+    <t>5 результат</t>
+  </si>
+  <si>
+    <t>6 результат</t>
+  </si>
+  <si>
+    <t>7 результат</t>
+  </si>
+  <si>
+    <t>8 результат</t>
+  </si>
+  <si>
+    <t>9 результат</t>
+  </si>
+  <si>
+    <t>10 результат</t>
+  </si>
+  <si>
+    <t>11 результат</t>
+  </si>
+  <si>
+    <t>12 результат</t>
+  </si>
+  <si>
+    <t>13 результат</t>
+  </si>
+  <si>
+    <t>14 результат</t>
+  </si>
+  <si>
+    <t>15 результат</t>
+  </si>
+  <si>
+    <t>16 результат</t>
+  </si>
+  <si>
+    <t>17 результат</t>
+  </si>
+  <si>
+    <t>18 результат</t>
+  </si>
+  <si>
+    <t>19 результат</t>
+  </si>
+  <si>
+    <t>20 результат</t>
+  </si>
+  <si>
+    <t>21 результат</t>
+  </si>
+  <si>
+    <t>22 результат</t>
+  </si>
+  <si>
+    <t>23 результат</t>
+  </si>
+  <si>
+    <t>24 результат</t>
+  </si>
+  <si>
+    <t>25 результат</t>
+  </si>
+  <si>
+    <t>26 результат</t>
+  </si>
+  <si>
+    <t>27 результат</t>
+  </si>
   <si>
     <t>22.09.2021 13:28:19 ----------
 Тест закончен...
@@ -36,6 +117,29 @@
 Маска времени обдумывания (в секундах): "1) 5 2) 7 ".
 Маска ответов: "1) 2; 2) 3; ".
 Маска штрафов за подсказку: "1) * 2) * ".
+Время начала: 13:28:05.
+Время завершения: 13:28:19.
+Продолжительность: 00:00:13</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:28:19 ----------
+Тест закончен...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "А кто кто кто"
+Название теста: ""
+Файл с тестом: "C:\Users\tabakaev_mv\Desktop\РАБОТА\ТЕСТЫ\MyTest\Безымянный.mtf"
+CRC Файла с тестом: "57C3A660"
+Всего заданий в тесте: 2.
+Выполнено заданий: 2.
+Из них правильно: 0 (0,0% выполненых заданий).
+Из них ошибок: 2 (100,0% выполненых заданий).
+Результативность: 0,0%.
+Использовано подсказок: 0.
+Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
+Оценка: 2.
+Маска результата: "1) - 2) - ".
+Маска времени обдумывания (в секундах): "1) 5 2) 7 ".
 Время начала: 13:28:05.
 Время завершения: 13:28:19.
 Продолжительность: 00:00:13</t>
@@ -66,6 +170,29 @@
 Продолжительность: 00:00:10</t>
   </si>
   <si>
+    <t>22.09.2021 13:29:13 ----------
+Тест закончен...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "Фамилия Имя"
+Название теста: ""
+Файл с тестом: "C:\Users\tabakaev_mv\Desktop\РАБОТА\ТЕСТЫ\MyTest\Безымянный.mtf"
+CRC Файла с тестом: "2598F9AC"
+Всего заданий в тесте: 2.
+Выполнено заданий: 2.
+Из них правильно: 2 (100,0% выполненых заданий).
+Из них ошибок: 0 (0,0% выполненых заданий).
+Результативность: 100,0%.
+Использовано подсказок: 0.
+Набрано баллов: 2,0 из 2 возможных. Ваш результат: 100,0%.
+Оценка: 5.
+Маска результата: "1) + 2) + ".
+Маска времени обдумывания (в секундах): "1) 6 2) 4 ".
+Время начала: 13:29:02.
+Время завершения: 13:29:13.
+Продолжительность: 00:00:10</t>
+  </si>
+  <si>
     <t>22.09.2021 13:47:58 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X04"
@@ -91,6 +218,29 @@
 Продолжительность: 00:00:06</t>
   </si>
   <si>
+    <t>22.09.2021 13:47:58 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X04"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "джлдлоогридл"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
+CRC Файла с тестом: "2598F9AC"
+Всего заданий в тесте: 2.
+Выполнено заданий: 2.
+Из них правильно: 2 (100,0% выполненых заданий).
+Из них ошибок: 0 (0,0% выполненых заданий).
+Результативность: 100,0%.
+Использовано подсказок: 0.
+Набрано баллов: 2,0 из 2 возможных. Ваш результат: 100,0%.
+Оценка: 5.
+Маска результата: "1) + 2) + ".
+Маска времени обдумывания (в секундах): "1) 3 2) 3 ".
+Время начала: 13:47:52.
+Время завершения: 13:47:58.
+Продолжительность: 00:00:06</t>
+  </si>
+  <si>
     <t>22.09.2021 13:48:39 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
@@ -111,6 +261,29 @@
 Маска времени обдумывания (в секундах): "1) 85 2) 1 ".
 Маска ответов: "1) 3; 2) 4; ".
 Маска штрафов за подсказку: "1) * 2) * ".
+Время начала: 13:47:11.
+Время завершения: 13:48:39.
+Продолжительность: 00:01:26</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:48:39 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X02"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "орпрдло"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
+CRC Файла с тестом: "2598F9AC"
+Всего заданий в тесте: 2.
+Выполнено заданий: 2.
+Из них правильно: 0 (0,0% выполненых заданий).
+Из них ошибок: 2 (100,0% выполненых заданий).
+Результативность: 0,0%.
+Использовано подсказок: 0.
+Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
+Оценка: 2.
+Маска результата: "1) - 2) - ".
+Маска времени обдумывания (в секундах): "1) 85 2) 1 ".
 Время начала: 13:47:11.
 Время завершения: 13:48:39.
 Продолжительность: 00:01:26</t>
@@ -141,6 +314,29 @@
 Продолжительность: 00:03:25</t>
   </si>
   <si>
+    <t>22.09.2021 13:49:01 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X01"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Петя"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
+CRC Файла с тестом: "2598F9AC"
+Всего заданий в тесте: 2.
+Выполнено заданий: 2.
+Из них правильно: 1 (50,0% выполненых заданий).
+Из них ошибок: 1 (50,0% выполненых заданий).
+Результативность: 50,0%.
+Использовано подсказок: 0.
+Набрано баллов: 1,0 из 2 возможных. Ваш результат: 50,0%.
+Оценка: 3.
+Маска результата: "1) - 2) + ".
+Маска времени обдумывания (в секундах): "1) 203 2) 1 ".
+Время начала: 13:45:32.
+Время завершения: 13:49:01.
+Продолжительность: 00:03:25</t>
+  </si>
+  <si>
     <t>22.09.2021 13:50:34 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K205-X09"
@@ -166,6 +362,29 @@
 Продолжительность: 00:05:37</t>
   </si>
   <si>
+    <t>22.09.2021 13:50:34 ----------
+Тест прерван - закрыта программа...
+Имя компьютера: "SHA-K205-X09"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Вася"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
+CRC Файла с тестом: "2598F9AC"
+Всего заданий в тесте: 2.
+Выполнено заданий: 1.
+Из них правильно: 0 (0,0% выполненых заданий).
+Из них ошибок: 0 (0,0% выполненых заданий).
+Результативность: 0,0%.
+Использовано подсказок: 0.
+Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
+Оценка: 2.
+Маска результата: "1) * 2) * ".
+Маска времени обдумывания (в секундах): "1) 337 2) * ".
+Время начала: 13:44:46.
+Время завершения: 13:50:34.
+Продолжительность: 00:05:37</t>
+  </si>
+  <si>
     <t>28.09.2021 10:43:58 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
@@ -191,6 +410,29 @@
 Продолжительность: 00:00:20</t>
   </si>
   <si>
+    <t>28.09.2021 10:43:58 ----------
+Тест закончен...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "оыважыва"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf"
+CRC Файла с тестом: "4F621F46"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 5 (16,7% выполненых заданий).
+Из них ошибок: 25 (83,3% выполненых заданий).
+Результативность: 16,7%.
+Использовано подсказок: 0.
+Набрано баллов: 5,0 из 30 возможных. Ваш результат: 16,7%.
+Оценка: 2.
+Маска результата: "1) - 2) - 3) + 4) - 5) + 6) - 7) - 8) - 9) - 10) - 11) - 12) - 13) - 14) - 15) - 16) - 17) - 18) - 19) + 20) - 21) + 22) - 23) - 24) - 25) + 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 1 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 1 25) 1 26) 0 27) 0 28) 0 29) 0 30) 0 ".
+Время начала: 10:43:37.
+Время завершения: 10:43:58.
+Продолжительность: 00:00:20</t>
+  </si>
+  <si>
     <t>28.09.2021 14:57:51 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
@@ -216,6 +458,29 @@
 Продолжительность: 00:00:18</t>
   </si>
   <si>
+    <t>28.09.2021 14:57:51 ----------
+Тест закончен...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "sdfjds"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 7 (23,3% выполненых заданий).
+Из них ошибок: 23 (76,7% выполненых заданий).
+Результативность: 23,3%.
+Использовано подсказок: 0.
+Набрано баллов: 7,0 из 30 возможных. Ваш результат: 23,3%.
+Оценка: 2.
+Маска результата: "1) - 2) + 3) - 4) + 5) - 6) - 7) + 8) - 9) - 10) - 11) + 12) - 13) + 14) + 15) - 16) - 17) + 18) - 19) - 20) - 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 5 2) 1 3) 1 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 0 30) 0 ".
+Время начала: 14:57:32.
+Время завершения: 14:57:51.
+Продолжительность: 00:00:18</t>
+  </si>
+  <si>
     <t>28.09.2021 14:59:57 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K323-WKS1"
@@ -241,6 +506,29 @@
 Продолжительность: 00:00:44</t>
   </si>
   <si>
+    <t>28.09.2021 14:59:57 ----------
+Тест прерван - закрыта программа...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "kdfjgdfhgfghjf"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf"
+CRC Файла с тестом: "4F621F46"
+Всего заданий в тесте: 30.
+Выполнено заданий: 1.
+Из них правильно: 0 (0,0% выполненых заданий).
+Из них ошибок: 0 (0,0% выполненых заданий).
+Результативность: 0,0%.
+Использовано подсказок: 0.
+Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
+Оценка: 2.
+Маска результата: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Маска времени обдумывания (в секундах): "1) 44 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Время начала: 14:59:11.
+Время завершения: 14:59:57.
+Продолжительность: 00:00:44</t>
+  </si>
+  <si>
     <t>05.10.2021 09:12:37 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "PUCILO-EV"
@@ -266,6 +554,29 @@
 Продолжительность: 00:00:28</t>
   </si>
   <si>
+    <t>05.10.2021 09:12:37 ----------
+Тест прерван - закрыта программа...
+Имя компьютера: "PUCILO-EV"
+Имя пользователя компьютера: "pucilo_ev"
+Имя пользователя (тестируемого): "я"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 2.
+Из них правильно: 0 (0,0% выполненых заданий).
+Из них ошибок: 1 (50,0% выполненых заданий).
+Результативность: 0,0%.
+Использовано подсказок: 0.
+Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
+Оценка: 2.
+Маска результата: "1) - 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Маска времени обдумывания (в секундах): "1) 19 2) 8 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Время начала: 09:12:08.
+Время завершения: 09:12:37.
+Продолжительность: 00:00:28</t>
+  </si>
+  <si>
     <t>05.10.2021 09:13:01 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K323-WKS1"
@@ -291,6 +602,29 @@
 Продолжительность: 00:00:48</t>
   </si>
   <si>
+    <t>05.10.2021 09:13:01 ----------
+Тест прерван - закрыта программа...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "sdfklsdfsdgsd"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 1.
+Из них правильно: 0 (0,0% выполненых заданий).
+Из них ошибок: 0 (0,0% выполненых заданий).
+Результативность: 0,0%.
+Использовано подсказок: 0.
+Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
+Оценка: 2.
+Маска результата: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Маска времени обдумывания (в секундах): "1) 48 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Время начала: 09:12:11.
+Время завершения: 09:13:00.
+Продолжительность: 00:00:48</t>
+  </si>
+  <si>
     <t>06.10.2021 15:01:45 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
@@ -316,6 +650,29 @@
 Продолжительность: 00:03:45</t>
   </si>
   <si>
+    <t>06.10.2021 15:01:45 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X01"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Фамилия Имя"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf"
+CRC Файла с тестом: "4F621F46"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 8 (26,7% выполненых заданий).
+Из них ошибок: 22 (73,3% выполненых заданий).
+Результативность: 26,7%.
+Использовано подсказок: 0.
+Набрано баллов: 8,0 из 30 возможных. Ваш результат: 26,7%.
+Оценка: 2.
+Маска результата: "1) - 2) - 3) - 4) - 5) + 6) + 7) - 8) - 9) + 10) - 11) + 12) + 13) + 14) - 15) - 16) - 17) - 18) - 19) - 20) - 21) - 22) - 23) - 24) + 25) - 26) - 27) - 28) - 29) - 30) + ".
+Маска времени обдумывания (в секундах): "1) 8 2) 4 3) 3 4) 4 5) 2 6) 3 7) 3 8) 4 9) 6 10) 6 11) 7 12) 6 13) 4 14) 5 15) 4 16) 2 17) 3 18) 6 19) 51 20) 4 21) 2 22) 4 23) 3 24) 5 25) 3 26) 3 27) 6 28) 37 29) 4 30) 9 ".
+Время начала: 14:57:52.
+Время завершения: 15:01:45.
+Продолжительность: 00:03:45</t>
+  </si>
+  <si>
     <t>12.10.2021 17:10:17 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
@@ -336,6 +693,29 @@
 Маска времени обдумывания (в секундах): "1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 1 30) 0 ".
 Маска ответов: "1) 2 2) 2 3) 2 4) 2 5) 2 6) 2 7) 2 8) 2 9) 2 10) 2 11) 2 12) 2 13) 2 14) 2 15) 2 16) 2 17) 2 18) 2 19) 2 20) 2 21) 2 22) 2; 23) 2 24) 3; 25) 2 26) 2; 27) 2 28) 2 29) 2 30) 2 ".
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Время начала: 17:10:02.
+Время завершения: 17:10:17.
+Продолжительность: 00:00:14</t>
+  </si>
+  <si>
+    <t>12.10.2021 17:10:17 ----------
+Тест закончен...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "lkjg;ldfjgiljg"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
+CRC Файла с тестом: "5A416D2A"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 4 (13,3% выполненых заданий).
+Из них ошибок: 26 (86,7% выполненых заданий).
+Результативность: 13,3%.
+Использовано подсказок: 0.
+Набрано баллов: 4,0 из 30 возможных. Ваш результат: 13,3%.
+Оценка: 2.
+Маска результата: "1) - 2) - 3) - 4) - 5) - 6) - 7) - 8) + 9) - 10) + 11) - 12) - 13) - 14) + 15) - 16) - 17) - 18) - 19) + 20) - 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 1 30) 0 ".
 Время начала: 17:10:02.
 Время завершения: 17:10:17.
 Продолжительность: 00:00:14</t>
@@ -366,6 +746,29 @@
 Продолжительность: 00:00:12</t>
   </si>
   <si>
+    <t>12.10.2021 17:10:46 ----------
+Тест закончен...
+Имя компьютера: "SHA-K323-WKS1"
+Имя пользователя компьютера: "tabakaev_mv"
+Имя пользователя (тестируемого): "lkjg;ldfjgiljg"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников продовольственной торговли.mtf"
+CRC Файла с тестом: "7AC88467"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 15 (50,0% выполненых заданий).
+Из них ошибок: 15 (50,0% выполненых заданий).
+Результативность: 50,0%.
+Использовано подсказок: 0.
+Набрано баллов: 15,0 из 30 возможных. Ваш результат: 50,0%.
+Оценка: 3.
+Маска результата: "1) + 2) - 3) + 4) + 5) - 6) + 7) + 8) + 9) + 10) - 11) + 12) + 13) + 14) - 15) - 16) + 17) + 18) - 19) + 20) - 21) + 22) - 23) - 24) - 25) + 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 1 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 1 29) 0 30) 0 ".
+Время начала: 17:10:34.
+Время завершения: 17:10:46.
+Продолжительность: 00:00:12</t>
+  </si>
+  <si>
     <t>13.10.2021 09:21:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X06"
@@ -386,6 +789,29 @@
 Маска времени обдумывания (в секундах): "1) 50 2) 29 3) 92 4) 27 5) 12 6) 16 7) 17 8) 13 9) 13 10) 10 11) 24 12) 16 13) 9 14) 7 15) 44 16) 13 17) 18 18) 14 19) 40 20) 12 21) 15 22) 10 23) 50 24) 18 25) 13 26) 11 27) 16 28) 24 29) 12 30) 12 ".
 Маска ответов: "1) 1; 2) 2 3) 1; 4) 2 5) 2; 6) 3 7) 1 8) 1; 9) 3 10) 1; 11) 1 12) 1 13) 1 14) 1 15) 3 16) 2 17) 1 18) 2; 19) 1 20) 1; 21) 2 22) 2 23) 1 24) 1; 25) 2; 26) 3 27) 1; 28) 2 29) 2 30) 1 ".
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Время начала: 09:10:20.
+Время завершения: 09:21:40.
+Продолжительность: 00:11:10</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:21:40 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X06"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "озерова елизавета денисовна"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 9 (30,0% выполненых заданий).
+Из них ошибок: 21 (70,0% выполненых заданий).
+Результативность: 30,0%.
+Использовано подсказок: 0.
+Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
+Оценка: 2.
+Маска результата: "1) - 2) + 3) - 4) - 5) - 6) + 7) + 8) - 9) - 10) - 11) + 12) - 13) + 14) + 15) - 16) + 17) + 18) - 19) - 20) - 21) - 22) + 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 50 2) 29 3) 92 4) 27 5) 12 6) 16 7) 17 8) 13 9) 13 10) 10 11) 24 12) 16 13) 9 14) 7 15) 44 16) 13 17) 18 18) 14 19) 40 20) 12 21) 15 22) 10 23) 50 24) 18 25) 13 26) 11 27) 16 28) 24 29) 12 30) 12 ".
 Время начала: 09:10:20.
 Время завершения: 09:21:40.
 Продолжительность: 00:11:10</t>
@@ -416,6 +842,29 @@
 Продолжительность: 00:17:50</t>
   </si>
   <si>
+    <t>13.10.2021 09:28:48 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X08"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Лоскутова"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
+CRC Файла с тестом: "5A416D2A"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 17 (56,7% выполненых заданий).
+Из них ошибок: 13 (43,3% выполненых заданий).
+Результативность: 56,7%.
+Использовано подсказок: 0.
+Набрано баллов: 17,0 из 30 возможных. Ваш результат: 56,7%.
+Оценка: 3.
+Маска результата: "1) - 2) + 3) + 4) + 5) - 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) + 17) + 18) + 19) - 20) + 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 48 2) 15 3) 14 4) 13 5) 37 6) 11 7) 13 8) 8 9) 23 10) 15 11) 12 12) 41 13) 42 14) 73 15) 13 16) 10 17) 93 18) 14 19) 43 20) 14 21) 31 22) 75 23) 68 24) 44 25) 40 26) 108 27) 26 28) 49 29) 33 30) 30 ".
+Время начала: 09:10:42.
+Время завершения: 09:28:48.
+Продолжительность: 00:17:50</t>
+  </si>
+  <si>
     <t>13.10.2021 09:34:31 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X09"
@@ -441,6 +890,29 @@
 Продолжительность: 00:21:55</t>
   </si>
   <si>
+    <t>13.10.2021 09:34:31 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X09"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Туманова Ирина Леонидовна"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
+CRC Файла с тестом: "5A416D2A"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 23 (76,7% выполненых заданий).
+Из них ошибок: 7 (23,3% выполненых заданий).
+Результативность: 76,7%.
+Использовано подсказок: 0.
+Набрано баллов: 23,0 из 30 возможных. Ваш результат: 76,7%.
+Оценка: 4.
+Маска результата: "1) + 2) + 3) + 4) + 5) + 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) + 19) + 20) + 21) + 22) - 23) - 24) - 25) - 26) - 27) - 28) + 29) + 30) + ".
+Маска времени обдумывания (в секундах): "1) 35 2) 17 3) 45 4) 14 5) 29 6) 24 7) 29 8) 28 9) 33 10) 25 11) 26 12) 176 13) 21 14) 162 15) 32 16) 24 17) 41 18) 19 19) 11 20) 18 21) 45 22) 59 23) 34 24) 86 25) 57 26) 56 27) 29 28) 57 29) 44 30) 23 ".
+Время начала: 09:12:17.
+Время завершения: 09:34:31.
+Продолжительность: 00:21:55</t>
+  </si>
+  <si>
     <t>13.10.2021 09:39:34 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
@@ -466,6 +938,29 @@
 Продолжительность: 00:24:39</t>
   </si>
   <si>
+    <t>13.10.2021 09:39:34 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X02"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Романцов Дмитрий Ильич"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
+CRC Файла с тестом: "5A416D2A"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 20 (66,7% выполненых заданий).
+Из них ошибок: 10 (33,3% выполненых заданий).
+Результативность: 66,7%.
+Использовано подсказок: 0.
+Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
+Оценка: 3.
+Маска результата: "1) - 2) + 3) + 4) + 5) + 6) - 7) + 8) + 9) + 10) + 11) + 12) - 13) + 14) + 15) + 16) - 17) + 18) + 19) + 20) + 21) + 22) - 23) - 24) - 25) - 26) - 27) + 28) + 29) - 30) + ".
+Маска времени обдумывания (в секундах): "1) 78 2) 35 3) 18 4) 14 5) 45 6) 44 7) 19 8) 9 9) 44 10) 25 11) 24 12) 130 13) 27 14) 75 15) 29 16) 25 17) 23 18) 16 19) 44 20) 32 21) 35 22) 48 23) 78 24) 154 25) 61 26) 43 27) 47 28) 94 29) 74 30) 73 ".
+Время начала: 09:14:34.
+Время завершения: 09:39:34.
+Продолжительность: 00:24:39</t>
+  </si>
+  <si>
     <t>13.10.2021 09:39:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
@@ -491,6 +986,29 @@
 Продолжительность: 00:24:43</t>
   </si>
   <si>
+    <t>13.10.2021 09:39:40 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X01"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Андреева Снежана Генадьевна"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
+CRC Файла с тестом: "5A416D2A"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 20 (66,7% выполненых заданий).
+Из них ошибок: 10 (33,3% выполненых заданий).
+Результативность: 66,7%.
+Использовано подсказок: 0.
+Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
+Оценка: 3.
+Маска результата: "1) - 2) + 3) + 4) + 5) + 6) - 7) + 8) + 9) + 10) + 11) + 12) - 13) + 14) + 15) + 16) - 17) + 18) + 19) + 20) + 21) + 22) - 23) - 24) - 25) - 26) - 27) + 28) + 29) - 30) + ".
+Маска времени обдумывания (в секундах): "1) 72 2) 33 3) 30 4) 22 5) 54 6) 27 7) 17 8) 19 9) 41 10) 24 11) 21 12) 134 13) 16 14) 85 15) 26 16) 23 17) 28 18) 17 19) 37 20) 30 21) 39 22) 49 23) 70 24) 196 25) 23 26) 42 27) 52 28) 93 29) 75 30) 72 ".
+Время начала: 09:14:36.
+Время завершения: 09:39:40.
+Продолжительность: 00:24:43</t>
+  </si>
+  <si>
     <t>13.10.2021 09:44:54 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X07"
@@ -516,6 +1034,29 @@
 Продолжительность: 00:33:20</t>
   </si>
   <si>
+    <t>13.10.2021 09:44:54 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X07"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Белоусова Наталья"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 18 (60,0% выполненых заданий).
+Из них ошибок: 12 (40,0% выполненых заданий).
+Результативность: 60,0%.
+Использовано подсказок: 0.
+Набрано баллов: 18,0 из 30 возможных. Ваш результат: 60,0%.
+Оценка: 3.
+Маска результата: "1) + 2) + 3) - 4) + 5) + 6) - 7) + 8) - 9) + 10) - 11) + 12) + 13) - 14) + 15) + 16) + 17) + 18) - 19) + 20) + 21) - 22) + 23) + 24) - 25) - 26) + 27) - 28) - 29) + 30) - ".
+Маска времени обдумывания (в секундах): "1) 233 2) 246 3) 64 4) 178 5) 78 6) 30 7) 16 8) 40 9) 12 10) 62 11) 10 12) 9 13) 27 14) 19 15) 13 16) 17 17) 46 18) 182 19) 30 20) 26 21) 41 22) 182 23) 17 24) 36 25) 60 26) 110 27) 48 28) 109 29) 22 30) 20 ".
+Время начала: 09:11:06.
+Время завершения: 09:44:54.
+Продолжительность: 00:33:20</t>
+  </si>
+  <si>
     <t>13.10.2021 09:51:08 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X04"
@@ -541,6 +1082,29 @@
 Продолжительность: 00:37:59</t>
   </si>
   <si>
+    <t>13.10.2021 09:51:08 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X04"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Петрова Марина Алексеевна"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 20 (66,7% выполненых заданий).
+Из них ошибок: 10 (33,3% выполненых заданий).
+Результативность: 66,7%.
+Использовано подсказок: 0.
+Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
+Оценка: 3.
+Маска результата: "1) + 2) + 3) - 4) + 5) + 6) + 7) + 8) - 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) + 17) + 18) - 19) - 20) + 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) + 30) - ".
+Маска времени обдумывания (в секундах): "1) 144 2) 26 3) 13 4) 373 5) 351 6) 4 7) 9 8) 207 9) 9 10) 82 11) 83 12) 8 13) 9 14) 8 15) 4 16) 6 17) 34 18) 81 19) 57 20) 51 21) 76 22) 112 23) 8 24) 10 25) 134 26) 207 27) 118 28) 13 29) 13 30) 15 ".
+Время начала: 09:12:37.
+Время завершения: 09:51:08.
+Продолжительность: 00:37:59</t>
+  </si>
+  <si>
     <t>20.10.2021 09:09:04 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
@@ -566,6 +1130,29 @@
 Продолжительность: 00:11:43</t>
   </si>
   <si>
+    <t>20.10.2021 09:09:04 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X01"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "озерова елизавета денисовна"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 9 (30,0% выполненых заданий).
+Из них ошибок: 21 (70,0% выполненых заданий).
+Результативность: 30,0%.
+Использовано подсказок: 0.
+Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
+Оценка: 2.
+Маска результата: "1) - 2) - 3) - 4) - 5) - 6) + 7) + 8) - 9) + 10) - 11) + 12) - 13) - 14) + 15) + 16) + 17) + 18) - 19) - 20) - 21) + 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 17 2) 35 3) 19 4) 54 5) 43 6) 5 7) 15 8) 33 9) 14 10) 30 11) 12 12) 33 13) 23 14) 21 15) 37 16) 16 17) 18 18) 17 19) 12 20) 15 21) 42 22) 15 23) 22 24) 19 25) 12 26) 11 27) 47 28) 11 29) 16 30) 25 ".
+Время начала: 08:57:10.
+Время завершения: 09:09:04.
+Продолжительность: 00:11:43</t>
+  </si>
+  <si>
     <t>20.10.2021 09:17:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
@@ -591,6 +1178,29 @@
 Продолжительность: 00:19:53</t>
   </si>
   <si>
+    <t>20.10.2021 09:17:40 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X02"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "кекина людмила федоровна"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 14 (46,7% выполненых заданий).
+Из них ошибок: 16 (53,3% выполненых заданий).
+Результативность: 46,7%.
+Использовано подсказок: 0.
+Набрано баллов: 14,0 из 30 возможных. Ваш результат: 46,7%.
+Оценка: 2.
+Маска результата: "1) - 2) + 3) - 4) - 5) - 6) + 7) + 8) - 9) + 10) - 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) - 19) + 20) - 21) - 22) - 23) + 24) - 25) - 26) - 27) - 28) - 29) + 30) + ".
+Маска времени обдумывания (в секундах): "1) 47 2) 79 3) 38 4) 52 5) 27 6) 17 7) 15 8) 40 9) 33 10) 32 11) 28 12) 31 13) 24 14) 17 15) 59 16) 20 17) 23 18) 63 19) 38 20) 21 21) 83 22) 36 23) 21 24) 30 25) 56 26) 34 27) 36 28) 81 29) 46 30) 51 ".
+Время начала: 08:57:30.
+Время завершения: 09:17:40.
+Продолжительность: 00:19:53</t>
+  </si>
+  <si>
     <t>20.10.2021 09:48:00 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X09"
@@ -616,6 +1226,29 @@
 Продолжительность: 00:43:13</t>
   </si>
   <si>
+    <t>20.10.2021 09:48:00 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X09"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Романцов Дмитрий Ильич"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
+CRC Файла с тестом: "2C7EB1D6"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 21 (70,0% выполненых заданий).
+Из них ошибок: 9 (30,0% выполненых заданий).
+Результативность: 70,0%.
+Использовано подсказок: 0.
+Набрано баллов: 21,0 из 30 возможных. Ваш результат: 70,0%.
+Оценка: 2.
+Маска результата: "1) + 2) + 3) + 4) + 5) + 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) + 19) - 20) - 21) + 22) - 23) + 24) - 25) - 26) - 27) + 28) + 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 193 2) 48 3) 17 4) 6 5) 36 6) 82 7) 7 8) 6 9) 86 10) 15 11) 24 12) 82 13) 19 14) 120 15) 7 16) 70 17) 9 18) 43 19) 243 20) 207 21) 105 22) 60 23) 343 24) 171 25) 65 26) 25 27) 186 28) 192 29) 47 30) 64 ".
+Время начала: 09:04:10.
+Время завершения: 09:48:00.
+Продолжительность: 00:43:13</t>
+  </si>
+  <si>
     <t>10.01.2022 17:28:01 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X08"
@@ -641,6 +1274,29 @@
 Продолжительность: 00:01:02</t>
   </si>
   <si>
+    <t>10.01.2022 17:28:01 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X08"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Фамилия Имя"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "554B1E8C"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 7 (23,3% выполненых заданий).
+Из них ошибок: 23 (76,7% выполненых заданий).
+Результативность: 23,3%.
+Использовано подсказок: 0.
+Набрано баллов: 7,0 из 30 возможных. Ваш результат: 23,3%.
+Оценка: 2.
+Маска результата: "1) - 2) + 3) - 4) + 5) - 6) - 7) + 8) - 9) - 10) - 11) - 12) - 13) - 14) - 15) - 16) - 17) + 18) - 19) - 20) - 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 6 2) 3 3) 2 4) 1 5) 1 6) 1 7) 1 8) 1 9) 1 10) 1 11) 1 12) 1 13) 1 14) 1 15) 1 16) 3 17) 1 18) 1 19) 1 20) 1 21) 1 22) 3 23) 2 24) 1 25) 1 26) 2 27) 1 28) 1 29) 1 30) 1 ".
+Время начала: 17:26:58.
+Время завершения: 17:28:01.
+Продолжительность: 00:01:02</t>
+  </si>
+  <si>
     <t>19.01.2022 10:22:18 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
@@ -666,6 +1322,29 @@
 Продолжительность: 00:01:44</t>
   </si>
   <si>
+    <t>19.01.2022 10:22:18 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X01"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Важенина"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников продовольственной торговли.mtf"
+CRC Файла с тестом: "1D498E48"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 9 (30,0% выполненых заданий).
+Из них ошибок: 21 (70,0% выполненых заданий).
+Результативность: 30,0%.
+Использовано подсказок: 0.
+Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
+Оценка: 2.
+Маска результата: "1) - 2) - 3) + 4) - 5) - 6) - 7) - 8) - 9) - 10) - 11) - 12) - 13) + 14) + 15) + 16) - 17) + 18) - 19) + 20) - 21) - 22) - 23) + 24) - 25) + 26) + 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 7 2) 6 3) 4 4) 2 5) 2 6) 3 7) 2 8) 4 9) 2 10) 2 11) 2 12) 2 13) 2 14) 2 15) 2 16) 2 17) 2 18) 2 19) 2 20) 4 21) 11 22) 6 23) 5 24) 3 25) 2 26) 1 27) 1 28) 2 29) 3 30) 1 ".
+Время начала: 10:20:33.
+Время завершения: 10:22:18.
+Продолжительность: 00:01:44</t>
+  </si>
+  <si>
     <t>19.01.2022 14:00:29 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
@@ -686,6 +1365,29 @@
 Маска времени обдумывания (в секундах): "1) 7 2) 2 3) 2 4) 1 5) 0 6) 1 7) 0 8) 1 9) 1 10) 1 11) 0 12) 0 13) 0 14) 0 15) 0 16) 1 17) 0 18) 0 19) 0 20) 1 21) 0 22) 1 23) 0 24) 2 25) 2 26) 1 27) 1 28) 0 29) 0 30) 1 ".
 Маска ответов: "1) 2; 2) 1 3) 2;3; 4) 1 5) 2; 6) 3 7) 1 8) 2;3; 9) 1 10) 2;3; 11) 3 12) 2 13) 1 14) 2 15) 3 16) 2 17) 1 18) 1; 19) 1 20) 2; 21) 2 22) 2 23) 2 24) 3; 25) 2;3; 26) 3 27) 2;3; 28) 1 29) 2 30) 3 ".
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
+Время начала: 13:59:44.
+Время завершения: 14:00:29.
+Продолжительность: 00:00:44</t>
+  </si>
+  <si>
+    <t>19.01.2022 14:00:29 ----------
+Тест закончен...
+Имя компьютера: "SHA-K205-X01"
+Имя пользователя компьютера: "brailovskiy_vv"
+Имя пользователя (тестируемого): "Фамилия Имя Тестируем 19.01.2022"
+Название теста: ""
+Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
+CRC Файла с тестом: "A3C16E8A"
+Всего заданий в тесте: 30.
+Выполнено заданий: 30.
+Из них правильно: 9 (30,0% выполненых заданий).
+Из них ошибок: 21 (70,0% выполненых заданий).
+Результативность: 30,0%.
+Использовано подсказок: 0.
+Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
+Оценка: Незачет.
+Маска результата: "1) - 2) - 3) - 4) + 5) - 6) + 7) + 8) - 9) - 10) - 11) - 12) + 13) + 14) - 15) - 16) + 17) + 18) - 19) - 20) - 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) - 29) - 30) - ".
+Маска времени обдумывания (в секундах): "1) 7 2) 2 3) 2 4) 1 5) 0 6) 1 7) 0 8) 1 9) 1 10) 1 11) 0 12) 0 13) 0 14) 0 15) 0 16) 1 17) 0 18) 0 19) 0 20) 1 21) 0 22) 1 23) 0 24) 2 25) 2 26) 1 27) 1 28) 0 29) 0 30) 1 ".
 Время начала: 13:59:44.
 Время завершения: 14:00:29.
 Продолжительность: 00:00:44</t>
@@ -1046,150 +1748,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1">
+    <row r="1" spans="1:27">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" t="s">
+        <v>66</v>
+      </c>
+      <c r="U3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" t="s">
+        <v>70</v>
+      </c>
+      <c r="W3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new file variablevaluesmarks - dictionary with variables borders. key in dictionary is a variable name and value of the dictionary is a list: first element is a row number of variable the second element - start border, the third element - the end border of variable value in the text with results of test. renamed the key in parsermodule in method content_slicer - the key in the returned dictionary is now full timestamp + student fio (the person tested)
</commit_message>
<xml_diff>
--- a/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
+++ b/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
@@ -14,87 +14,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
-  <si>
-    <t>1 результат</t>
-  </si>
-  <si>
-    <t>2 результат</t>
-  </si>
-  <si>
-    <t>3 результат</t>
-  </si>
-  <si>
-    <t>4 результат</t>
-  </si>
-  <si>
-    <t>5 результат</t>
-  </si>
-  <si>
-    <t>6 результат</t>
-  </si>
-  <si>
-    <t>7 результат</t>
-  </si>
-  <si>
-    <t>8 результат</t>
-  </si>
-  <si>
-    <t>9 результат</t>
-  </si>
-  <si>
-    <t>10 результат</t>
-  </si>
-  <si>
-    <t>11 результат</t>
-  </si>
-  <si>
-    <t>12 результат</t>
-  </si>
-  <si>
-    <t>13 результат</t>
-  </si>
-  <si>
-    <t>14 результат</t>
-  </si>
-  <si>
-    <t>15 результат</t>
-  </si>
-  <si>
-    <t>16 результат</t>
-  </si>
-  <si>
-    <t>17 результат</t>
-  </si>
-  <si>
-    <t>18 результат</t>
-  </si>
-  <si>
-    <t>19 результат</t>
-  </si>
-  <si>
-    <t>20 результат</t>
-  </si>
-  <si>
-    <t>21 результат</t>
-  </si>
-  <si>
-    <t>22 результат</t>
-  </si>
-  <si>
-    <t>23 результат</t>
-  </si>
-  <si>
-    <t>24 результат</t>
-  </si>
-  <si>
-    <t>25 результат</t>
-  </si>
-  <si>
-    <t>26 результат</t>
-  </si>
-  <si>
-    <t>27 результат</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
+  <si>
+    <t>22.09.2021 13:28:19 -||-А кто кто кто</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:29:13 -||-Фамилия Имя</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:47:58 -||-джлдлоогридл</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:48:39 -||-орпрдло</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:49:01 -||-Петя</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:50:34 -||-Вася</t>
+  </si>
+  <si>
+    <t>28.09.2021 10:43:58 -||-оыважыва</t>
+  </si>
+  <si>
+    <t>28.09.2021 14:57:51 -||-sdfjds</t>
+  </si>
+  <si>
+    <t>28.09.2021 14:59:57 -||-kdfjgdfhgfghjf</t>
+  </si>
+  <si>
+    <t>05.10.2021 09:12:37 -||-я</t>
+  </si>
+  <si>
+    <t>05.10.2021 09:13:01 -||-sdfklsdfsdgsd</t>
+  </si>
+  <si>
+    <t>06.10.2021 15:01:45 -||-Фамилия Имя</t>
+  </si>
+  <si>
+    <t>12.10.2021 17:10:17 -||-lkjg;ldfjgiljg</t>
+  </si>
+  <si>
+    <t>12.10.2021 17:10:46 -||-lkjg;ldfjgiljg</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:21:40 -||-озерова елизавета денисовна</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:28:48 -||-Лоскутова</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:34:31 -||-Туманова Ирина Леонидовна</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:39:34 -||-Романцов Дмитрий Ильич</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:39:40 -||-Андреева Снежана Генадьевна</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:44:54 -||-Белоусова Наталья</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:51:08 -||-Петрова Марина Алексеевна</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:09:04 -||-озерова елизавета денисовна</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:17:40 -||-кекина людмила федоровна</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:48:00 -||-Романцов Дмитрий Ильич</t>
+  </si>
+  <si>
+    <t>10.01.2022 17:28:01 -||-Фамилия Имя</t>
+  </si>
+  <si>
+    <t>19.01.2022 10:22:18 -||-Важенина</t>
+  </si>
+  <si>
+    <t>19.01.2022 14:00:29 -||-Фамилия Имя Тестируем 19.01.2022</t>
   </si>
   <si>
     <t>22.09.2021 13:28:19 ----------
@@ -119,7 +119,7 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:28:05.
 Время завершения: 13:28:19.
-Продолжительность: 00:00:13</t>
+Продолжительность: 00:00:13.</t>
   </si>
   <si>
     <t>22.09.2021 13:28:19 ----------
@@ -142,7 +142,19 @@
 Маска времени обдумывания (в секундах): "1) 5 2) 7 ".
 Время начала: 13:28:05.
 Время завершения: 13:28:19.
-Продолжительность: 00:00:13</t>
+Продолжительность: 00:00:13.</t>
+  </si>
+  <si>
+    <t>SHA-K323-WKS1</t>
+  </si>
+  <si>
+    <t>tabakaev_mv</t>
+  </si>
+  <si>
+    <t>А кто кто кто</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) - </t>
   </si>
   <si>
     <t>22.09.2021 13:29:13 ----------
@@ -167,7 +179,7 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:29:02.
 Время завершения: 13:29:13.
-Продолжительность: 00:00:10</t>
+Продолжительность: 00:00:10.</t>
   </si>
   <si>
     <t>22.09.2021 13:29:13 ----------
@@ -190,7 +202,13 @@
 Маска времени обдумывания (в секундах): "1) 6 2) 4 ".
 Время начала: 13:29:02.
 Время завершения: 13:29:13.
-Продолжительность: 00:00:10</t>
+Продолжительность: 00:00:10.</t>
+  </si>
+  <si>
+    <t>Фамилия Имя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) + 2) + </t>
   </si>
   <si>
     <t>22.09.2021 13:47:58 ----------
@@ -215,7 +233,7 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:47:52.
 Время завершения: 13:47:58.
-Продолжительность: 00:00:06</t>
+Продолжительность: 00:00:06.</t>
   </si>
   <si>
     <t>22.09.2021 13:47:58 ----------
@@ -238,7 +256,16 @@
 Маска времени обдумывания (в секундах): "1) 3 2) 3 ".
 Время начала: 13:47:52.
 Время завершения: 13:47:58.
-Продолжительность: 00:00:06</t>
+Продолжительность: 00:00:06.</t>
+  </si>
+  <si>
+    <t>SHA-K205-X04</t>
+  </si>
+  <si>
+    <t>brailovskiy_vv</t>
+  </si>
+  <si>
+    <t>джлдлоогридл</t>
   </si>
   <si>
     <t>22.09.2021 13:48:39 ----------
@@ -263,7 +290,7 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:47:11.
 Время завершения: 13:48:39.
-Продолжительность: 00:01:26</t>
+Продолжительность: 00:01:26.</t>
   </si>
   <si>
     <t>22.09.2021 13:48:39 ----------
@@ -286,7 +313,13 @@
 Маска времени обдумывания (в секундах): "1) 85 2) 1 ".
 Время начала: 13:47:11.
 Время завершения: 13:48:39.
-Продолжительность: 00:01:26</t>
+Продолжительность: 00:01:26.</t>
+  </si>
+  <si>
+    <t>SHA-K205-X02</t>
+  </si>
+  <si>
+    <t>орпрдло</t>
   </si>
   <si>
     <t>22.09.2021 13:49:01 ----------
@@ -311,7 +344,7 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:45:32.
 Время завершения: 13:49:01.
-Продолжительность: 00:03:25</t>
+Продолжительность: 00:03:25.</t>
   </si>
   <si>
     <t>22.09.2021 13:49:01 ----------
@@ -334,7 +367,16 @@
 Маска времени обдумывания (в секундах): "1) 203 2) 1 ".
 Время начала: 13:45:32.
 Время завершения: 13:49:01.
-Продолжительность: 00:03:25</t>
+Продолжительность: 00:03:25.</t>
+  </si>
+  <si>
+    <t>SHA-K205-X01</t>
+  </si>
+  <si>
+    <t>Петя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) + </t>
   </si>
   <si>
     <t>22.09.2021 13:50:34 ----------
@@ -359,7 +401,7 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:44:46.
 Время завершения: 13:50:34.
-Продолжительность: 00:05:37</t>
+Продолжительность: 00:05:37.</t>
   </si>
   <si>
     <t>22.09.2021 13:50:34 ----------
@@ -382,7 +424,16 @@
 Маска времени обдумывания (в секундах): "1) 337 2) * ".
 Время начала: 13:44:46.
 Время завершения: 13:50:34.
-Продолжительность: 00:05:37</t>
+Продолжительность: 00:05:37.</t>
+  </si>
+  <si>
+    <t>SHA-K205-X09</t>
+  </si>
+  <si>
+    <t>Вася</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) * 2) * </t>
   </si>
   <si>
     <t>28.09.2021 10:43:58 ----------
@@ -407,7 +458,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 10:43:37.
 Время завершения: 10:43:58.
-Продолжительность: 00:00:20</t>
+Продолжительность: 00:00:20.</t>
   </si>
   <si>
     <t>28.09.2021 10:43:58 ----------
@@ -430,7 +481,13 @@
 Маска времени обдумывания (в секундах): "1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 1 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 1 25) 1 26) 0 27) 0 28) 0 29) 0 30) 0 ".
 Время начала: 10:43:37.
 Время завершения: 10:43:58.
-Продолжительность: 00:00:20</t>
+Продолжительность: 00:00:20.</t>
+  </si>
+  <si>
+    <t>оыважыва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) - 3) + 4) - 5) + 6) - 7) - 8) - 9) - 10) - 11) - 12) - 13) - 14) - 15) - 16) - 17) - 18) - 19) + 20) - 21) + 22) - 23) - 24) - 25) + 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>28.09.2021 14:57:51 ----------
@@ -455,7 +512,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:57:32.
 Время завершения: 14:57:51.
-Продолжительность: 00:00:18</t>
+Продолжительность: 00:00:18.</t>
   </si>
   <si>
     <t>28.09.2021 14:57:51 ----------
@@ -478,7 +535,13 @@
 Маска времени обдумывания (в секундах): "1) 5 2) 1 3) 1 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 0 30) 0 ".
 Время начала: 14:57:32.
 Время завершения: 14:57:51.
-Продолжительность: 00:00:18</t>
+Продолжительность: 00:00:18.</t>
+  </si>
+  <si>
+    <t>sdfjds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) + 3) - 4) + 5) - 6) - 7) + 8) - 9) - 10) - 11) + 12) - 13) + 14) + 15) - 16) - 17) + 18) - 19) - 20) - 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>28.09.2021 14:59:57 ----------
@@ -503,7 +566,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:59:11.
 Время завершения: 14:59:57.
-Продолжительность: 00:00:44</t>
+Продолжительность: 00:00:44.</t>
   </si>
   <si>
     <t>28.09.2021 14:59:57 ----------
@@ -526,7 +589,13 @@
 Маска времени обдумывания (в секундах): "1) 44 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:59:11.
 Время завершения: 14:59:57.
-Продолжительность: 00:00:44</t>
+Продолжительность: 00:00:44.</t>
+  </si>
+  <si>
+    <t>kdfjgdfhgfghjf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
   </si>
   <si>
     <t>05.10.2021 09:12:37 ----------
@@ -551,7 +620,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:08.
 Время завершения: 09:12:37.
-Продолжительность: 00:00:28</t>
+Продолжительность: 00:00:28.</t>
   </si>
   <si>
     <t>05.10.2021 09:12:37 ----------
@@ -574,7 +643,19 @@
 Маска времени обдумывания (в секундах): "1) 19 2) 8 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:08.
 Время завершения: 09:12:37.
-Продолжительность: 00:00:28</t>
+Продолжительность: 00:00:28.</t>
+  </si>
+  <si>
+    <t>PUCILO-EV</t>
+  </si>
+  <si>
+    <t>pucilo_ev</t>
+  </si>
+  <si>
+    <t>я</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
   </si>
   <si>
     <t>05.10.2021 09:13:01 ----------
@@ -599,7 +680,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:11.
 Время завершения: 09:13:00.
-Продолжительность: 00:00:48</t>
+Продолжительность: 00:00:48.</t>
   </si>
   <si>
     <t>05.10.2021 09:13:01 ----------
@@ -622,7 +703,10 @@
 Маска времени обдумывания (в секундах): "1) 48 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:11.
 Время завершения: 09:13:00.
-Продолжительность: 00:00:48</t>
+Продолжительность: 00:00:48.</t>
+  </si>
+  <si>
+    <t>sdfklsdfsdgsd</t>
   </si>
   <si>
     <t>06.10.2021 15:01:45 ----------
@@ -647,7 +731,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:57:52.
 Время завершения: 15:01:45.
-Продолжительность: 00:03:45</t>
+Продолжительность: 00:03:45.</t>
   </si>
   <si>
     <t>06.10.2021 15:01:45 ----------
@@ -670,7 +754,10 @@
 Маска времени обдумывания (в секундах): "1) 8 2) 4 3) 3 4) 4 5) 2 6) 3 7) 3 8) 4 9) 6 10) 6 11) 7 12) 6 13) 4 14) 5 15) 4 16) 2 17) 3 18) 6 19) 51 20) 4 21) 2 22) 4 23) 3 24) 5 25) 3 26) 3 27) 6 28) 37 29) 4 30) 9 ".
 Время начала: 14:57:52.
 Время завершения: 15:01:45.
-Продолжительность: 00:03:45</t>
+Продолжительность: 00:03:45.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) - 3) - 4) - 5) + 6) + 7) - 8) - 9) + 10) - 11) + 12) + 13) + 14) - 15) - 16) - 17) - 18) - 19) - 20) - 21) - 22) - 23) - 24) + 25) - 26) - 27) - 28) - 29) - 30) + </t>
   </si>
   <si>
     <t>12.10.2021 17:10:17 ----------
@@ -695,7 +782,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 17:10:02.
 Время завершения: 17:10:17.
-Продолжительность: 00:00:14</t>
+Продолжительность: 00:00:14.</t>
   </si>
   <si>
     <t>12.10.2021 17:10:17 ----------
@@ -718,7 +805,13 @@
 Маска времени обдумывания (в секундах): "1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 1 30) 0 ".
 Время начала: 17:10:02.
 Время завершения: 17:10:17.
-Продолжительность: 00:00:14</t>
+Продолжительность: 00:00:14.</t>
+  </si>
+  <si>
+    <t>lkjg;ldfjgiljg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) - 3) - 4) - 5) - 6) - 7) - 8) + 9) - 10) + 11) - 12) - 13) - 14) + 15) - 16) - 17) - 18) - 19) + 20) - 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>12.10.2021 17:10:46 ----------
@@ -743,7 +836,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 17:10:34.
 Время завершения: 17:10:46.
-Продолжительность: 00:00:12</t>
+Продолжительность: 00:00:12.</t>
   </si>
   <si>
     <t>12.10.2021 17:10:46 ----------
@@ -766,7 +859,10 @@
 Маска времени обдумывания (в секундах): "1) 1 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 1 29) 0 30) 0 ".
 Время начала: 17:10:34.
 Время завершения: 17:10:46.
-Продолжительность: 00:00:12</t>
+Продолжительность: 00:00:12.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) + 2) - 3) + 4) + 5) - 6) + 7) + 8) + 9) + 10) - 11) + 12) + 13) + 14) - 15) - 16) + 17) + 18) - 19) + 20) - 21) + 22) - 23) - 24) - 25) + 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>13.10.2021 09:21:40 ----------
@@ -791,7 +887,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:10:20.
 Время завершения: 09:21:40.
-Продолжительность: 00:11:10</t>
+Продолжительность: 00:11:10.</t>
   </si>
   <si>
     <t>13.10.2021 09:21:40 ----------
@@ -814,7 +910,16 @@
 Маска времени обдумывания (в секундах): "1) 50 2) 29 3) 92 4) 27 5) 12 6) 16 7) 17 8) 13 9) 13 10) 10 11) 24 12) 16 13) 9 14) 7 15) 44 16) 13 17) 18 18) 14 19) 40 20) 12 21) 15 22) 10 23) 50 24) 18 25) 13 26) 11 27) 16 28) 24 29) 12 30) 12 ".
 Время начала: 09:10:20.
 Время завершения: 09:21:40.
-Продолжительность: 00:11:10</t>
+Продолжительность: 00:11:10.</t>
+  </si>
+  <si>
+    <t>SHA-K205-X06</t>
+  </si>
+  <si>
+    <t>озерова елизавета денисовна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) + 3) - 4) - 5) - 6) + 7) + 8) - 9) - 10) - 11) + 12) - 13) + 14) + 15) - 16) + 17) + 18) - 19) - 20) - 21) - 22) + 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>13.10.2021 09:28:48 ----------
@@ -839,7 +944,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:10:42.
 Время завершения: 09:28:48.
-Продолжительность: 00:17:50</t>
+Продолжительность: 00:17:50.</t>
   </si>
   <si>
     <t>13.10.2021 09:28:48 ----------
@@ -862,7 +967,16 @@
 Маска времени обдумывания (в секундах): "1) 48 2) 15 3) 14 4) 13 5) 37 6) 11 7) 13 8) 8 9) 23 10) 15 11) 12 12) 41 13) 42 14) 73 15) 13 16) 10 17) 93 18) 14 19) 43 20) 14 21) 31 22) 75 23) 68 24) 44 25) 40 26) 108 27) 26 28) 49 29) 33 30) 30 ".
 Время начала: 09:10:42.
 Время завершения: 09:28:48.
-Продолжительность: 00:17:50</t>
+Продолжительность: 00:17:50.</t>
+  </si>
+  <si>
+    <t>SHA-K205-X08</t>
+  </si>
+  <si>
+    <t>Лоскутова</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) + 3) + 4) + 5) - 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) + 17) + 18) + 19) - 20) + 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>13.10.2021 09:34:31 ----------
@@ -887,7 +1001,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:17.
 Время завершения: 09:34:31.
-Продолжительность: 00:21:55</t>
+Продолжительность: 00:21:55.</t>
   </si>
   <si>
     <t>13.10.2021 09:34:31 ----------
@@ -910,7 +1024,13 @@
 Маска времени обдумывания (в секундах): "1) 35 2) 17 3) 45 4) 14 5) 29 6) 24 7) 29 8) 28 9) 33 10) 25 11) 26 12) 176 13) 21 14) 162 15) 32 16) 24 17) 41 18) 19 19) 11 20) 18 21) 45 22) 59 23) 34 24) 86 25) 57 26) 56 27) 29 28) 57 29) 44 30) 23 ".
 Время начала: 09:12:17.
 Время завершения: 09:34:31.
-Продолжительность: 00:21:55</t>
+Продолжительность: 00:21:55.</t>
+  </si>
+  <si>
+    <t>Туманова Ирина Леонидовна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) + 2) + 3) + 4) + 5) + 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) + 19) + 20) + 21) + 22) - 23) - 24) - 25) - 26) - 27) - 28) + 29) + 30) + </t>
   </si>
   <si>
     <t>13.10.2021 09:39:34 ----------
@@ -935,7 +1055,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:14:34.
 Время завершения: 09:39:34.
-Продолжительность: 00:24:39</t>
+Продолжительность: 00:24:39.</t>
   </si>
   <si>
     <t>13.10.2021 09:39:34 ----------
@@ -958,7 +1078,13 @@
 Маска времени обдумывания (в секундах): "1) 78 2) 35 3) 18 4) 14 5) 45 6) 44 7) 19 8) 9 9) 44 10) 25 11) 24 12) 130 13) 27 14) 75 15) 29 16) 25 17) 23 18) 16 19) 44 20) 32 21) 35 22) 48 23) 78 24) 154 25) 61 26) 43 27) 47 28) 94 29) 74 30) 73 ".
 Время начала: 09:14:34.
 Время завершения: 09:39:34.
-Продолжительность: 00:24:39</t>
+Продолжительность: 00:24:39.</t>
+  </si>
+  <si>
+    <t>Романцов Дмитрий Ильич</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) + 3) + 4) + 5) + 6) - 7) + 8) + 9) + 10) + 11) + 12) - 13) + 14) + 15) + 16) - 17) + 18) + 19) + 20) + 21) + 22) - 23) - 24) - 25) - 26) - 27) + 28) + 29) - 30) + </t>
   </si>
   <si>
     <t>13.10.2021 09:39:40 ----------
@@ -983,7 +1109,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:14:36.
 Время завершения: 09:39:40.
-Продолжительность: 00:24:43</t>
+Продолжительность: 00:24:43.</t>
   </si>
   <si>
     <t>13.10.2021 09:39:40 ----------
@@ -1006,7 +1132,10 @@
 Маска времени обдумывания (в секундах): "1) 72 2) 33 3) 30 4) 22 5) 54 6) 27 7) 17 8) 19 9) 41 10) 24 11) 21 12) 134 13) 16 14) 85 15) 26 16) 23 17) 28 18) 17 19) 37 20) 30 21) 39 22) 49 23) 70 24) 196 25) 23 26) 42 27) 52 28) 93 29) 75 30) 72 ".
 Время начала: 09:14:36.
 Время завершения: 09:39:40.
-Продолжительность: 00:24:43</t>
+Продолжительность: 00:24:43.</t>
+  </si>
+  <si>
+    <t>Андреева Снежана Генадьевна</t>
   </si>
   <si>
     <t>13.10.2021 09:44:54 ----------
@@ -1031,7 +1160,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:11:06.
 Время завершения: 09:44:54.
-Продолжительность: 00:33:20</t>
+Продолжительность: 00:33:20.</t>
   </si>
   <si>
     <t>13.10.2021 09:44:54 ----------
@@ -1054,7 +1183,16 @@
 Маска времени обдумывания (в секундах): "1) 233 2) 246 3) 64 4) 178 5) 78 6) 30 7) 16 8) 40 9) 12 10) 62 11) 10 12) 9 13) 27 14) 19 15) 13 16) 17 17) 46 18) 182 19) 30 20) 26 21) 41 22) 182 23) 17 24) 36 25) 60 26) 110 27) 48 28) 109 29) 22 30) 20 ".
 Время начала: 09:11:06.
 Время завершения: 09:44:54.
-Продолжительность: 00:33:20</t>
+Продолжительность: 00:33:20.</t>
+  </si>
+  <si>
+    <t>SHA-K205-X07</t>
+  </si>
+  <si>
+    <t>Белоусова Наталья</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) + 2) + 3) - 4) + 5) + 6) - 7) + 8) - 9) + 10) - 11) + 12) + 13) - 14) + 15) + 16) + 17) + 18) - 19) + 20) + 21) - 22) + 23) + 24) - 25) - 26) + 27) - 28) - 29) + 30) - </t>
   </si>
   <si>
     <t>13.10.2021 09:51:08 ----------
@@ -1079,7 +1217,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:37.
 Время завершения: 09:51:08.
-Продолжительность: 00:37:59</t>
+Продолжительность: 00:37:59.</t>
   </si>
   <si>
     <t>13.10.2021 09:51:08 ----------
@@ -1102,7 +1240,13 @@
 Маска времени обдумывания (в секундах): "1) 144 2) 26 3) 13 4) 373 5) 351 6) 4 7) 9 8) 207 9) 9 10) 82 11) 83 12) 8 13) 9 14) 8 15) 4 16) 6 17) 34 18) 81 19) 57 20) 51 21) 76 22) 112 23) 8 24) 10 25) 134 26) 207 27) 118 28) 13 29) 13 30) 15 ".
 Время начала: 09:12:37.
 Время завершения: 09:51:08.
-Продолжительность: 00:37:59</t>
+Продолжительность: 00:37:59.</t>
+  </si>
+  <si>
+    <t>Петрова Марина Алексеевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) + 2) + 3) - 4) + 5) + 6) + 7) + 8) - 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) + 17) + 18) - 19) - 20) + 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) + 30) - </t>
   </si>
   <si>
     <t>20.10.2021 09:09:04 ----------
@@ -1127,7 +1271,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 08:57:10.
 Время завершения: 09:09:04.
-Продолжительность: 00:11:43</t>
+Продолжительность: 00:11:43.</t>
   </si>
   <si>
     <t>20.10.2021 09:09:04 ----------
@@ -1150,7 +1294,10 @@
 Маска времени обдумывания (в секундах): "1) 17 2) 35 3) 19 4) 54 5) 43 6) 5 7) 15 8) 33 9) 14 10) 30 11) 12 12) 33 13) 23 14) 21 15) 37 16) 16 17) 18 18) 17 19) 12 20) 15 21) 42 22) 15 23) 22 24) 19 25) 12 26) 11 27) 47 28) 11 29) 16 30) 25 ".
 Время начала: 08:57:10.
 Время завершения: 09:09:04.
-Продолжительность: 00:11:43</t>
+Продолжительность: 00:11:43.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) - 3) - 4) - 5) - 6) + 7) + 8) - 9) + 10) - 11) + 12) - 13) - 14) + 15) + 16) + 17) + 18) - 19) - 20) - 21) + 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>20.10.2021 09:17:40 ----------
@@ -1175,7 +1322,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 08:57:30.
 Время завершения: 09:17:40.
-Продолжительность: 00:19:53</t>
+Продолжительность: 00:19:53.</t>
   </si>
   <si>
     <t>20.10.2021 09:17:40 ----------
@@ -1198,7 +1345,13 @@
 Маска времени обдумывания (в секундах): "1) 47 2) 79 3) 38 4) 52 5) 27 6) 17 7) 15 8) 40 9) 33 10) 32 11) 28 12) 31 13) 24 14) 17 15) 59 16) 20 17) 23 18) 63 19) 38 20) 21 21) 83 22) 36 23) 21 24) 30 25) 56 26) 34 27) 36 28) 81 29) 46 30) 51 ".
 Время начала: 08:57:30.
 Время завершения: 09:17:40.
-Продолжительность: 00:19:53</t>
+Продолжительность: 00:19:53.</t>
+  </si>
+  <si>
+    <t>кекина людмила федоровна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) + 3) - 4) - 5) - 6) + 7) + 8) - 9) + 10) - 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) - 19) + 20) - 21) - 22) - 23) + 24) - 25) - 26) - 27) - 28) - 29) + 30) + </t>
   </si>
   <si>
     <t>20.10.2021 09:48:00 ----------
@@ -1223,7 +1376,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:04:10.
 Время завершения: 09:48:00.
-Продолжительность: 00:43:13</t>
+Продолжительность: 00:43:13.</t>
   </si>
   <si>
     <t>20.10.2021 09:48:00 ----------
@@ -1246,7 +1399,10 @@
 Маска времени обдумывания (в секундах): "1) 193 2) 48 3) 17 4) 6 5) 36 6) 82 7) 7 8) 6 9) 86 10) 15 11) 24 12) 82 13) 19 14) 120 15) 7 16) 70 17) 9 18) 43 19) 243 20) 207 21) 105 22) 60 23) 343 24) 171 25) 65 26) 25 27) 186 28) 192 29) 47 30) 64 ".
 Время начала: 09:04:10.
 Время завершения: 09:48:00.
-Продолжительность: 00:43:13</t>
+Продолжительность: 00:43:13.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) + 2) + 3) + 4) + 5) + 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) + 19) - 20) - 21) + 22) - 23) + 24) - 25) - 26) - 27) + 28) + 29) - 30) - </t>
   </si>
   <si>
     <t>10.01.2022 17:28:01 ----------
@@ -1271,7 +1427,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 17:26:58.
 Время завершения: 17:28:01.
-Продолжительность: 00:01:02</t>
+Продолжительность: 00:01:02.</t>
   </si>
   <si>
     <t>10.01.2022 17:28:01 ----------
@@ -1294,7 +1450,10 @@
 Маска времени обдумывания (в секундах): "1) 6 2) 3 3) 2 4) 1 5) 1 6) 1 7) 1 8) 1 9) 1 10) 1 11) 1 12) 1 13) 1 14) 1 15) 1 16) 3 17) 1 18) 1 19) 1 20) 1 21) 1 22) 3 23) 2 24) 1 25) 1 26) 2 27) 1 28) 1 29) 1 30) 1 ".
 Время начала: 17:26:58.
 Время завершения: 17:28:01.
-Продолжительность: 00:01:02</t>
+Продолжительность: 00:01:02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) + 3) - 4) + 5) - 6) - 7) + 8) - 9) - 10) - 11) - 12) - 13) - 14) - 15) - 16) - 17) + 18) - 19) - 20) - 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) - 30) - </t>
   </si>
   <si>
     <t>19.01.2022 10:22:18 ----------
@@ -1319,7 +1478,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 10:20:33.
 Время завершения: 10:22:18.
-Продолжительность: 00:01:44</t>
+Продолжительность: 00:01:44.</t>
   </si>
   <si>
     <t>19.01.2022 10:22:18 ----------
@@ -1342,7 +1501,13 @@
 Маска времени обдумывания (в секундах): "1) 7 2) 6 3) 4 4) 2 5) 2 6) 3 7) 2 8) 4 9) 2 10) 2 11) 2 12) 2 13) 2 14) 2 15) 2 16) 2 17) 2 18) 2 19) 2 20) 4 21) 11 22) 6 23) 5 24) 3 25) 2 26) 1 27) 1 28) 2 29) 3 30) 1 ".
 Время начала: 10:20:33.
 Время завершения: 10:22:18.
-Продолжительность: 00:01:44</t>
+Продолжительность: 00:01:44.</t>
+  </si>
+  <si>
+    <t>Важенина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) - 3) + 4) - 5) - 6) - 7) - 8) - 9) - 10) - 11) - 12) - 13) + 14) + 15) + 16) - 17) + 18) - 19) + 20) - 21) - 22) - 23) + 24) - 25) + 26) + 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
     <t>19.01.2022 14:00:29 ----------
@@ -1367,7 +1532,7 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 13:59:44.
 Время завершения: 14:00:29.
-Продолжительность: 00:00:44</t>
+Продолжительность: 00:00:44.</t>
   </si>
   <si>
     <t>19.01.2022 14:00:29 ----------
@@ -1390,7 +1555,13 @@
 Маска времени обдумывания (в секундах): "1) 7 2) 2 3) 2 4) 1 5) 0 6) 1 7) 0 8) 1 9) 1 10) 1 11) 0 12) 0 13) 0 14) 0 15) 0 16) 1 17) 0 18) 0 19) 0 20) 1 21) 0 22) 1 23) 0 24) 2 25) 2 26) 1 27) 1 28) 0 29) 0 30) 1 ".
 Время начала: 13:59:44.
 Время завершения: 14:00:29.
-Продолжительность: 00:00:44</t>
+Продолжительность: 00:00:44.</t>
+  </si>
+  <si>
+    <t>Фамилия Имя Тестируем 19.01.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) - 2) - 3) - 4) + 5) - 6) + 7) + 8) - 9) - 10) - 11) - 12) + 13) + 14) - 15) - 16) + 17) + 18) - 19) - 20) - 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
   </si>
 </sst>
 </file>
@@ -1748,7 +1919,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1842,82 +2013,82 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="M2" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="P2" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="T2" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="U2" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="V2" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="W2" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="X2" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="Y2" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="Z2" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="AA2" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -1925,82 +2096,414 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O3" t="s">
+        <v>88</v>
+      </c>
+      <c r="P3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>98</v>
+      </c>
+      <c r="R3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" t="s">
+        <v>106</v>
+      </c>
+      <c r="T3" t="s">
+        <v>109</v>
+      </c>
+      <c r="U3" t="s">
+        <v>114</v>
+      </c>
+      <c r="V3" t="s">
+        <v>118</v>
+      </c>
+      <c r="W3" t="s">
+        <v>121</v>
+      </c>
+      <c r="X3" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T4" t="s">
+        <v>110</v>
+      </c>
+      <c r="U4" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" t="s">
+        <v>48</v>
+      </c>
+      <c r="W4" t="s">
+        <v>44</v>
+      </c>
+      <c r="X4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" t="s">
+        <v>40</v>
+      </c>
+      <c r="U5" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" t="s">
+        <v>82</v>
+      </c>
+      <c r="N6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O6" t="s">
+        <v>90</v>
+      </c>
+      <c r="P6" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>99</v>
+      </c>
+      <c r="R6" t="s">
+        <v>103</v>
+      </c>
+      <c r="S6" t="s">
+        <v>107</v>
+      </c>
+      <c r="T6" t="s">
+        <v>111</v>
+      </c>
+      <c r="U6" t="s">
+        <v>115</v>
+      </c>
+      <c r="V6" t="s">
+        <v>90</v>
+      </c>
+      <c r="W6" t="s">
+        <v>122</v>
+      </c>
+      <c r="X6" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
         <v>50</v>
       </c>
-      <c r="M3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>60</v>
-      </c>
-      <c r="R3" t="s">
-        <v>62</v>
-      </c>
-      <c r="S3" t="s">
-        <v>64</v>
-      </c>
-      <c r="T3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" t="s">
-        <v>68</v>
-      </c>
-      <c r="V3" t="s">
-        <v>70</v>
-      </c>
-      <c r="W3" t="s">
-        <v>72</v>
-      </c>
-      <c r="X3" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>80</v>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M18" t="s">
+        <v>83</v>
+      </c>
+      <c r="N18" t="s">
+        <v>86</v>
+      </c>
+      <c r="O18" t="s">
+        <v>91</v>
+      </c>
+      <c r="P18" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>100</v>
+      </c>
+      <c r="R18" t="s">
+        <v>104</v>
+      </c>
+      <c r="S18" t="s">
+        <v>104</v>
+      </c>
+      <c r="T18" t="s">
+        <v>112</v>
+      </c>
+      <c r="U18" t="s">
+        <v>116</v>
+      </c>
+      <c r="V18" t="s">
+        <v>119</v>
+      </c>
+      <c r="W18" t="s">
+        <v>123</v>
+      </c>
+      <c r="X18" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some fixes. mainly in module variablevaluesmarks.py in its dictionary: borders for extracted variable values. some little fixes in other modules
</commit_message>
<xml_diff>
--- a/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
+++ b/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
@@ -14,87 +14,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
-  <si>
-    <t>22.09.2021 13:28:19 -||-А кто кто кто</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:29:13 -||-Фамилия Имя</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:47:58 -||-джлдлоогридл</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:48:39 -||-орпрдло</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:49:01 -||-Петя</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:50:34 -||-Вася</t>
-  </si>
-  <si>
-    <t>28.09.2021 10:43:58 -||-оыважыва</t>
-  </si>
-  <si>
-    <t>28.09.2021 14:57:51 -||-sdfjds</t>
-  </si>
-  <si>
-    <t>28.09.2021 14:59:57 -||-kdfjgdfhgfghjf</t>
-  </si>
-  <si>
-    <t>05.10.2021 09:12:37 -||-я</t>
-  </si>
-  <si>
-    <t>05.10.2021 09:13:01 -||-sdfklsdfsdgsd</t>
-  </si>
-  <si>
-    <t>06.10.2021 15:01:45 -||-Фамилия Имя</t>
-  </si>
-  <si>
-    <t>12.10.2021 17:10:17 -||-lkjg;ldfjgiljg</t>
-  </si>
-  <si>
-    <t>12.10.2021 17:10:46 -||-lkjg;ldfjgiljg</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:21:40 -||-озерова елизавета денисовна</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:28:48 -||-Лоскутова</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:34:31 -||-Туманова Ирина Леонидовна</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:39:34 -||-Романцов Дмитрий Ильич</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:39:40 -||-Андреева Снежана Генадьевна</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:44:54 -||-Белоусова Наталья</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:51:08 -||-Петрова Марина Алексеевна</t>
-  </si>
-  <si>
-    <t>20.10.2021 09:09:04 -||-озерова елизавета денисовна</t>
-  </si>
-  <si>
-    <t>20.10.2021 09:17:40 -||-кекина людмила федоровна</t>
-  </si>
-  <si>
-    <t>20.10.2021 09:48:00 -||-Романцов Дмитрий Ильич</t>
-  </si>
-  <si>
-    <t>10.01.2022 17:28:01 -||-Фамилия Имя</t>
-  </si>
-  <si>
-    <t>19.01.2022 10:22:18 -||-Важенина</t>
-  </si>
-  <si>
-    <t>19.01.2022 14:00:29 -||-Фамилия Имя Тестируем 19.01.2022</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="345">
+  <si>
+    <t>22.09.2021 13:28:19{-}А кто кто кто</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:29:13{-}Фамилия Имя</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:47:58{-}джлдлоогридл</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:48:39{-}орпрдло</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:49:01{-}Петя</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:50:34{-}Вася</t>
+  </si>
+  <si>
+    <t>28.09.2021 10:43:58{-}оыважыва</t>
+  </si>
+  <si>
+    <t>28.09.2021 14:57:51{-}sdfjds</t>
+  </si>
+  <si>
+    <t>28.09.2021 14:59:57{-}kdfjgdfhgfghjf</t>
+  </si>
+  <si>
+    <t>05.10.2021 09:12:37{-}я</t>
+  </si>
+  <si>
+    <t>05.10.2021 09:13:01{-}sdfklsdfsdgsd</t>
+  </si>
+  <si>
+    <t>06.10.2021 15:01:45{-}Фамилия Имя</t>
+  </si>
+  <si>
+    <t>12.10.2021 17:10:17{-}lkjg;ldfjgiljg</t>
+  </si>
+  <si>
+    <t>12.10.2021 17:10:46{-}lkjg;ldfjgiljg</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:21:40{-}озерова елизавета денисовна</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:28:48{-}Лоскутова</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:34:31{-}Туманова Ирина Леонидовна</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:39:34{-}Романцов Дмитрий Ильич</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:39:40{-}Андреева Снежана Генадьевна</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:44:54{-}Белоусова Наталья</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:51:08{-}Петрова Марина Алексеевна</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:09:04{-}озерова елизавета денисовна</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:17:40{-}кекина людмила федоровна</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:48:00{-}Романцов Дмитрий Ильич</t>
+  </si>
+  <si>
+    <t>10.01.2022 17:28:01{-}Фамилия Имя</t>
+  </si>
+  <si>
+    <t>19.01.2022 10:22:18{-}Важенина</t>
+  </si>
+  <si>
+    <t>19.01.2022 14:00:29{-}Фамилия Имя Тестируем 19.01.2022</t>
   </si>
   <si>
     <t>22.09.2021 13:28:19 ----------
@@ -102,7 +102,7 @@
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "А кто кто кто"
-Название теста: ""
+Название теста: "название теста"
 Файл с тестом: "C:\Users\tabakaev_mv\Desktop\РАБОТА\ТЕСТЫ\MyTest\Безымянный.mtf"
 CRC Файла с тестом: "57C3A660"
 Всего заданий в тесте: 2.
@@ -119,7 +119,8 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:28:05.
 Время завершения: 13:28:19.
-Продолжительность: 00:00:13.</t>
+Продолжительность: 00:00:13.
+------------------------------------------------</t>
   </si>
   <si>
     <t>22.09.2021 13:28:19 ----------
@@ -127,9 +128,7 @@
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "А кто кто кто"
-Название теста: ""
-Файл с тестом: "C:\Users\tabakaev_mv\Desktop\РАБОТА\ТЕСТЫ\MyTest\Безымянный.mtf"
-CRC Файла с тестом: "57C3A660"
+Название теста: "название теста"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
 Из них правильно: 0 (0,0% выполненых заданий).
@@ -142,7 +141,8 @@
 Маска времени обдумывания (в секундах): "1) 5 2) 7 ".
 Время начала: 13:28:05.
 Время завершения: 13:28:19.
-Продолжительность: 00:00:13.</t>
+Продолжительность: 00:00:13.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K323-WKS1</t>
@@ -154,7 +154,52 @@
     <t>А кто кто кто</t>
   </si>
   <si>
+    <t>название теста</t>
+  </si>
+  <si>
+    <t>C:\Users\tabakaev_mv\Desktop\РАБОТА\ТЕСТЫ\MyTest\Безымянный.mtf</t>
+  </si>
+  <si>
+    <t>57C3A660</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0 (0,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>2 (100,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>0,0%</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0,0 из 2 возможных. Ваш результат: 0,0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 5 2) 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2; 2) 3; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) * 2) * </t>
+  </si>
+  <si>
+    <t>13:28:05</t>
+  </si>
+  <si>
+    <t>13:28:19</t>
+  </si>
+  <si>
+    <t>00:00:13</t>
   </si>
   <si>
     <t>22.09.2021 13:29:13 ----------
@@ -179,7 +224,8 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:29:02.
 Время завершения: 13:29:13.
-Продолжительность: 00:00:10.</t>
+Продолжительность: 00:00:10.
+------------------------------------------------</t>
   </si>
   <si>
     <t>22.09.2021 13:29:13 ----------
@@ -188,8 +234,6 @@
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "Фамилия Имя"
 Название теста: ""
-Файл с тестом: "C:\Users\tabakaev_mv\Desktop\РАБОТА\ТЕСТЫ\MyTest\Безымянный.mtf"
-CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
 Из них правильно: 2 (100,0% выполненых заданий).
@@ -202,13 +246,41 @@
 Маска времени обдумывания (в секундах): "1) 6 2) 4 ".
 Время начала: 13:29:02.
 Время завершения: 13:29:13.
-Продолжительность: 00:00:10.</t>
+Продолжительность: 00:00:10.
+------------------------------------------------</t>
   </si>
   <si>
     <t>Фамилия Имя</t>
   </si>
   <si>
+    <t>2598F9AC</t>
+  </si>
+  <si>
+    <t>100,0%</t>
+  </si>
+  <si>
+    <t>2,0 из 2 возможных. Ваш результат: 100,0%</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) + 2) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 6 2) 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2; 2) 2; </t>
+  </si>
+  <si>
+    <t>13:29:02</t>
+  </si>
+  <si>
+    <t>13:29:13</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
   </si>
   <si>
     <t>22.09.2021 13:47:58 ----------
@@ -233,7 +305,8 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:47:52.
 Время завершения: 13:47:58.
-Продолжительность: 00:00:06.</t>
+Продолжительность: 00:00:06.
+------------------------------------------------</t>
   </si>
   <si>
     <t>22.09.2021 13:47:58 ----------
@@ -242,8 +315,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "джлдлоогридл"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
-CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
 Из них правильно: 2 (100,0% выполненых заданий).
@@ -256,7 +327,8 @@
 Маска времени обдумывания (в секундах): "1) 3 2) 3 ".
 Время начала: 13:47:52.
 Время завершения: 13:47:58.
-Продолжительность: 00:00:06.</t>
+Продолжительность: 00:00:06.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K205-X04</t>
@@ -266,6 +338,21 @@
   </si>
   <si>
     <t>джлдлоогридл</t>
+  </si>
+  <si>
+    <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 3 2) 3 </t>
+  </si>
+  <si>
+    <t>13:47:52</t>
+  </si>
+  <si>
+    <t>13:47:58</t>
+  </si>
+  <si>
+    <t>00:00:06</t>
   </si>
   <si>
     <t>22.09.2021 13:48:39 ----------
@@ -290,7 +377,8 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:47:11.
 Время завершения: 13:48:39.
-Продолжительность: 00:01:26.</t>
+Продолжительность: 00:01:26.
+------------------------------------------------</t>
   </si>
   <si>
     <t>22.09.2021 13:48:39 ----------
@@ -299,8 +387,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "орпрдло"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
-CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
 Из них правильно: 0 (0,0% выполненых заданий).
@@ -313,13 +399,29 @@
 Маска времени обдумывания (в секундах): "1) 85 2) 1 ".
 Время начала: 13:47:11.
 Время завершения: 13:48:39.
-Продолжительность: 00:01:26.</t>
+Продолжительность: 00:01:26.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K205-X02</t>
   </si>
   <si>
     <t>орпрдло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 85 2) 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 3; 2) 4; </t>
+  </si>
+  <si>
+    <t>13:47:11</t>
+  </si>
+  <si>
+    <t>13:48:39</t>
+  </si>
+  <si>
+    <t>00:01:26</t>
   </si>
   <si>
     <t>22.09.2021 13:49:01 ----------
@@ -344,7 +446,8 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:45:32.
 Время завершения: 13:49:01.
-Продолжительность: 00:03:25.</t>
+Продолжительность: 00:03:25.
+------------------------------------------------</t>
   </si>
   <si>
     <t>22.09.2021 13:49:01 ----------
@@ -353,8 +456,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Петя"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
-CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
 Из них правильно: 1 (50,0% выполненых заданий).
@@ -367,7 +468,8 @@
 Маска времени обдумывания (в секундах): "1) 203 2) 1 ".
 Время начала: 13:45:32.
 Время завершения: 13:49:01.
-Продолжительность: 00:03:25.</t>
+Продолжительность: 00:03:25.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K205-X01</t>
@@ -376,7 +478,34 @@
     <t>Петя</t>
   </si>
   <si>
+    <t>1 (50,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>50,0%</t>
+  </si>
+  <si>
+    <t>1,0 из 2 возможных. Ваш результат: 50,0%</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 203 2) 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1; 2) 2; </t>
+  </si>
+  <si>
+    <t>13:45:32</t>
+  </si>
+  <si>
+    <t>13:49:01</t>
+  </si>
+  <si>
+    <t>00:03:25</t>
   </si>
   <si>
     <t>22.09.2021 13:50:34 ----------
@@ -401,7 +530,8 @@
 Маска штрафов за подсказку: "1) * 2) * ".
 Время начала: 13:44:46.
 Время завершения: 13:50:34.
-Продолжительность: 00:05:37.</t>
+Продолжительность: 00:05:37.
+------------------------------------------------</t>
   </si>
   <si>
     <t>22.09.2021 13:50:34 ----------
@@ -410,8 +540,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Вася"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf"
-CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 1.
 Из них правильно: 0 (0,0% выполненых заданий).
@@ -424,7 +552,8 @@
 Маска времени обдумывания (в секундах): "1) 337 2) * ".
 Время начала: 13:44:46.
 Время завершения: 13:50:34.
-Продолжительность: 00:05:37.</t>
+Продолжительность: 00:05:37.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K205-X09</t>
@@ -433,7 +562,22 @@
     <t>Вася</t>
   </si>
   <si>
-    <t xml:space="preserve">1) * 2) * </t>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 337 2) * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  2)  </t>
+  </si>
+  <si>
+    <t>13:44:46</t>
+  </si>
+  <si>
+    <t>13:50:34</t>
+  </si>
+  <si>
+    <t>00:05:37</t>
   </si>
   <si>
     <t>28.09.2021 10:43:58 ----------
@@ -458,7 +602,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 10:43:37.
 Время завершения: 10:43:58.
-Продолжительность: 00:00:20.</t>
+Продолжительность: 00:00:20.
+------------------------------------------------</t>
   </si>
   <si>
     <t>28.09.2021 10:43:58 ----------
@@ -467,8 +612,6 @@
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "оыважыва"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf"
-CRC Файла с тестом: "4F621F46"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 5 (16,7% выполненых заданий).
@@ -481,13 +624,53 @@
 Маска времени обдумывания (в секундах): "1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 1 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 1 25) 1 26) 0 27) 0 28) 0 29) 0 30) 0 ".
 Время начала: 10:43:37.
 Время завершения: 10:43:58.
-Продолжительность: 00:00:20.</t>
+Продолжительность: 00:00:20.
+------------------------------------------------</t>
   </si>
   <si>
     <t>оыважыва</t>
   </si>
   <si>
+    <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf</t>
+  </si>
+  <si>
+    <t>4F621F46</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>5 (16,7% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>25 (83,3% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>16,7%</t>
+  </si>
+  <si>
+    <t>5,0 из 30 возможных. Ваш результат: 16,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) - 3) + 4) - 5) + 6) - 7) - 8) - 9) - 10) - 11) - 12) - 13) - 14) - 15) - 16) - 17) - 18) - 19) + 20) - 21) + 22) - 23) - 24) - 25) + 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 1 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 1 25) 1 26) 0 27) 0 28) 0 29) 0 30) 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 3 2) 3; 3) 3 4) 3 5) 3 6) 3 7) 3 8) 4 9) 3 10) 3; 11) 3 12) 3 13) 3 14) 2 15) 2 16) 2; 17) 2 18) 2 19) 2 20) 2 21) 2 22) 2 23) 2 24) 2 25) 2 26) 2 27) 1 28) 1; 29) 1; 30) 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
+  </si>
+  <si>
+    <t>10:43:37</t>
+  </si>
+  <si>
+    <t>10:43:58</t>
+  </si>
+  <si>
+    <t>00:00:20</t>
   </si>
   <si>
     <t>28.09.2021 14:57:51 ----------
@@ -512,7 +695,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:57:32.
 Время завершения: 14:57:51.
-Продолжительность: 00:00:18.</t>
+Продолжительность: 00:00:18.
+------------------------------------------------</t>
   </si>
   <si>
     <t>28.09.2021 14:57:51 ----------
@@ -521,8 +705,6 @@
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "sdfjds"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 7 (23,3% выполненых заданий).
@@ -535,13 +717,47 @@
 Маска времени обдумывания (в секундах): "1) 5 2) 1 3) 1 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 0 30) 0 ".
 Время начала: 14:57:32.
 Время завершения: 14:57:51.
-Продолжительность: 00:00:18.</t>
+Продолжительность: 00:00:18.
+------------------------------------------------</t>
   </si>
   <si>
     <t>sdfjds</t>
   </si>
   <si>
+    <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf</t>
+  </si>
+  <si>
+    <t>554B1E8C</t>
+  </si>
+  <si>
+    <t>7 (23,3% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>23 (76,7% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>23,3%</t>
+  </si>
+  <si>
+    <t>7,0 из 30 возможных. Ваш результат: 23,3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) + 3) - 4) + 5) - 6) - 7) + 8) - 9) - 10) - 11) + 12) - 13) + 14) + 15) - 16) - 17) + 18) - 19) - 20) - 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 5 2) 1 3) 1 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 0 30) 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1; 2) 2 3) 1; 4) 1 5)  6) 1 7) 1 8) 1; 9) 1 10) 1; 11) 1 12) 1 13) 1 14) 1 15) 1 16) 1 17) 1 18)  19) 1 20) 1; 21) 1 22) 1 23) 1 24) 1; 25) 1; 26) 1 27)  28) 1 29) 1 30) 1 </t>
+  </si>
+  <si>
+    <t>14:57:32</t>
+  </si>
+  <si>
+    <t>14:57:51</t>
+  </si>
+  <si>
+    <t>00:00:18</t>
   </si>
   <si>
     <t>28.09.2021 14:59:57 ----------
@@ -566,7 +782,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:59:11.
 Время завершения: 14:59:57.
-Продолжительность: 00:00:44.</t>
+Продолжительность: 00:00:44.
+------------------------------------------------</t>
   </si>
   <si>
     <t>28.09.2021 14:59:57 ----------
@@ -575,8 +792,6 @@
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "kdfjgdfhgfghjf"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf"
-CRC Файла с тестом: "4F621F46"
 Всего заданий в тесте: 30.
 Выполнено заданий: 1.
 Из них правильно: 0 (0,0% выполненых заданий).
@@ -589,13 +804,29 @@
 Маска времени обдумывания (в секундах): "1) 44 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:59:11.
 Время завершения: 14:59:57.
-Продолжительность: 00:00:44.</t>
+Продолжительность: 00:00:44.
+------------------------------------------------</t>
   </si>
   <si>
     <t>kdfjgdfhgfghjf</t>
   </si>
   <si>
-    <t xml:space="preserve">1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
+    <t>0,0 из 30 возможных. Ваш результат: 0,0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 44 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  2)  3)  4)  5)  6)  7)  8)  9)  10)  11)  12)  13)  14)  15)  16)  17)  18)  19)  20)  21)  22)  23)  24)  25)  26)  27)  28)  29)  30)  </t>
+  </si>
+  <si>
+    <t>14:59:11</t>
+  </si>
+  <si>
+    <t>14:59:57</t>
+  </si>
+  <si>
+    <t>00:00:44</t>
   </si>
   <si>
     <t>05.10.2021 09:12:37 ----------
@@ -620,7 +851,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:08.
 Время завершения: 09:12:37.
-Продолжительность: 00:00:28.</t>
+Продолжительность: 00:00:28.
+------------------------------------------------</t>
   </si>
   <si>
     <t>05.10.2021 09:12:37 ----------
@@ -629,8 +861,6 @@
 Имя пользователя компьютера: "pucilo_ev"
 Имя пользователя (тестируемого): "я"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 2.
 Из них правильно: 0 (0,0% выполненых заданий).
@@ -643,7 +873,8 @@
 Маска времени обдумывания (в секундах): "1) 19 2) 8 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:08.
 Время завершения: 09:12:37.
-Продолжительность: 00:00:28.</t>
+Продолжительность: 00:00:28.
+------------------------------------------------</t>
   </si>
   <si>
     <t>PUCILO-EV</t>
@@ -656,6 +887,21 @@
   </si>
   <si>
     <t xml:space="preserve">1) - 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 19 2) 8 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1; 2)  3)  4)  5)  6)  7)  8)  9)  10)  11)  12)  13)  14)  15)  16)  17)  18)  19)  20)  21)  22)  23)  24)  25)  26)  27)  28)  29)  30)  </t>
+  </si>
+  <si>
+    <t>09:12:08</t>
+  </si>
+  <si>
+    <t>09:12:37</t>
+  </si>
+  <si>
+    <t>00:00:28</t>
   </si>
   <si>
     <t>05.10.2021 09:13:01 ----------
@@ -680,7 +926,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:11.
 Время завершения: 09:13:00.
-Продолжительность: 00:00:48.</t>
+Продолжительность: 00:00:48.
+------------------------------------------------</t>
   </si>
   <si>
     <t>05.10.2021 09:13:01 ----------
@@ -689,8 +936,6 @@
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "sdfklsdfsdgsd"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 1.
 Из них правильно: 0 (0,0% выполненых заданий).
@@ -703,10 +948,23 @@
 Маска времени обдумывания (в секундах): "1) 48 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:11.
 Время завершения: 09:13:00.
-Продолжительность: 00:00:48.</t>
+Продолжительность: 00:00:48.
+------------------------------------------------</t>
   </si>
   <si>
     <t>sdfklsdfsdgsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 48 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
+  </si>
+  <si>
+    <t>09:12:11</t>
+  </si>
+  <si>
+    <t>09:13:00</t>
+  </si>
+  <si>
+    <t>00:00:48</t>
   </si>
   <si>
     <t>06.10.2021 15:01:45 ----------
@@ -731,7 +989,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 14:57:52.
 Время завершения: 15:01:45.
-Продолжительность: 00:03:45.</t>
+Продолжительность: 00:03:45.
+------------------------------------------------</t>
   </si>
   <si>
     <t>06.10.2021 15:01:45 ----------
@@ -740,8 +999,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Фамилия Имя"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf"
-CRC Файла с тестом: "4F621F46"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 8 (26,7% выполненых заданий).
@@ -754,10 +1011,38 @@
 Маска времени обдумывания (в секундах): "1) 8 2) 4 3) 3 4) 4 5) 2 6) 3 7) 3 8) 4 9) 6 10) 6 11) 7 12) 6 13) 4 14) 5 15) 4 16) 2 17) 3 18) 6 19) 51 20) 4 21) 2 22) 4 23) 3 24) 5 25) 3 26) 3 27) 6 28) 37 29) 4 30) 9 ".
 Время начала: 14:57:52.
 Время завершения: 15:01:45.
-Продолжительность: 00:03:45.</t>
+Продолжительность: 00:03:45.
+------------------------------------------------</t>
+  </si>
+  <si>
+    <t>8 (26,7% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>22 (73,3% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>26,7%</t>
+  </si>
+  <si>
+    <t>8,0 из 30 возможных. Ваш результат: 26,7%</t>
   </si>
   <si>
     <t xml:space="preserve">1) - 2) - 3) - 4) - 5) + 6) + 7) - 8) - 9) + 10) - 11) + 12) + 13) + 14) - 15) - 16) - 17) - 18) - 19) - 20) - 21) - 22) - 23) - 24) + 25) - 26) - 27) - 28) - 29) - 30) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 8 2) 4 3) 3 4) 4 5) 2 6) 3 7) 3 8) 4 9) 6 10) 6 11) 7 12) 6 13) 4 14) 5 15) 4 16) 2 17) 3 18) 6 19) 51 20) 4 21) 2 22) 4 23) 3 24) 5 25) 3 26) 3 27) 6 28) 37 29) 4 30) 9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1 2) 3; 3) 2 4) 3 5) 3 6) 2 7) 3 8) 5 9) 1 10) 1; 11) 2 12) 1 13) 2 14) 2 15) 2 16) 2; 17) 3 18) 1 19) 3 20) 2 21) 1 22) 3 23) 1 24) 3 25) 3 26) 4 27) 3 28) 3;4; 29) 2;3; 30) 3 </t>
+  </si>
+  <si>
+    <t>14:57:52</t>
+  </si>
+  <si>
+    <t>15:01:45</t>
+  </si>
+  <si>
+    <t>00:03:45</t>
   </si>
   <si>
     <t>12.10.2021 17:10:17 ----------
@@ -782,7 +1067,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 17:10:02.
 Время завершения: 17:10:17.
-Продолжительность: 00:00:14.</t>
+Продолжительность: 00:00:14.
+------------------------------------------------</t>
   </si>
   <si>
     <t>12.10.2021 17:10:17 ----------
@@ -791,8 +1077,6 @@
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "lkjg;ldfjgiljg"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
-CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 4 (13,3% выполненых заданий).
@@ -805,13 +1089,47 @@
 Маска времени обдумывания (в секундах): "1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 1 30) 0 ".
 Время начала: 17:10:02.
 Время завершения: 17:10:17.
-Продолжительность: 00:00:14.</t>
+Продолжительность: 00:00:14.
+------------------------------------------------</t>
   </si>
   <si>
     <t>lkjg;ldfjgiljg</t>
   </si>
   <si>
+    <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf</t>
+  </si>
+  <si>
+    <t>5A416D2A</t>
+  </si>
+  <si>
+    <t>4 (13,3% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>26 (86,7% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>13,3%</t>
+  </si>
+  <si>
+    <t>4,0 из 30 возможных. Ваш результат: 13,3%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) - 3) - 4) - 5) - 6) - 7) - 8) + 9) - 10) + 11) - 12) - 13) - 14) + 15) - 16) - 17) - 18) - 19) + 20) - 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 3 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 0 29) 1 30) 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2 2) 2 3) 2 4) 2 5) 2 6) 2 7) 2 8) 2 9) 2 10) 2 11) 2 12) 2 13) 2 14) 2 15) 2 16) 2 17) 2 18) 2 19) 2 20) 2 21) 2 22) 2; 23) 2 24) 3; 25) 2 26) 2; 27) 2 28) 2 29) 2 30) 2 </t>
+  </si>
+  <si>
+    <t>17:10:02</t>
+  </si>
+  <si>
+    <t>17:10:17</t>
+  </si>
+  <si>
+    <t>00:00:14</t>
   </si>
   <si>
     <t>12.10.2021 17:10:46 ----------
@@ -836,7 +1154,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 17:10:34.
 Время завершения: 17:10:46.
-Продолжительность: 00:00:12.</t>
+Продолжительность: 00:00:12.
+------------------------------------------------</t>
   </si>
   <si>
     <t>12.10.2021 17:10:46 ----------
@@ -845,8 +1164,6 @@
 Имя пользователя компьютера: "tabakaev_mv"
 Имя пользователя (тестируемого): "lkjg;ldfjgiljg"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников продовольственной торговли.mtf"
-CRC Файла с тестом: "7AC88467"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 15 (50,0% выполненых заданий).
@@ -859,10 +1176,38 @@
 Маска времени обдумывания (в секундах): "1) 1 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 1 29) 0 30) 0 ".
 Время начала: 17:10:34.
 Время завершения: 17:10:46.
-Продолжительность: 00:00:12.</t>
+Продолжительность: 00:00:12.
+------------------------------------------------</t>
+  </si>
+  <si>
+    <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников продовольственной торговли.mtf</t>
+  </si>
+  <si>
+    <t>7AC88467</t>
+  </si>
+  <si>
+    <t>15 (50,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>15,0 из 30 возможных. Ваш результат: 50,0%</t>
   </si>
   <si>
     <t xml:space="preserve">1) + 2) - 3) + 4) + 5) - 6) + 7) + 8) + 9) + 10) - 11) + 12) + 13) + 14) - 15) - 16) + 17) + 18) - 19) + 20) - 21) + 22) - 23) - 24) - 25) + 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1 2) 0 3) 0 4) 0 5) 0 6) 0 7) 0 8) 0 9) 0 10) 0 11) 0 12) 0 13) 0 14) 0 15) 0 16) 0 17) 0 18) 0 19) 0 20) 0 21) 0 22) 0 23) 0 24) 0 25) 0 26) 0 27) 0 28) 1 29) 0 30) 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 3 2) 3 3) 3 4) 3 5) 3; 6) 3 7) 3 8) 3 9) 3 10) 3 11) 3 12) 3 13) 3 14) 3 15) 3 16) 3 17) 3 18) 3; 19) 3 20) 3 21) 3 22) 3 23) 3; 24) 3; 25) 3 26) 3 27) 4; 28) 3 29) 3 30) 3 </t>
+  </si>
+  <si>
+    <t>17:10:34</t>
+  </si>
+  <si>
+    <t>17:10:46</t>
+  </si>
+  <si>
+    <t>00:00:12</t>
   </si>
   <si>
     <t>13.10.2021 09:21:40 ----------
@@ -887,7 +1232,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:10:20.
 Время завершения: 09:21:40.
-Продолжительность: 00:11:10.</t>
+Продолжительность: 00:11:10.
+------------------------------------------------</t>
   </si>
   <si>
     <t>13.10.2021 09:21:40 ----------
@@ -896,8 +1242,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "озерова елизавета денисовна"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 9 (30,0% выполненых заданий).
@@ -910,7 +1254,8 @@
 Маска времени обдумывания (в секундах): "1) 50 2) 29 3) 92 4) 27 5) 12 6) 16 7) 17 8) 13 9) 13 10) 10 11) 24 12) 16 13) 9 14) 7 15) 44 16) 13 17) 18 18) 14 19) 40 20) 12 21) 15 22) 10 23) 50 24) 18 25) 13 26) 11 27) 16 28) 24 29) 12 30) 12 ".
 Время начала: 09:10:20.
 Время завершения: 09:21:40.
-Продолжительность: 00:11:10.</t>
+Продолжительность: 00:11:10.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K205-X06</t>
@@ -919,7 +1264,34 @@
     <t>озерова елизавета денисовна</t>
   </si>
   <si>
+    <t>9 (30,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>21 (70,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>30,0%</t>
+  </si>
+  <si>
+    <t>9,0 из 30 возможных. Ваш результат: 30,0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) + 3) - 4) - 5) - 6) + 7) + 8) - 9) - 10) - 11) + 12) - 13) + 14) + 15) - 16) + 17) + 18) - 19) - 20) - 21) - 22) + 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 50 2) 29 3) 92 4) 27 5) 12 6) 16 7) 17 8) 13 9) 13 10) 10 11) 24 12) 16 13) 9 14) 7 15) 44 16) 13 17) 18 18) 14 19) 40 20) 12 21) 15 22) 10 23) 50 24) 18 25) 13 26) 11 27) 16 28) 24 29) 12 30) 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1; 2) 2 3) 1; 4) 2 5) 2; 6) 3 7) 1 8) 1; 9) 3 10) 1; 11) 1 12) 1 13) 1 14) 1 15) 3 16) 2 17) 1 18) 2; 19) 1 20) 1; 21) 2 22) 2 23) 1 24) 1; 25) 2; 26) 3 27) 1; 28) 2 29) 2 30) 1 </t>
+  </si>
+  <si>
+    <t>09:10:20</t>
+  </si>
+  <si>
+    <t>09:21:40</t>
+  </si>
+  <si>
+    <t>00:11:10</t>
   </si>
   <si>
     <t>13.10.2021 09:28:48 ----------
@@ -944,7 +1316,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:10:42.
 Время завершения: 09:28:48.
-Продолжительность: 00:17:50.</t>
+Продолжительность: 00:17:50.
+------------------------------------------------</t>
   </si>
   <si>
     <t>13.10.2021 09:28:48 ----------
@@ -953,8 +1326,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Лоскутова"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
-CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 17 (56,7% выполненых заданий).
@@ -967,7 +1338,8 @@
 Маска времени обдумывания (в секундах): "1) 48 2) 15 3) 14 4) 13 5) 37 6) 11 7) 13 8) 8 9) 23 10) 15 11) 12 12) 41 13) 42 14) 73 15) 13 16) 10 17) 93 18) 14 19) 43 20) 14 21) 31 22) 75 23) 68 24) 44 25) 40 26) 108 27) 26 28) 49 29) 33 30) 30 ".
 Время начала: 09:10:42.
 Время завершения: 09:28:48.
-Продолжительность: 00:17:50.</t>
+Продолжительность: 00:17:50.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K205-X08</t>
@@ -976,7 +1348,34 @@
     <t>Лоскутова</t>
   </si>
   <si>
+    <t>17 (56,7% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>13 (43,3% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>56,7%</t>
+  </si>
+  <si>
+    <t>17,0 из 30 возможных. Ваш результат: 56,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) + 3) + 4) + 5) - 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) + 17) + 18) + 19) - 20) + 21) - 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 48 2) 15 3) 14 4) 13 5) 37 6) 11 7) 13 8) 8 9) 23 10) 15 11) 12 12) 41 13) 42 14) 73 15) 13 16) 10 17) 93 18) 14 19) 43 20) 14 21) 31 22) 75 23) 68 24) 44 25) 40 26) 108 27) 26 28) 49 29) 33 30) 30 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2 2) 3 3) 3 4) 1 5) 1 6) 1 7) 1 8) 2 9) 3 10) 2 11) 1 12) 1 13) 1 14) 2 15) 1 16) 3 17) 3 18) 3 19) 3 20) 3 21) 2 22) 2; 23) 5 24) 3; 25) 2 26) 3;5; 27) 1 28) 1 29) 1 30) 4 </t>
+  </si>
+  <si>
+    <t>09:10:42</t>
+  </si>
+  <si>
+    <t>09:28:48</t>
+  </si>
+  <si>
+    <t>00:17:50</t>
   </si>
   <si>
     <t>13.10.2021 09:34:31 ----------
@@ -1001,7 +1400,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:17.
 Время завершения: 09:34:31.
-Продолжительность: 00:21:55.</t>
+Продолжительность: 00:21:55.
+------------------------------------------------</t>
   </si>
   <si>
     <t>13.10.2021 09:34:31 ----------
@@ -1010,8 +1410,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Туманова Ирина Леонидовна"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
-CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 23 (76,7% выполненых заданий).
@@ -1024,13 +1422,38 @@
 Маска времени обдумывания (в секундах): "1) 35 2) 17 3) 45 4) 14 5) 29 6) 24 7) 29 8) 28 9) 33 10) 25 11) 26 12) 176 13) 21 14) 162 15) 32 16) 24 17) 41 18) 19 19) 11 20) 18 21) 45 22) 59 23) 34 24) 86 25) 57 26) 56 27) 29 28) 57 29) 44 30) 23 ".
 Время начала: 09:12:17.
 Время завершения: 09:34:31.
-Продолжительность: 00:21:55.</t>
+Продолжительность: 00:21:55.
+------------------------------------------------</t>
   </si>
   <si>
     <t>Туманова Ирина Леонидовна</t>
   </si>
   <si>
+    <t>76,7%</t>
+  </si>
+  <si>
+    <t>23,0 из 30 возможных. Ваш результат: 76,7%</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) + 2) + 3) + 4) + 5) + 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) + 19) + 20) + 21) + 22) - 23) - 24) - 25) - 26) - 27) - 28) + 29) + 30) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 35 2) 17 3) 45 4) 14 5) 29 6) 24 7) 29 8) 28 9) 33 10) 25 11) 26 12) 176 13) 21 14) 162 15) 32 16) 24 17) 41 18) 19 19) 11 20) 18 21) 45 22) 59 23) 34 24) 86 25) 57 26) 56 27) 29 28) 57 29) 44 30) 23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 4 2) 3 3) 3 4) 1 5) 3 6) 1 7) 1 8) 2 9) 3 10) 2 11) 1 12) 1 13) 1 14) 2 15) 1 16) 1 17) 3 18) 3 19) 2 20) 3 21) 4 22) 3; 23) 5 24) 5; 25) 1 26) 6; 27) 4 28) 4 29) 4 30) 5 </t>
+  </si>
+  <si>
+    <t>09:12:17</t>
+  </si>
+  <si>
+    <t>09:34:31</t>
+  </si>
+  <si>
+    <t>00:21:55</t>
   </si>
   <si>
     <t>13.10.2021 09:39:34 ----------
@@ -1055,7 +1478,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:14:34.
 Время завершения: 09:39:34.
-Продолжительность: 00:24:39.</t>
+Продолжительность: 00:24:39.
+------------------------------------------------</t>
   </si>
   <si>
     <t>13.10.2021 09:39:34 ----------
@@ -1064,8 +1488,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Романцов Дмитрий Ильич"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
-CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 20 (66,7% выполненых заданий).
@@ -1078,13 +1500,41 @@
 Маска времени обдумывания (в секундах): "1) 78 2) 35 3) 18 4) 14 5) 45 6) 44 7) 19 8) 9 9) 44 10) 25 11) 24 12) 130 13) 27 14) 75 15) 29 16) 25 17) 23 18) 16 19) 44 20) 32 21) 35 22) 48 23) 78 24) 154 25) 61 26) 43 27) 47 28) 94 29) 74 30) 73 ".
 Время начала: 09:14:34.
 Время завершения: 09:39:34.
-Продолжительность: 00:24:39.</t>
+Продолжительность: 00:24:39.
+------------------------------------------------</t>
   </si>
   <si>
     <t>Романцов Дмитрий Ильич</t>
   </si>
   <si>
+    <t>20 (66,7% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>10 (33,3% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>66,7%</t>
+  </si>
+  <si>
+    <t>20,0 из 30 возможных. Ваш результат: 66,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) + 3) + 4) + 5) + 6) - 7) + 8) + 9) + 10) + 11) + 12) - 13) + 14) + 15) + 16) - 17) + 18) + 19) + 20) + 21) + 22) - 23) - 24) - 25) - 26) - 27) + 28) + 29) - 30) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 78 2) 35 3) 18 4) 14 5) 45 6) 44 7) 19 8) 9 9) 44 10) 25 11) 24 12) 130 13) 27 14) 75 15) 29 16) 25 17) 23 18) 16 19) 44 20) 32 21) 35 22) 48 23) 78 24) 154 25) 61 26) 43 27) 47 28) 94 29) 74 30) 73 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2 2) 3 3) 3 4) 1 5) 3 6) 2 7) 1 8) 2 9) 3 10) 2 11) 1 12) 3 13) 1 14) 2 15) 1 16) 1 17) 3 18) 3 19) 2 20) 3 21) 4 22) 3; 23) 2 24) 2;5;6; 25) 2 26) 6; 27) 5 28) 4 29) 2 30) 5 </t>
+  </si>
+  <si>
+    <t>09:14:34</t>
+  </si>
+  <si>
+    <t>09:39:34</t>
+  </si>
+  <si>
+    <t>00:24:39</t>
   </si>
   <si>
     <t>13.10.2021 09:39:40 ----------
@@ -1109,7 +1559,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:14:36.
 Время завершения: 09:39:40.
-Продолжительность: 00:24:43.</t>
+Продолжительность: 00:24:43.
+------------------------------------------------</t>
   </si>
   <si>
     <t>13.10.2021 09:39:40 ----------
@@ -1118,8 +1569,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Андреева Снежана Генадьевна"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
-CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 20 (66,7% выполненых заданий).
@@ -1132,10 +1581,26 @@
 Маска времени обдумывания (в секундах): "1) 72 2) 33 3) 30 4) 22 5) 54 6) 27 7) 17 8) 19 9) 41 10) 24 11) 21 12) 134 13) 16 14) 85 15) 26 16) 23 17) 28 18) 17 19) 37 20) 30 21) 39 22) 49 23) 70 24) 196 25) 23 26) 42 27) 52 28) 93 29) 75 30) 72 ".
 Время начала: 09:14:36.
 Время завершения: 09:39:40.
-Продолжительность: 00:24:43.</t>
+Продолжительность: 00:24:43.
+------------------------------------------------</t>
   </si>
   <si>
     <t>Андреева Снежана Генадьевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 72 2) 33 3) 30 4) 22 5) 54 6) 27 7) 17 8) 19 9) 41 10) 24 11) 21 12) 134 13) 16 14) 85 15) 26 16) 23 17) 28 18) 17 19) 37 20) 30 21) 39 22) 49 23) 70 24) 196 25) 23 26) 42 27) 52 28) 93 29) 75 30) 72 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2 2) 3 3) 3 4) 1 5) 3 6) 2 7) 1 8) 2 9) 3 10) 2 11) 1 12) 3 13) 1 14) 2 15) 1 16) 1 17) 3 18) 3 19) 2 20) 3 21) 4 22) 3; 23) 2 24) 5;6; 25) 2 26) 6; 27) 5 28) 4 29) 2 30) 5 </t>
+  </si>
+  <si>
+    <t>09:14:36</t>
+  </si>
+  <si>
+    <t>09:39:40</t>
+  </si>
+  <si>
+    <t>00:24:43</t>
   </si>
   <si>
     <t>13.10.2021 09:44:54 ----------
@@ -1160,7 +1625,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:11:06.
 Время завершения: 09:44:54.
-Продолжительность: 00:33:20.</t>
+Продолжительность: 00:33:20.
+------------------------------------------------</t>
   </si>
   <si>
     <t>13.10.2021 09:44:54 ----------
@@ -1169,8 +1635,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Белоусова Наталья"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 18 (60,0% выполненых заданий).
@@ -1183,7 +1647,8 @@
 Маска времени обдумывания (в секундах): "1) 233 2) 246 3) 64 4) 178 5) 78 6) 30 7) 16 8) 40 9) 12 10) 62 11) 10 12) 9 13) 27 14) 19 15) 13 16) 17 17) 46 18) 182 19) 30 20) 26 21) 41 22) 182 23) 17 24) 36 25) 60 26) 110 27) 48 28) 109 29) 22 30) 20 ".
 Время начала: 09:11:06.
 Время завершения: 09:44:54.
-Продолжительность: 00:33:20.</t>
+Продолжительность: 00:33:20.
+------------------------------------------------</t>
   </si>
   <si>
     <t>SHA-K205-X07</t>
@@ -1192,7 +1657,34 @@
     <t>Белоусова Наталья</t>
   </si>
   <si>
+    <t>18 (60,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>12 (40,0% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>60,0%</t>
+  </si>
+  <si>
+    <t>18,0 из 30 возможных. Ваш результат: 60,0%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) + 2) + 3) - 4) + 5) + 6) - 7) + 8) - 9) + 10) - 11) + 12) + 13) - 14) + 15) + 16) + 17) + 18) - 19) + 20) + 21) - 22) + 23) + 24) - 25) - 26) + 27) - 28) - 29) + 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 233 2) 246 3) 64 4) 178 5) 78 6) 30 7) 16 8) 40 9) 12 10) 62 11) 10 12) 9 13) 27 14) 19 15) 13 16) 17 17) 46 18) 182 19) 30 20) 26 21) 41 22) 182 23) 17 24) 36 25) 60 26) 110 27) 48 28) 109 29) 22 30) 20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1;3; 2) 2 3) 2;3;4; 4) 1 5) 1;2; 6) 1 7) 1 8) 1;4; 9) 2 10) 1;2; 11) 1 12) 2 13) 2 14) 1 15) 2 16) 2 17) 1 18) 2; 19) 2 20) 1;2; 21) 4 22) 2 23) 2 24) 1;2;4;5; 25) 1;2; 26) 2 27) 2;3;4;6; 28) 1 29) 4 30) 1 </t>
+  </si>
+  <si>
+    <t>09:11:06</t>
+  </si>
+  <si>
+    <t>09:44:54</t>
+  </si>
+  <si>
+    <t>00:33:20</t>
   </si>
   <si>
     <t>13.10.2021 09:51:08 ----------
@@ -1217,7 +1709,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:12:37.
 Время завершения: 09:51:08.
-Продолжительность: 00:37:59.</t>
+Продолжительность: 00:37:59.
+------------------------------------------------</t>
   </si>
   <si>
     <t>13.10.2021 09:51:08 ----------
@@ -1226,8 +1719,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Петрова Марина Алексеевна"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 20 (66,7% выполненых заданий).
@@ -1240,13 +1731,26 @@
 Маска времени обдумывания (в секундах): "1) 144 2) 26 3) 13 4) 373 5) 351 6) 4 7) 9 8) 207 9) 9 10) 82 11) 83 12) 8 13) 9 14) 8 15) 4 16) 6 17) 34 18) 81 19) 57 20) 51 21) 76 22) 112 23) 8 24) 10 25) 134 26) 207 27) 118 28) 13 29) 13 30) 15 ".
 Время начала: 09:12:37.
 Время завершения: 09:51:08.
-Продолжительность: 00:37:59.</t>
+Продолжительность: 00:37:59.
+------------------------------------------------</t>
   </si>
   <si>
     <t>Петрова Марина Алексеевна</t>
   </si>
   <si>
     <t xml:space="preserve">1) + 2) + 3) - 4) + 5) + 6) + 7) + 8) - 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) + 17) + 18) - 19) - 20) + 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) + 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 144 2) 26 3) 13 4) 373 5) 351 6) 4 7) 9 8) 207 9) 9 10) 82 11) 83 12) 8 13) 9 14) 8 15) 4 16) 6 17) 34 18) 81 19) 57 20) 51 21) 76 22) 112 23) 8 24) 10 25) 134 26) 207 27) 118 28) 13 29) 13 30) 15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1;3; 2) 2 3) 3; 4) 1 5) 1;2; 6) 3 7) 1 8) 4; 9) 2 10) 1;2;3;4; 11) 1 12) 2 13) 1 14) 1 15) 2 16) 2 17) 1 18) 2; 19) 3 20) 1;2; 21) 4 22) 2 23) 2 24) 6; 25) 1;2;4; 26) 1 27) 1;2;5; 28) 3 29) 4 30) 1 </t>
+  </si>
+  <si>
+    <t>09:51:08</t>
+  </si>
+  <si>
+    <t>00:37:59</t>
   </si>
   <si>
     <t>20.10.2021 09:09:04 ----------
@@ -1271,7 +1775,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 08:57:10.
 Время завершения: 09:09:04.
-Продолжительность: 00:11:43.</t>
+Продолжительность: 00:11:43.
+------------------------------------------------</t>
   </si>
   <si>
     <t>20.10.2021 09:09:04 ----------
@@ -1280,8 +1785,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "озерова елизавета денисовна"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 9 (30,0% выполненых заданий).
@@ -1294,10 +1797,26 @@
 Маска времени обдумывания (в секундах): "1) 17 2) 35 3) 19 4) 54 5) 43 6) 5 7) 15 8) 33 9) 14 10) 30 11) 12 12) 33 13) 23 14) 21 15) 37 16) 16 17) 18 18) 17 19) 12 20) 15 21) 42 22) 15 23) 22 24) 19 25) 12 26) 11 27) 47 28) 11 29) 16 30) 25 ".
 Время начала: 08:57:10.
 Время завершения: 09:09:04.
-Продолжительность: 00:11:43.</t>
+Продолжительность: 00:11:43.
+------------------------------------------------</t>
   </si>
   <si>
     <t xml:space="preserve">1) - 2) - 3) - 4) - 5) - 6) + 7) + 8) - 9) + 10) - 11) + 12) - 13) - 14) + 15) + 16) + 17) + 18) - 19) - 20) - 21) + 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 17 2) 35 3) 19 4) 54 5) 43 6) 5 7) 15 8) 33 9) 14 10) 30 11) 12 12) 33 13) 23 14) 21 15) 37 16) 16 17) 18 18) 17 19) 12 20) 15 21) 42 22) 15 23) 22 24) 19 25) 12 26) 11 27) 47 28) 11 29) 16 30) 25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1; 2) 1 3) 1; 4) 2 5) 2; 6) 3 7) 1 8) 4; 9) 2 10) 3; 11) 1 12) 1 13) 2 14) 1 15) 2 16) 2 17) 1 18) 2; 19) 1 20) 1; 21) 3 22) 3 23) 1 24) 1; 25) 1; 26) 3 27) 3; 28) 2 29) 2 30) 1 </t>
+  </si>
+  <si>
+    <t>08:57:10</t>
+  </si>
+  <si>
+    <t>09:09:04</t>
+  </si>
+  <si>
+    <t>00:11:43</t>
   </si>
   <si>
     <t>20.10.2021 09:17:40 ----------
@@ -1322,7 +1841,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 08:57:30.
 Время завершения: 09:17:40.
-Продолжительность: 00:19:53.</t>
+Продолжительность: 00:19:53.
+------------------------------------------------</t>
   </si>
   <si>
     <t>20.10.2021 09:17:40 ----------
@@ -1331,8 +1851,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "кекина людмила федоровна"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 14 (46,7% выполненых заданий).
@@ -1345,13 +1863,41 @@
 Маска времени обдумывания (в секундах): "1) 47 2) 79 3) 38 4) 52 5) 27 6) 17 7) 15 8) 40 9) 33 10) 32 11) 28 12) 31 13) 24 14) 17 15) 59 16) 20 17) 23 18) 63 19) 38 20) 21 21) 83 22) 36 23) 21 24) 30 25) 56 26) 34 27) 36 28) 81 29) 46 30) 51 ".
 Время начала: 08:57:30.
 Время завершения: 09:17:40.
-Продолжительность: 00:19:53.</t>
+Продолжительность: 00:19:53.
+------------------------------------------------</t>
   </si>
   <si>
     <t>кекина людмила федоровна</t>
   </si>
   <si>
+    <t>14 (46,7% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>16 (53,3% выполненых заданий).</t>
+  </si>
+  <si>
+    <t>46,7%</t>
+  </si>
+  <si>
+    <t>14,0 из 30 возможных. Ваш результат: 46,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) + 3) - 4) - 5) - 6) + 7) + 8) - 9) + 10) - 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) - 19) + 20) - 21) - 22) - 23) + 24) - 25) - 26) - 27) - 28) - 29) + 30) + </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 47 2) 79 3) 38 4) 52 5) 27 6) 17 7) 15 8) 40 9) 33 10) 32 11) 28 12) 31 13) 24 14) 17 15) 59 16) 20 17) 23 18) 63 19) 38 20) 21 21) 83 22) 36 23) 21 24) 30 25) 56 26) 34 27) 36 28) 81 29) 46 30) 51 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 4; 2) 2 3) 2; 4) 2 5) 3; 6) 3 7) 1 8) 4; 9) 2 10) 1; 11) 1 12) 2 13) 1 14) 1 15) 2 16) 3 17) 1 18) 1; 19) 2 20) 1; 21) 4 22) 1 23) 2 24) 6; 25) 1;4; 26) 1 27) 3; 28) 2 29) 4 30) 2 </t>
+  </si>
+  <si>
+    <t>08:57:30</t>
+  </si>
+  <si>
+    <t>09:17:40</t>
+  </si>
+  <si>
+    <t>00:19:53</t>
   </si>
   <si>
     <t>20.10.2021 09:48:00 ----------
@@ -1376,7 +1922,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 09:04:10.
 Время завершения: 09:48:00.
-Продолжительность: 00:43:13.</t>
+Продолжительность: 00:43:13.
+------------------------------------------------</t>
   </si>
   <si>
     <t>20.10.2021 09:48:00 ----------
@@ -1385,8 +1932,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Романцов Дмитрий Ильич"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf"
-CRC Файла с тестом: "2C7EB1D6"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 21 (70,0% выполненых заданий).
@@ -1399,10 +1944,35 @@
 Маска времени обдумывания (в секундах): "1) 193 2) 48 3) 17 4) 6 5) 36 6) 82 7) 7 8) 6 9) 86 10) 15 11) 24 12) 82 13) 19 14) 120 15) 7 16) 70 17) 9 18) 43 19) 243 20) 207 21) 105 22) 60 23) 343 24) 171 25) 65 26) 25 27) 186 28) 192 29) 47 30) 64 ".
 Время начала: 09:04:10.
 Время завершения: 09:48:00.
-Продолжительность: 00:43:13.</t>
+Продолжительность: 00:43:13.
+------------------------------------------------</t>
+  </si>
+  <si>
+    <t>2C7EB1D6</t>
+  </si>
+  <si>
+    <t>70,0%</t>
+  </si>
+  <si>
+    <t>21,0 из 30 возможных. Ваш результат: 70,0%</t>
   </si>
   <si>
     <t xml:space="preserve">1) + 2) + 3) + 4) + 5) + 6) + 7) + 8) + 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) - 17) + 18) + 19) - 20) - 21) + 22) - 23) + 24) - 25) - 26) - 27) + 28) + 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 193 2) 48 3) 17 4) 6 5) 36 6) 82 7) 7 8) 6 9) 86 10) 15 11) 24 12) 82 13) 19 14) 120 15) 7 16) 70 17) 9 18) 43 19) 243 20) 207 21) 105 22) 60 23) 343 24) 171 25) 65 26) 25 27) 186 28) 192 29) 47 30) 64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 4 2) 3 3) 3 4) 1 5) 3 6) 1 7) 1 8) 2 9) 3 10) 2 11) 1 12) 1 13) 1 14) 2 15) 1 16) 1 17) 3 18) 3 19) 3 20) 2 21) 4 22) 2; 23) 1 24) 2;4;5;7; 25) 1 26) 6; 27) 5 28) 4 29) 2 30) 4 </t>
+  </si>
+  <si>
+    <t>09:04:10</t>
+  </si>
+  <si>
+    <t>09:48:00</t>
+  </si>
+  <si>
+    <t>00:43:13</t>
   </si>
   <si>
     <t>10.01.2022 17:28:01 ----------
@@ -1427,7 +1997,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 17:26:58.
 Время завершения: 17:28:01.
-Продолжительность: 00:01:02.</t>
+Продолжительность: 00:01:02.
+------------------------------------------------</t>
   </si>
   <si>
     <t>10.01.2022 17:28:01 ----------
@@ -1436,8 +2007,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Фамилия Имя"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 7 (23,3% выполненых заданий).
@@ -1450,10 +2019,26 @@
 Маска времени обдумывания (в секундах): "1) 6 2) 3 3) 2 4) 1 5) 1 6) 1 7) 1 8) 1 9) 1 10) 1 11) 1 12) 1 13) 1 14) 1 15) 1 16) 3 17) 1 18) 1 19) 1 20) 1 21) 1 22) 3 23) 2 24) 1 25) 1 26) 2 27) 1 28) 1 29) 1 30) 1 ".
 Время начала: 17:26:58.
 Время завершения: 17:28:01.
-Продолжительность: 00:01:02.</t>
+Продолжительность: 00:01:02.
+------------------------------------------------</t>
   </si>
   <si>
     <t xml:space="preserve">1) - 2) + 3) - 4) + 5) - 6) - 7) + 8) - 9) - 10) - 11) - 12) - 13) - 14) - 15) - 16) - 17) + 18) - 19) - 20) - 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 6 2) 3 3) 2 4) 1 5) 1 6) 1 7) 1 8) 1 9) 1 10) 1 11) 1 12) 1 13) 1 14) 1 15) 1 16) 3 17) 1 18) 1 19) 1 20) 1 21) 1 22) 3 23) 2 24) 1 25) 1 26) 2 27) 1 28) 1 29) 1 30) 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 1; 2) 2 3) 1; 4) 1 5) 1; 6) 1 7) 1 8) 1; 9) 1 10) 2; 11) 3 12) 3 13) 3 14) 3 15) 3 16) 1 17) 1 18) 1; 19) 1 20) 1; 21) 1 22) 2 23) 2 24) 3; 25) 3; 26) 3 27) 4; 28) 3 29) 3 30) 3 </t>
+  </si>
+  <si>
+    <t>17:26:58</t>
+  </si>
+  <si>
+    <t>17:28:01</t>
+  </si>
+  <si>
+    <t>00:01:02</t>
   </si>
   <si>
     <t>19.01.2022 10:22:18 ----------
@@ -1478,7 +2063,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 10:20:33.
 Время завершения: 10:22:18.
-Продолжительность: 00:01:44.</t>
+Продолжительность: 00:01:44.
+------------------------------------------------</t>
   </si>
   <si>
     <t>19.01.2022 10:22:18 ----------
@@ -1487,8 +2073,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Важенина"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников продовольственной торговли.mtf"
-CRC Файла с тестом: "1D498E48"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 9 (30,0% выполненых заданий).
@@ -1501,13 +2085,32 @@
 Маска времени обдумывания (в секундах): "1) 7 2) 6 3) 4 4) 2 5) 2 6) 3 7) 2 8) 4 9) 2 10) 2 11) 2 12) 2 13) 2 14) 2 15) 2 16) 2 17) 2 18) 2 19) 2 20) 4 21) 11 22) 6 23) 5 24) 3 25) 2 26) 1 27) 1 28) 2 29) 3 30) 1 ".
 Время начала: 10:20:33.
 Время завершения: 10:22:18.
-Продолжительность: 00:01:44.</t>
+Продолжительность: 00:01:44.
+------------------------------------------------</t>
   </si>
   <si>
     <t>Важенина</t>
   </si>
   <si>
+    <t>1D498E48</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) - 3) + 4) - 5) - 6) - 7) - 8) - 9) - 10) - 11) - 12) - 13) + 14) + 15) + 16) - 17) + 18) - 19) + 20) - 21) - 22) - 23) + 24) - 25) + 26) + 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 7 2) 6 3) 4 4) 2 5) 2 6) 3 7) 2 8) 4 9) 2 10) 2 11) 2 12) 2 13) 2 14) 2 15) 2 16) 2 17) 2 18) 2 19) 2 20) 4 21) 11 22) 6 23) 5 24) 3 25) 2 26) 1 27) 1 28) 2 29) 3 30) 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2 2) 2 3) 3 4) 2 5) 1; 6) 2 7) 2 8) 2 9) 2 10) 3 11) 1 12) 2 13) 3 14) 2 15) 1 16) 2 17) 3 18) 2; 19) 3 20) 3 21) 2 22) 2 23) 2;3; 24) 2;4; 25) 3 26) 2 27) 2; 28) 3 29) 2 30) 4 </t>
+  </si>
+  <si>
+    <t>10:20:33</t>
+  </si>
+  <si>
+    <t>10:22:18</t>
+  </si>
+  <si>
+    <t>00:01:44</t>
   </si>
   <si>
     <t>19.01.2022 14:00:29 ----------
@@ -1532,7 +2135,8 @@
 Маска штрафов за подсказку: "1) * 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * ".
 Время начала: 13:59:44.
 Время завершения: 14:00:29.
-Продолжительность: 00:00:44.</t>
+Продолжительность: 00:00:44.
+------------------------------------------------</t>
   </si>
   <si>
     <t>19.01.2022 14:00:29 ----------
@@ -1541,8 +2145,6 @@
 Имя пользователя компьютера: "brailovskiy_vv"
 Имя пользователя (тестируемого): "Фамилия Имя Тестируем 19.01.2022"
 Название теста: ""
-Файл с тестом: "\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf"
-CRC Файла с тестом: "A3C16E8A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
 Из них правильно: 9 (30,0% выполненых заданий).
@@ -1555,13 +2157,32 @@
 Маска времени обдумывания (в секундах): "1) 7 2) 2 3) 2 4) 1 5) 0 6) 1 7) 0 8) 1 9) 1 10) 1 11) 0 12) 0 13) 0 14) 0 15) 0 16) 1 17) 0 18) 0 19) 0 20) 1 21) 0 22) 1 23) 0 24) 2 25) 2 26) 1 27) 1 28) 0 29) 0 30) 1 ".
 Время начала: 13:59:44.
 Время завершения: 14:00:29.
-Продолжительность: 00:00:44.</t>
+Продолжительность: 00:00:44.
+------------------------------------------------</t>
   </si>
   <si>
     <t>Фамилия Имя Тестируем 19.01.2022</t>
   </si>
   <si>
+    <t>A3C16E8A</t>
+  </si>
+  <si>
+    <t>Незачет</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) - 3) - 4) + 5) - 6) + 7) + 8) - 9) - 10) - 11) - 12) + 13) + 14) - 15) - 16) + 17) + 18) - 19) - 20) - 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 7 2) 2 3) 2 4) 1 5) 0 6) 1 7) 0 8) 1 9) 1 10) 1 11) 0 12) 0 13) 0 14) 0 15) 0 16) 1 17) 0 18) 0 19) 0 20) 1 21) 0 22) 1 23) 0 24) 2 25) 2 26) 1 27) 1 28) 0 29) 0 30) 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) 2; 2) 1 3) 2;3; 4) 1 5) 2; 6) 3 7) 1 8) 2;3; 9) 1 10) 2;3; 11) 3 12) 2 13) 1 14) 2 15) 3 16) 2 17) 1 18) 1; 19) 1 20) 2; 21) 2 22) 2 23) 2 24) 3; 25) 2;3; 26) 3 27) 2;3; 28) 1 29) 2 30) 3 </t>
+  </si>
+  <si>
+    <t>13:59:44</t>
+  </si>
+  <si>
+    <t>14:00:29</t>
   </si>
 </sst>
 </file>
@@ -1919,7 +2540,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA18"/>
+  <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2013,82 +2634,82 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>136</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>156</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>175</v>
       </c>
       <c r="N2" t="s">
-        <v>84</v>
+        <v>190</v>
       </c>
       <c r="O2" t="s">
-        <v>87</v>
+        <v>202</v>
       </c>
       <c r="P2" t="s">
-        <v>92</v>
+        <v>216</v>
       </c>
       <c r="Q2" t="s">
-        <v>97</v>
+        <v>230</v>
       </c>
       <c r="R2" t="s">
-        <v>101</v>
+        <v>242</v>
       </c>
       <c r="S2" t="s">
-        <v>105</v>
+        <v>255</v>
       </c>
       <c r="T2" t="s">
-        <v>108</v>
+        <v>263</v>
       </c>
       <c r="U2" t="s">
-        <v>113</v>
+        <v>277</v>
       </c>
       <c r="V2" t="s">
-        <v>117</v>
+        <v>285</v>
       </c>
       <c r="W2" t="s">
-        <v>120</v>
+        <v>293</v>
       </c>
       <c r="X2" t="s">
-        <v>124</v>
+        <v>306</v>
       </c>
       <c r="Y2" t="s">
-        <v>127</v>
+        <v>317</v>
       </c>
       <c r="Z2" t="s">
-        <v>130</v>
+        <v>325</v>
       </c>
       <c r="AA2" t="s">
-        <v>134</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -2096,82 +2717,82 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>157</v>
       </c>
       <c r="L3" t="s">
-        <v>78</v>
+        <v>164</v>
       </c>
       <c r="M3" t="s">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>191</v>
       </c>
       <c r="O3" t="s">
-        <v>88</v>
+        <v>203</v>
       </c>
       <c r="P3" t="s">
-        <v>93</v>
+        <v>217</v>
       </c>
       <c r="Q3" t="s">
-        <v>98</v>
+        <v>231</v>
       </c>
       <c r="R3" t="s">
-        <v>102</v>
+        <v>243</v>
       </c>
       <c r="S3" t="s">
-        <v>106</v>
+        <v>256</v>
       </c>
       <c r="T3" t="s">
-        <v>109</v>
+        <v>264</v>
       </c>
       <c r="U3" t="s">
-        <v>114</v>
+        <v>278</v>
       </c>
       <c r="V3" t="s">
-        <v>118</v>
+        <v>286</v>
       </c>
       <c r="W3" t="s">
-        <v>121</v>
+        <v>294</v>
       </c>
       <c r="X3" t="s">
-        <v>125</v>
+        <v>307</v>
       </c>
       <c r="Y3" t="s">
-        <v>128</v>
+        <v>318</v>
       </c>
       <c r="Z3" t="s">
-        <v>131</v>
+        <v>326</v>
       </c>
       <c r="AA3" t="s">
-        <v>135</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -2182,16 +2803,16 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -2203,13 +2824,13 @@
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>147</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="M4" t="s">
         <v>29</v>
@@ -2218,43 +2839,43 @@
         <v>29</v>
       </c>
       <c r="O4" t="s">
-        <v>89</v>
+        <v>204</v>
       </c>
       <c r="P4" t="s">
-        <v>94</v>
+        <v>218</v>
       </c>
       <c r="Q4" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="R4" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="S4" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="T4" t="s">
-        <v>110</v>
+        <v>265</v>
       </c>
       <c r="U4" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="V4" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="W4" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="X4" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="Y4" t="s">
-        <v>94</v>
+        <v>218</v>
       </c>
       <c r="Z4" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="AA4" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -2265,16 +2886,16 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -2286,13 +2907,13 @@
         <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="K5" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="M5" t="s">
         <v>30</v>
@@ -2301,43 +2922,43 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="P5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="Q5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="R5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="S5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="T5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="U5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="V5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="W5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="X5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="Y5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="Z5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="AA5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -2345,165 +2966,1498 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" t="s">
+        <v>138</v>
+      </c>
+      <c r="J6" t="s">
+        <v>149</v>
+      </c>
+      <c r="K6" t="s">
+        <v>158</v>
+      </c>
+      <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" t="s">
+        <v>177</v>
+      </c>
+      <c r="N6" t="s">
+        <v>177</v>
+      </c>
+      <c r="O6" t="s">
+        <v>205</v>
+      </c>
+      <c r="P6" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>232</v>
+      </c>
+      <c r="R6" t="s">
+        <v>244</v>
+      </c>
+      <c r="S6" t="s">
+        <v>257</v>
+      </c>
+      <c r="T6" t="s">
+        <v>266</v>
+      </c>
+      <c r="U6" t="s">
+        <v>279</v>
+      </c>
+      <c r="V6" t="s">
+        <v>205</v>
+      </c>
+      <c r="W6" t="s">
+        <v>295</v>
+      </c>
+      <c r="X6" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>327</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J8" t="s">
+        <v>124</v>
+      </c>
+      <c r="K8" t="s">
+        <v>124</v>
+      </c>
+      <c r="L8" t="s">
+        <v>107</v>
+      </c>
+      <c r="M8" t="s">
+        <v>178</v>
+      </c>
+      <c r="N8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O8" t="s">
+        <v>124</v>
+      </c>
+      <c r="P8" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>178</v>
+      </c>
+      <c r="R8" t="s">
+        <v>178</v>
+      </c>
+      <c r="S8" t="s">
+        <v>178</v>
+      </c>
+      <c r="T8" t="s">
+        <v>124</v>
+      </c>
+      <c r="U8" t="s">
+        <v>124</v>
+      </c>
+      <c r="V8" t="s">
+        <v>124</v>
+      </c>
+      <c r="W8" t="s">
+        <v>124</v>
+      </c>
+      <c r="X8" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K9" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" t="s">
+        <v>179</v>
+      </c>
+      <c r="N9" t="s">
+        <v>193</v>
+      </c>
+      <c r="O9" t="s">
+        <v>125</v>
+      </c>
+      <c r="P9" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>179</v>
+      </c>
+      <c r="R9" t="s">
+        <v>179</v>
+      </c>
+      <c r="S9" t="s">
+        <v>179</v>
+      </c>
+      <c r="T9" t="s">
+        <v>125</v>
+      </c>
+      <c r="U9" t="s">
+        <v>125</v>
+      </c>
+      <c r="V9" t="s">
+        <v>125</v>
+      </c>
+      <c r="W9" t="s">
+        <v>125</v>
+      </c>
+      <c r="X9" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>328</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" t="s">
+        <v>109</v>
+      </c>
+      <c r="M10" t="s">
+        <v>109</v>
+      </c>
+      <c r="N10" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" t="s">
+        <v>109</v>
+      </c>
+      <c r="P10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>109</v>
+      </c>
+      <c r="R10" t="s">
+        <v>109</v>
+      </c>
+      <c r="S10" t="s">
+        <v>109</v>
+      </c>
+      <c r="T10" t="s">
+        <v>109</v>
+      </c>
+      <c r="U10" t="s">
+        <v>109</v>
+      </c>
+      <c r="V10" t="s">
+        <v>109</v>
+      </c>
+      <c r="W10" t="s">
+        <v>109</v>
+      </c>
+      <c r="X10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" t="s">
+        <v>109</v>
+      </c>
+      <c r="M11" t="s">
+        <v>109</v>
+      </c>
+      <c r="N11" t="s">
+        <v>109</v>
+      </c>
+      <c r="O11" t="s">
+        <v>109</v>
+      </c>
+      <c r="P11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>109</v>
+      </c>
+      <c r="R11" t="s">
+        <v>109</v>
+      </c>
+      <c r="S11" t="s">
+        <v>109</v>
+      </c>
+      <c r="T11" t="s">
+        <v>109</v>
+      </c>
+      <c r="U11" t="s">
+        <v>109</v>
+      </c>
+      <c r="V11" t="s">
+        <v>109</v>
+      </c>
+      <c r="W11" t="s">
+        <v>109</v>
+      </c>
+      <c r="X11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" t="s">
+        <v>165</v>
+      </c>
+      <c r="M12" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" t="s">
+        <v>194</v>
+      </c>
+      <c r="O12" t="s">
+        <v>206</v>
+      </c>
+      <c r="P12" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>127</v>
+      </c>
+      <c r="R12" t="s">
+        <v>245</v>
+      </c>
+      <c r="S12" t="s">
+        <v>245</v>
+      </c>
+      <c r="T12" t="s">
+        <v>267</v>
+      </c>
+      <c r="U12" t="s">
+        <v>245</v>
+      </c>
+      <c r="V12" t="s">
+        <v>206</v>
+      </c>
+      <c r="W12" t="s">
+        <v>296</v>
+      </c>
+      <c r="X12" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>206</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" t="s">
+        <v>166</v>
+      </c>
+      <c r="M13" t="s">
+        <v>181</v>
+      </c>
+      <c r="N13" t="s">
+        <v>194</v>
+      </c>
+      <c r="O13" t="s">
+        <v>207</v>
+      </c>
+      <c r="P13" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>126</v>
+      </c>
+      <c r="R13" t="s">
+        <v>246</v>
+      </c>
+      <c r="S13" t="s">
+        <v>246</v>
+      </c>
+      <c r="T13" t="s">
+        <v>268</v>
+      </c>
+      <c r="U13" t="s">
+        <v>246</v>
+      </c>
+      <c r="V13" t="s">
+        <v>207</v>
+      </c>
+      <c r="W13" t="s">
+        <v>297</v>
+      </c>
+      <c r="X13" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" t="s">
+        <v>128</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" t="s">
+        <v>167</v>
+      </c>
+      <c r="M14" t="s">
+        <v>182</v>
+      </c>
+      <c r="N14" t="s">
+        <v>85</v>
+      </c>
+      <c r="O14" t="s">
+        <v>208</v>
+      </c>
+      <c r="P14" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>233</v>
+      </c>
+      <c r="R14" t="s">
+        <v>247</v>
+      </c>
+      <c r="S14" t="s">
+        <v>247</v>
+      </c>
+      <c r="T14" t="s">
+        <v>269</v>
+      </c>
+      <c r="U14" t="s">
+        <v>247</v>
+      </c>
+      <c r="V14" t="s">
+        <v>208</v>
+      </c>
+      <c r="W14" t="s">
+        <v>298</v>
+      </c>
+      <c r="X14" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>208</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T15" t="s">
+        <v>39</v>
+      </c>
+      <c r="U15" t="s">
+        <v>39</v>
+      </c>
+      <c r="V15" t="s">
+        <v>39</v>
+      </c>
+      <c r="W15" t="s">
+        <v>39</v>
+      </c>
+      <c r="X15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" t="s">
+        <v>139</v>
+      </c>
+      <c r="J16" t="s">
+        <v>139</v>
+      </c>
+      <c r="K16" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" t="s">
+        <v>168</v>
+      </c>
+      <c r="M16" t="s">
+        <v>183</v>
+      </c>
+      <c r="N16" t="s">
+        <v>195</v>
+      </c>
+      <c r="O16" t="s">
+        <v>209</v>
+      </c>
+      <c r="P16" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>234</v>
+      </c>
+      <c r="R16" t="s">
+        <v>248</v>
+      </c>
+      <c r="S16" t="s">
+        <v>248</v>
+      </c>
+      <c r="T16" t="s">
+        <v>270</v>
+      </c>
+      <c r="U16" t="s">
+        <v>248</v>
+      </c>
+      <c r="V16" t="s">
+        <v>209</v>
+      </c>
+      <c r="W16" t="s">
+        <v>299</v>
+      </c>
+      <c r="X16" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="G6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" t="s">
-        <v>76</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
         <v>35</v>
       </c>
-      <c r="M6" t="s">
-        <v>82</v>
-      </c>
-      <c r="N6" t="s">
-        <v>82</v>
-      </c>
-      <c r="O6" t="s">
-        <v>90</v>
-      </c>
-      <c r="P6" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>99</v>
-      </c>
-      <c r="R6" t="s">
-        <v>103</v>
-      </c>
-      <c r="S6" t="s">
-        <v>107</v>
-      </c>
-      <c r="T6" t="s">
-        <v>111</v>
-      </c>
-      <c r="U6" t="s">
-        <v>115</v>
-      </c>
-      <c r="V6" t="s">
-        <v>90</v>
-      </c>
-      <c r="W6" t="s">
-        <v>122</v>
-      </c>
-      <c r="X6" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y6" t="s">
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
         <v>35</v>
       </c>
-      <c r="Z6" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>136</v>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" t="s">
+        <v>87</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>235</v>
+      </c>
+      <c r="R17" t="s">
+        <v>87</v>
+      </c>
+      <c r="S17" t="s">
+        <v>87</v>
+      </c>
+      <c r="T17" t="s">
+        <v>87</v>
+      </c>
+      <c r="U17" t="s">
+        <v>87</v>
+      </c>
+      <c r="V17" t="s">
+        <v>35</v>
+      </c>
+      <c r="W17" t="s">
+        <v>35</v>
+      </c>
+      <c r="X17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:27">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" t="s">
+        <v>130</v>
+      </c>
+      <c r="I18" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" t="s">
+        <v>150</v>
+      </c>
+      <c r="K18" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" t="s">
+        <v>169</v>
+      </c>
+      <c r="M18" t="s">
+        <v>184</v>
+      </c>
+      <c r="N18" t="s">
+        <v>196</v>
+      </c>
+      <c r="O18" t="s">
+        <v>210</v>
+      </c>
+      <c r="P18" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>236</v>
+      </c>
+      <c r="R18" t="s">
+        <v>249</v>
+      </c>
+      <c r="S18" t="s">
+        <v>249</v>
+      </c>
+      <c r="T18" t="s">
+        <v>271</v>
+      </c>
+      <c r="U18" t="s">
+        <v>280</v>
+      </c>
+      <c r="V18" t="s">
+        <v>287</v>
+      </c>
+      <c r="W18" t="s">
+        <v>300</v>
+      </c>
+      <c r="X18" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>319</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>329</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" t="s">
+        <v>151</v>
+      </c>
+      <c r="K19" t="s">
+        <v>159</v>
+      </c>
+      <c r="L19" t="s">
+        <v>170</v>
+      </c>
+      <c r="M19" t="s">
+        <v>185</v>
+      </c>
+      <c r="N19" t="s">
+        <v>197</v>
+      </c>
+      <c r="O19" t="s">
+        <v>211</v>
+      </c>
+      <c r="P19" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>237</v>
+      </c>
+      <c r="R19" t="s">
+        <v>250</v>
+      </c>
+      <c r="S19" t="s">
+        <v>258</v>
+      </c>
+      <c r="T19" t="s">
+        <v>272</v>
+      </c>
+      <c r="U19" t="s">
+        <v>281</v>
+      </c>
+      <c r="V19" t="s">
+        <v>288</v>
+      </c>
+      <c r="W19" t="s">
+        <v>301</v>
+      </c>
+      <c r="X19" t="s">
+        <v>312</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>330</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" t="s">
+        <v>132</v>
+      </c>
+      <c r="I20" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20" t="s">
+        <v>152</v>
+      </c>
+      <c r="K20" t="s">
+        <v>141</v>
+      </c>
+      <c r="L20" t="s">
+        <v>171</v>
+      </c>
+      <c r="M20" t="s">
+        <v>186</v>
+      </c>
+      <c r="N20" t="s">
+        <v>198</v>
+      </c>
+      <c r="O20" t="s">
+        <v>212</v>
+      </c>
+      <c r="P20" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>238</v>
+      </c>
+      <c r="R20" t="s">
+        <v>251</v>
+      </c>
+      <c r="S20" t="s">
+        <v>259</v>
+      </c>
+      <c r="T20" t="s">
+        <v>273</v>
+      </c>
+      <c r="U20" t="s">
+        <v>282</v>
+      </c>
+      <c r="V20" t="s">
+        <v>289</v>
+      </c>
+      <c r="W20" t="s">
+        <v>302</v>
+      </c>
+      <c r="X20" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>321</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>331</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" t="s">
+        <v>117</v>
+      </c>
+      <c r="K21" t="s">
+        <v>117</v>
+      </c>
+      <c r="L21" t="s">
+        <v>117</v>
+      </c>
+      <c r="M21" t="s">
+        <v>117</v>
+      </c>
+      <c r="N21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O21" t="s">
+        <v>117</v>
+      </c>
+      <c r="P21" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>117</v>
+      </c>
+      <c r="R21" t="s">
+        <v>117</v>
+      </c>
+      <c r="S21" t="s">
+        <v>117</v>
+      </c>
+      <c r="T21" t="s">
+        <v>117</v>
+      </c>
+      <c r="U21" t="s">
+        <v>117</v>
+      </c>
+      <c r="V21" t="s">
+        <v>117</v>
+      </c>
+      <c r="W21" t="s">
+        <v>117</v>
+      </c>
+      <c r="X21" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" t="s">
+        <v>133</v>
+      </c>
+      <c r="I22" t="s">
+        <v>142</v>
+      </c>
+      <c r="J22" t="s">
+        <v>153</v>
+      </c>
+      <c r="K22" t="s">
+        <v>160</v>
+      </c>
+      <c r="L22" t="s">
+        <v>172</v>
+      </c>
+      <c r="M22" t="s">
+        <v>187</v>
+      </c>
+      <c r="N22" t="s">
+        <v>199</v>
+      </c>
+      <c r="O22" t="s">
+        <v>213</v>
+      </c>
+      <c r="P22" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>239</v>
+      </c>
+      <c r="R22" t="s">
+        <v>252</v>
+      </c>
+      <c r="S22" t="s">
+        <v>260</v>
+      </c>
+      <c r="T22" t="s">
+        <v>274</v>
+      </c>
+      <c r="U22" t="s">
+        <v>154</v>
+      </c>
+      <c r="V22" t="s">
+        <v>290</v>
+      </c>
+      <c r="W22" t="s">
+        <v>303</v>
+      </c>
+      <c r="X22" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>322</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>332</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="H18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" t="s">
-        <v>67</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" t="s">
+        <v>134</v>
+      </c>
+      <c r="I23" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" t="s">
+        <v>154</v>
+      </c>
+      <c r="K23" t="s">
+        <v>161</v>
+      </c>
+      <c r="L23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M23" t="s">
+        <v>188</v>
+      </c>
+      <c r="N23" t="s">
+        <v>200</v>
+      </c>
+      <c r="O23" t="s">
+        <v>214</v>
+      </c>
+      <c r="P23" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>240</v>
+      </c>
+      <c r="R23" t="s">
+        <v>253</v>
+      </c>
+      <c r="S23" t="s">
+        <v>261</v>
+      </c>
+      <c r="T23" t="s">
+        <v>275</v>
+      </c>
+      <c r="U23" t="s">
+        <v>283</v>
+      </c>
+      <c r="V23" t="s">
+        <v>291</v>
+      </c>
+      <c r="W23" t="s">
+        <v>304</v>
+      </c>
+      <c r="X23" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>323</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
         <v>79</v>
       </c>
-      <c r="M18" t="s">
-        <v>83</v>
-      </c>
-      <c r="N18" t="s">
-        <v>86</v>
-      </c>
-      <c r="O18" t="s">
-        <v>91</v>
-      </c>
-      <c r="P18" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>100</v>
-      </c>
-      <c r="R18" t="s">
-        <v>104</v>
-      </c>
-      <c r="S18" t="s">
-        <v>104</v>
-      </c>
-      <c r="T18" t="s">
-        <v>112</v>
-      </c>
-      <c r="U18" t="s">
-        <v>116</v>
-      </c>
-      <c r="V18" t="s">
-        <v>119</v>
-      </c>
-      <c r="W18" t="s">
-        <v>123</v>
-      </c>
-      <c r="X18" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>137</v>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H24" t="s">
+        <v>135</v>
+      </c>
+      <c r="I24" t="s">
+        <v>144</v>
+      </c>
+      <c r="J24" t="s">
+        <v>155</v>
+      </c>
+      <c r="K24" t="s">
+        <v>162</v>
+      </c>
+      <c r="L24" t="s">
+        <v>174</v>
+      </c>
+      <c r="M24" t="s">
+        <v>189</v>
+      </c>
+      <c r="N24" t="s">
+        <v>201</v>
+      </c>
+      <c r="O24" t="s">
+        <v>215</v>
+      </c>
+      <c r="P24" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>241</v>
+      </c>
+      <c r="R24" t="s">
+        <v>254</v>
+      </c>
+      <c r="S24" t="s">
+        <v>262</v>
+      </c>
+      <c r="T24" t="s">
+        <v>276</v>
+      </c>
+      <c r="U24" t="s">
+        <v>284</v>
+      </c>
+      <c r="V24" t="s">
+        <v>292</v>
+      </c>
+      <c r="W24" t="s">
+        <v>305</v>
+      </c>
+      <c r="X24" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>334</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new key-value in variablevaluesmarks.py module dict: test timestamp. because it is necessary to have an info about any test result day. each time operator will get test results info from txt-file, convert & save them in docx-format the folders  year > test_date (dd.mm.yyyy) will be created. in the date folders will be saved word files with names <test timestap + tested person fio>.docx(doc)
</commit_message>
<xml_diff>
--- a/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
+++ b/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="372">
   <si>
     <t>22.09.2021 13:28:19{-}А кто кто кто</t>
   </si>
@@ -97,7 +97,7 @@
     <t>19.01.2022 14:00:29{-}Фамилия Имя Тестируем 19.01.2022</t>
   </si>
   <si>
-    <t>22.09.2021 13:28:19 ----------
+    <t>---------- 22.09.2021 13:28:19 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -123,7 +123,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>22.09.2021 13:28:19 ----------
+    <t>---------- 22.09.2021 13:28:19 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -145,6 +145,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>22.09.2021 13:28:19</t>
+  </si>
+  <si>
     <t>SHA-K323-WKS1</t>
   </si>
   <si>
@@ -202,7 +205,7 @@
     <t>00:00:13</t>
   </si>
   <si>
-    <t>22.09.2021 13:29:13 ----------
+    <t>---------- 22.09.2021 13:29:13 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -228,7 +231,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>22.09.2021 13:29:13 ----------
+    <t>---------- 22.09.2021 13:29:13 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -250,6 +253,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>22.09.2021 13:29:13</t>
+  </si>
+  <si>
     <t>Фамилия Имя</t>
   </si>
   <si>
@@ -283,7 +289,7 @@
     <t>00:00:10</t>
   </si>
   <si>
-    <t>22.09.2021 13:47:58 ----------
+    <t>---------- 22.09.2021 13:47:58 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X04"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -309,7 +315,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>22.09.2021 13:47:58 ----------
+    <t>---------- 22.09.2021 13:47:58 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X04"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -331,6 +337,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>22.09.2021 13:47:58</t>
+  </si>
+  <si>
     <t>SHA-K205-X04</t>
   </si>
   <si>
@@ -355,7 +364,7 @@
     <t>00:00:06</t>
   </si>
   <si>
-    <t>22.09.2021 13:48:39 ----------
+    <t>---------- 22.09.2021 13:48:39 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -381,7 +390,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>22.09.2021 13:48:39 ----------
+    <t>---------- 22.09.2021 13:48:39 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -403,6 +412,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>22.09.2021 13:48:39</t>
+  </si>
+  <si>
     <t>SHA-K205-X02</t>
   </si>
   <si>
@@ -424,7 +436,7 @@
     <t>00:01:26</t>
   </si>
   <si>
-    <t>22.09.2021 13:49:01 ----------
+    <t>---------- 22.09.2021 13:49:01 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -450,7 +462,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>22.09.2021 13:49:01 ----------
+    <t>---------- 22.09.2021 13:49:01 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -472,6 +484,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>22.09.2021 13:49:01</t>
+  </si>
+  <si>
     <t>SHA-K205-X01</t>
   </si>
   <si>
@@ -508,7 +523,7 @@
     <t>00:03:25</t>
   </si>
   <si>
-    <t>22.09.2021 13:50:34 ----------
+    <t>---------- 22.09.2021 13:50:34 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K205-X09"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -534,7 +549,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>22.09.2021 13:50:34 ----------
+    <t>---------- 22.09.2021 13:50:34 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K205-X09"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -556,6 +571,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>22.09.2021 13:50:34</t>
+  </si>
+  <si>
     <t>SHA-K205-X09</t>
   </si>
   <si>
@@ -580,7 +598,7 @@
     <t>00:05:37</t>
   </si>
   <si>
-    <t>28.09.2021 10:43:58 ----------
+    <t>---------- 28.09.2021 10:43:58 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -606,7 +624,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>28.09.2021 10:43:58 ----------
+    <t>---------- 28.09.2021 10:43:58 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -628,6 +646,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>28.09.2021 10:43:58</t>
+  </si>
+  <si>
     <t>оыважыва</t>
   </si>
   <si>
@@ -673,7 +694,7 @@
     <t>00:00:20</t>
   </si>
   <si>
-    <t>28.09.2021 14:57:51 ----------
+    <t>---------- 28.09.2021 14:57:51 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -699,7 +720,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>28.09.2021 14:57:51 ----------
+    <t>---------- 28.09.2021 14:57:51 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -721,6 +742,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>28.09.2021 14:57:51</t>
+  </si>
+  <si>
     <t>sdfjds</t>
   </si>
   <si>
@@ -760,7 +784,7 @@
     <t>00:00:18</t>
   </si>
   <si>
-    <t>28.09.2021 14:59:57 ----------
+    <t>---------- 28.09.2021 14:59:57 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -786,7 +810,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>28.09.2021 14:59:57 ----------
+    <t>---------- 28.09.2021 14:59:57 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -808,6 +832,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>28.09.2021 14:59:57</t>
+  </si>
+  <si>
     <t>kdfjgdfhgfghjf</t>
   </si>
   <si>
@@ -829,7 +856,7 @@
     <t>00:00:44</t>
   </si>
   <si>
-    <t>05.10.2021 09:12:37 ----------
+    <t>---------- 05.10.2021 09:12:37 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "PUCILO-EV"
 Имя пользователя компьютера: "pucilo_ev"
@@ -855,7 +882,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>05.10.2021 09:12:37 ----------
+    <t>---------- 05.10.2021 09:12:37 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "PUCILO-EV"
 Имя пользователя компьютера: "pucilo_ev"
@@ -877,6 +904,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>05.10.2021 09:12:37</t>
+  </si>
+  <si>
     <t>PUCILO-EV</t>
   </si>
   <si>
@@ -904,7 +934,7 @@
     <t>00:00:28</t>
   </si>
   <si>
-    <t>05.10.2021 09:13:01 ----------
+    <t>---------- 05.10.2021 09:13:01 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -930,7 +960,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>05.10.2021 09:13:01 ----------
+    <t>---------- 05.10.2021 09:13:01 ----------
 Тест прерван - закрыта программа...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -952,6 +982,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>05.10.2021 09:13:01</t>
+  </si>
+  <si>
     <t>sdfklsdfsdgsd</t>
   </si>
   <si>
@@ -967,7 +1000,7 @@
     <t>00:00:48</t>
   </si>
   <si>
-    <t>06.10.2021 15:01:45 ----------
+    <t>---------- 06.10.2021 15:01:45 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -993,7 +1026,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>06.10.2021 15:01:45 ----------
+    <t>---------- 06.10.2021 15:01:45 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1015,6 +1048,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>06.10.2021 15:01:45</t>
+  </si>
+  <si>
     <t>8 (26,7% выполненых заданий).</t>
   </si>
   <si>
@@ -1045,7 +1081,7 @@
     <t>00:03:45</t>
   </si>
   <si>
-    <t>12.10.2021 17:10:17 ----------
+    <t>---------- 12.10.2021 17:10:17 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -1071,7 +1107,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>12.10.2021 17:10:17 ----------
+    <t>---------- 12.10.2021 17:10:17 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -1093,6 +1129,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>12.10.2021 17:10:17</t>
+  </si>
+  <si>
     <t>lkjg;ldfjgiljg</t>
   </si>
   <si>
@@ -1132,7 +1171,7 @@
     <t>00:00:14</t>
   </si>
   <si>
-    <t>12.10.2021 17:10:46 ----------
+    <t>---------- 12.10.2021 17:10:46 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -1158,7 +1197,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>12.10.2021 17:10:46 ----------
+    <t>---------- 12.10.2021 17:10:46 ----------
 Тест закончен...
 Имя компьютера: "SHA-K323-WKS1"
 Имя пользователя компьютера: "tabakaev_mv"
@@ -1180,6 +1219,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>12.10.2021 17:10:46</t>
+  </si>
+  <si>
     <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников продовольственной торговли.mtf</t>
   </si>
   <si>
@@ -1210,7 +1252,7 @@
     <t>00:00:12</t>
   </si>
   <si>
-    <t>13.10.2021 09:21:40 ----------
+    <t>---------- 13.10.2021 09:21:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X06"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1236,7 +1278,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>13.10.2021 09:21:40 ----------
+    <t>---------- 13.10.2021 09:21:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X06"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1258,6 +1300,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>13.10.2021 09:21:40</t>
+  </si>
+  <si>
     <t>SHA-K205-X06</t>
   </si>
   <si>
@@ -1294,7 +1339,7 @@
     <t>00:11:10</t>
   </si>
   <si>
-    <t>13.10.2021 09:28:48 ----------
+    <t>---------- 13.10.2021 09:28:48 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X08"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1320,7 +1365,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>13.10.2021 09:28:48 ----------
+    <t>---------- 13.10.2021 09:28:48 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X08"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1342,6 +1387,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>13.10.2021 09:28:48</t>
+  </si>
+  <si>
     <t>SHA-K205-X08</t>
   </si>
   <si>
@@ -1378,7 +1426,7 @@
     <t>00:17:50</t>
   </si>
   <si>
-    <t>13.10.2021 09:34:31 ----------
+    <t>---------- 13.10.2021 09:34:31 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X09"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1404,7 +1452,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>13.10.2021 09:34:31 ----------
+    <t>---------- 13.10.2021 09:34:31 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X09"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1426,6 +1474,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>13.10.2021 09:34:31</t>
+  </si>
+  <si>
     <t>Туманова Ирина Леонидовна</t>
   </si>
   <si>
@@ -1456,7 +1507,7 @@
     <t>00:21:55</t>
   </si>
   <si>
-    <t>13.10.2021 09:39:34 ----------
+    <t>---------- 13.10.2021 09:39:34 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1482,7 +1533,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>13.10.2021 09:39:34 ----------
+    <t>---------- 13.10.2021 09:39:34 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1504,6 +1555,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>13.10.2021 09:39:34</t>
+  </si>
+  <si>
     <t>Романцов Дмитрий Ильич</t>
   </si>
   <si>
@@ -1537,7 +1591,7 @@
     <t>00:24:39</t>
   </si>
   <si>
-    <t>13.10.2021 09:39:40 ----------
+    <t>---------- 13.10.2021 09:39:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1563,7 +1617,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>13.10.2021 09:39:40 ----------
+    <t>---------- 13.10.2021 09:39:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1585,6 +1639,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>13.10.2021 09:39:40</t>
+  </si>
+  <si>
     <t>Андреева Снежана Генадьевна</t>
   </si>
   <si>
@@ -1603,7 +1660,7 @@
     <t>00:24:43</t>
   </si>
   <si>
-    <t>13.10.2021 09:44:54 ----------
+    <t>---------- 13.10.2021 09:44:54 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X07"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1629,7 +1686,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>13.10.2021 09:44:54 ----------
+    <t>---------- 13.10.2021 09:44:54 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X07"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1651,6 +1708,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>13.10.2021 09:44:54</t>
+  </si>
+  <si>
     <t>SHA-K205-X07</t>
   </si>
   <si>
@@ -1687,7 +1747,7 @@
     <t>00:33:20</t>
   </si>
   <si>
-    <t>13.10.2021 09:51:08 ----------
+    <t>---------- 13.10.2021 09:51:08 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X04"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1713,7 +1773,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>13.10.2021 09:51:08 ----------
+    <t>---------- 13.10.2021 09:51:08 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X04"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1735,6 +1795,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>13.10.2021 09:51:08</t>
+  </si>
+  <si>
     <t>Петрова Марина Алексеевна</t>
   </si>
   <si>
@@ -1753,7 +1816,7 @@
     <t>00:37:59</t>
   </si>
   <si>
-    <t>20.10.2021 09:09:04 ----------
+    <t>---------- 20.10.2021 09:09:04 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1779,7 +1842,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>20.10.2021 09:09:04 ----------
+    <t>---------- 20.10.2021 09:09:04 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1801,6 +1864,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>20.10.2021 09:09:04</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) - 3) - 4) - 5) - 6) + 7) + 8) - 9) + 10) - 11) + 12) - 13) - 14) + 15) + 16) + 17) + 18) - 19) - 20) - 21) + 22) - 23) - 24) - 25) - 26) - 27) - 28) - 29) - 30) - </t>
   </si>
   <si>
@@ -1819,7 +1885,7 @@
     <t>00:11:43</t>
   </si>
   <si>
-    <t>20.10.2021 09:17:40 ----------
+    <t>---------- 20.10.2021 09:17:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1845,7 +1911,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>20.10.2021 09:17:40 ----------
+    <t>---------- 20.10.2021 09:17:40 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X02"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1867,6 +1933,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>20.10.2021 09:17:40</t>
+  </si>
+  <si>
     <t>кекина людмила федоровна</t>
   </si>
   <si>
@@ -1900,7 +1969,7 @@
     <t>00:19:53</t>
   </si>
   <si>
-    <t>20.10.2021 09:48:00 ----------
+    <t>---------- 20.10.2021 09:48:00 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X09"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1926,7 +1995,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>20.10.2021 09:48:00 ----------
+    <t>---------- 20.10.2021 09:48:00 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X09"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -1948,6 +2017,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>20.10.2021 09:48:00</t>
+  </si>
+  <si>
     <t>2C7EB1D6</t>
   </si>
   <si>
@@ -1975,7 +2047,7 @@
     <t>00:43:13</t>
   </si>
   <si>
-    <t>10.01.2022 17:28:01 ----------
+    <t>---------- 10.01.2022 17:28:01 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X08"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -2001,7 +2073,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>10.01.2022 17:28:01 ----------
+    <t>---------- 10.01.2022 17:28:01 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X08"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -2023,6 +2095,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>10.01.2022 17:28:01</t>
+  </si>
+  <si>
     <t xml:space="preserve">1) - 2) + 3) - 4) + 5) - 6) - 7) + 8) - 9) - 10) - 11) - 12) - 13) - 14) - 15) - 16) - 17) + 18) - 19) - 20) - 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) - 30) - </t>
   </si>
   <si>
@@ -2041,7 +2116,7 @@
     <t>00:01:02</t>
   </si>
   <si>
-    <t>19.01.2022 10:22:18 ----------
+    <t>---------- 19.01.2022 10:22:18 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -2067,7 +2142,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>19.01.2022 10:22:18 ----------
+    <t>---------- 19.01.2022 10:22:18 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -2089,6 +2164,9 @@
 ------------------------------------------------</t>
   </si>
   <si>
+    <t>19.01.2022 10:22:18</t>
+  </si>
+  <si>
     <t>Важенина</t>
   </si>
   <si>
@@ -2113,7 +2191,7 @@
     <t>00:01:44</t>
   </si>
   <si>
-    <t>19.01.2022 14:00:29 ----------
+    <t>---------- 19.01.2022 14:00:29 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -2139,7 +2217,7 @@
 ------------------------------------------------</t>
   </si>
   <si>
-    <t>19.01.2022 14:00:29 ----------
+    <t>---------- 19.01.2022 14:00:29 ----------
 Тест закончен...
 Имя компьютера: "SHA-K205-X01"
 Имя пользователя компьютера: "brailovskiy_vv"
@@ -2159,6 +2237,9 @@
 Время завершения: 14:00:29.
 Продолжительность: 00:00:44.
 ------------------------------------------------</t>
+  </si>
+  <si>
+    <t>19.01.2022 14:00:29</t>
   </si>
   <si>
     <t>Фамилия Имя Тестируем 19.01.2022</t>
@@ -2540,7 +2621,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA24"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2634,82 +2715,82 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="J2" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="K2" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="L2" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="M2" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="N2" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="O2" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="P2" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="Q2" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="R2" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="S2" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="T2" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="U2" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="V2" t="s">
-        <v>285</v>
+        <v>306</v>
       </c>
       <c r="W2" t="s">
-        <v>293</v>
+        <v>315</v>
       </c>
       <c r="X2" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="Y2" t="s">
-        <v>317</v>
+        <v>341</v>
       </c>
       <c r="Z2" t="s">
-        <v>325</v>
+        <v>350</v>
       </c>
       <c r="AA2" t="s">
-        <v>335</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -2717,82 +2798,82 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="I3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="J3" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="K3" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="L3" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="M3" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="N3" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="O3" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="P3" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="Q3" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="R3" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="S3" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="T3" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="U3" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="V3" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="W3" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
       <c r="X3" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="Y3" t="s">
-        <v>318</v>
+        <v>342</v>
       </c>
       <c r="Z3" t="s">
-        <v>326</v>
+        <v>351</v>
       </c>
       <c r="AA3" t="s">
-        <v>336</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -2800,82 +2881,82 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="J4" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="L4" t="s">
-        <v>82</v>
+        <v>176</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>189</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
       <c r="O4" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="P4" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="Q4" t="s">
-        <v>96</v>
+        <v>248</v>
       </c>
       <c r="R4" t="s">
-        <v>73</v>
+        <v>261</v>
       </c>
       <c r="S4" t="s">
-        <v>82</v>
+        <v>275</v>
       </c>
       <c r="T4" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="U4" t="s">
-        <v>63</v>
+        <v>299</v>
       </c>
       <c r="V4" t="s">
-        <v>82</v>
+        <v>308</v>
       </c>
       <c r="W4" t="s">
-        <v>73</v>
+        <v>317</v>
       </c>
       <c r="X4" t="s">
-        <v>96</v>
+        <v>331</v>
       </c>
       <c r="Y4" t="s">
-        <v>218</v>
+        <v>343</v>
       </c>
       <c r="Z4" t="s">
-        <v>82</v>
+        <v>352</v>
       </c>
       <c r="AA4" t="s">
-        <v>82</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -2886,16 +2967,16 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
         <v>30</v>
@@ -2907,13 +2988,13 @@
         <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="K5" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="M5" t="s">
         <v>30</v>
@@ -2922,43 +3003,43 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>64</v>
+        <v>219</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="Q5" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="R5" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="S5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="T5" t="s">
-        <v>64</v>
+        <v>285</v>
       </c>
       <c r="U5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="V5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="W5" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="X5" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="Y5" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="Z5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="AA5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -2966,253 +3047,253 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>123</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="K6" t="s">
-        <v>158</v>
+        <v>31</v>
       </c>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="M6" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="N6" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="O6" t="s">
-        <v>205</v>
+        <v>67</v>
       </c>
       <c r="P6" t="s">
-        <v>219</v>
+        <v>67</v>
       </c>
       <c r="Q6" t="s">
-        <v>232</v>
+        <v>67</v>
       </c>
       <c r="R6" t="s">
-        <v>244</v>
+        <v>67</v>
       </c>
       <c r="S6" t="s">
-        <v>257</v>
+        <v>67</v>
       </c>
       <c r="T6" t="s">
-        <v>266</v>
+        <v>67</v>
       </c>
       <c r="U6" t="s">
-        <v>279</v>
+        <v>67</v>
       </c>
       <c r="V6" t="s">
-        <v>205</v>
+        <v>67</v>
       </c>
       <c r="W6" t="s">
-        <v>295</v>
+        <v>67</v>
       </c>
       <c r="X6" t="s">
-        <v>244</v>
+        <v>67</v>
       </c>
       <c r="Y6" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="Z6" t="s">
-        <v>327</v>
+        <v>67</v>
       </c>
       <c r="AA6" t="s">
-        <v>337</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:27">
       <c r="A7" t="s">
         <v>32</v>
       </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" t="s">
+        <v>147</v>
+      </c>
+      <c r="J7" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" t="s">
+        <v>169</v>
+      </c>
+      <c r="L7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" t="s">
+        <v>190</v>
+      </c>
+      <c r="N7" t="s">
+        <v>190</v>
+      </c>
+      <c r="O7" t="s">
+        <v>220</v>
+      </c>
+      <c r="P7" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>249</v>
+      </c>
+      <c r="R7" t="s">
+        <v>262</v>
+      </c>
+      <c r="S7" t="s">
+        <v>276</v>
+      </c>
+      <c r="T7" t="s">
+        <v>286</v>
+      </c>
+      <c r="U7" t="s">
+        <v>300</v>
+      </c>
+      <c r="V7" t="s">
+        <v>220</v>
+      </c>
+      <c r="W7" t="s">
+        <v>318</v>
+      </c>
+      <c r="X7" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>353</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J8" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" t="s">
-        <v>124</v>
-      </c>
-      <c r="L8" t="s">
-        <v>107</v>
-      </c>
-      <c r="M8" t="s">
-        <v>178</v>
-      </c>
-      <c r="N8" t="s">
-        <v>192</v>
-      </c>
-      <c r="O8" t="s">
-        <v>124</v>
-      </c>
-      <c r="P8" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>178</v>
-      </c>
-      <c r="R8" t="s">
-        <v>178</v>
-      </c>
-      <c r="S8" t="s">
-        <v>178</v>
-      </c>
-      <c r="T8" t="s">
-        <v>124</v>
-      </c>
-      <c r="U8" t="s">
-        <v>124</v>
-      </c>
-      <c r="V8" t="s">
-        <v>124</v>
-      </c>
-      <c r="W8" t="s">
-        <v>124</v>
-      </c>
-      <c r="X8" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>192</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="9" spans="1:27">
       <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="J9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="K9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="L9" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="M9" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="N9" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="O9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="P9" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="Q9" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="R9" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="S9" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="T9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="U9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="V9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="W9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="X9" t="s">
-        <v>308</v>
+        <v>191</v>
       </c>
       <c r="Y9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="Z9" t="s">
-        <v>328</v>
+        <v>206</v>
       </c>
       <c r="AA9" t="s">
-        <v>338</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -3220,165 +3301,165 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="I10" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="J10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="K10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="L10" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="M10" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="N10" t="s">
-        <v>109</v>
+        <v>207</v>
       </c>
       <c r="O10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="P10" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="Q10" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="R10" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="S10" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="T10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="U10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="V10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="W10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="X10" t="s">
-        <v>109</v>
+        <v>332</v>
       </c>
       <c r="Y10" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="Z10" t="s">
-        <v>109</v>
+        <v>354</v>
       </c>
       <c r="AA10" t="s">
-        <v>109</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="I11" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="K11" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="L11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="N11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="O11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="P11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="Q11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="R11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="S11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="T11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="U11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="V11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="W11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="X11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="Y11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="Z11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="AA11" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -3386,82 +3467,82 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="G12" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="I12" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="J12" t="s">
         <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="L12" t="s">
-        <v>165</v>
+        <v>116</v>
       </c>
       <c r="M12" t="s">
-        <v>180</v>
+        <v>116</v>
       </c>
       <c r="N12" t="s">
-        <v>194</v>
+        <v>116</v>
       </c>
       <c r="O12" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="P12" t="s">
-        <v>220</v>
+        <v>116</v>
       </c>
       <c r="Q12" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="R12" t="s">
-        <v>245</v>
+        <v>116</v>
       </c>
       <c r="S12" t="s">
-        <v>245</v>
+        <v>116</v>
       </c>
       <c r="T12" t="s">
-        <v>267</v>
+        <v>116</v>
       </c>
       <c r="U12" t="s">
-        <v>245</v>
+        <v>116</v>
       </c>
       <c r="V12" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="W12" t="s">
-        <v>296</v>
+        <v>116</v>
       </c>
       <c r="X12" t="s">
-        <v>207</v>
+        <v>116</v>
       </c>
       <c r="Y12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="Z12" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="AA12" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -3469,82 +3550,82 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="H13" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J13" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="K13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L13" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="M13" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="N13" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="O13" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="P13" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>135</v>
+      </c>
+      <c r="R13" t="s">
+        <v>263</v>
+      </c>
+      <c r="S13" t="s">
+        <v>263</v>
+      </c>
+      <c r="T13" t="s">
+        <v>287</v>
+      </c>
+      <c r="U13" t="s">
+        <v>263</v>
+      </c>
+      <c r="V13" t="s">
         <v>221</v>
       </c>
-      <c r="Q13" t="s">
-        <v>126</v>
-      </c>
-      <c r="R13" t="s">
-        <v>246</v>
-      </c>
-      <c r="S13" t="s">
-        <v>246</v>
-      </c>
-      <c r="T13" t="s">
-        <v>268</v>
-      </c>
-      <c r="U13" t="s">
-        <v>246</v>
-      </c>
-      <c r="V13" t="s">
-        <v>207</v>
-      </c>
       <c r="W13" t="s">
-        <v>297</v>
+        <v>319</v>
       </c>
       <c r="X13" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="Y13" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="Z13" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="AA13" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -3552,82 +3633,82 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H14" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="I14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="M14" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="N14" t="s">
-        <v>85</v>
+        <v>208</v>
       </c>
       <c r="O14" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="P14" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>134</v>
+      </c>
+      <c r="R14" t="s">
+        <v>264</v>
+      </c>
+      <c r="S14" t="s">
+        <v>264</v>
+      </c>
+      <c r="T14" t="s">
+        <v>288</v>
+      </c>
+      <c r="U14" t="s">
+        <v>264</v>
+      </c>
+      <c r="V14" t="s">
         <v>222</v>
       </c>
-      <c r="Q14" t="s">
-        <v>233</v>
-      </c>
-      <c r="R14" t="s">
-        <v>247</v>
-      </c>
-      <c r="S14" t="s">
-        <v>247</v>
-      </c>
-      <c r="T14" t="s">
-        <v>269</v>
-      </c>
-      <c r="U14" t="s">
-        <v>247</v>
-      </c>
-      <c r="V14" t="s">
-        <v>208</v>
-      </c>
       <c r="W14" t="s">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="X14" t="s">
-        <v>309</v>
+        <v>221</v>
       </c>
       <c r="Y14" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="Z14" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="AA14" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -3635,25 +3716,25 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
         <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="I15" t="s">
         <v>39</v>
@@ -3665,52 +3746,52 @@
         <v>39</v>
       </c>
       <c r="L15" t="s">
-        <v>39</v>
+        <v>179</v>
       </c>
       <c r="M15" t="s">
-        <v>39</v>
+        <v>195</v>
       </c>
       <c r="N15" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="O15" t="s">
-        <v>39</v>
+        <v>223</v>
       </c>
       <c r="P15" t="s">
-        <v>39</v>
+        <v>238</v>
       </c>
       <c r="Q15" t="s">
-        <v>39</v>
+        <v>250</v>
       </c>
       <c r="R15" t="s">
-        <v>39</v>
+        <v>265</v>
       </c>
       <c r="S15" t="s">
-        <v>39</v>
+        <v>265</v>
       </c>
       <c r="T15" t="s">
-        <v>39</v>
+        <v>289</v>
       </c>
       <c r="U15" t="s">
-        <v>39</v>
+        <v>265</v>
       </c>
       <c r="V15" t="s">
-        <v>39</v>
+        <v>223</v>
       </c>
       <c r="W15" t="s">
-        <v>39</v>
+        <v>321</v>
       </c>
       <c r="X15" t="s">
-        <v>39</v>
+        <v>333</v>
       </c>
       <c r="Y15" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="Z15" t="s">
-        <v>39</v>
+        <v>223</v>
       </c>
       <c r="AA15" t="s">
-        <v>39</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -3718,248 +3799,248 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
         <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
         <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="I16" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="J16" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="L16" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="M16" t="s">
-        <v>183</v>
+        <v>40</v>
       </c>
       <c r="N16" t="s">
-        <v>195</v>
+        <v>40</v>
       </c>
       <c r="O16" t="s">
-        <v>209</v>
+        <v>40</v>
       </c>
       <c r="P16" t="s">
-        <v>223</v>
+        <v>40</v>
       </c>
       <c r="Q16" t="s">
-        <v>234</v>
+        <v>40</v>
       </c>
       <c r="R16" t="s">
-        <v>248</v>
+        <v>40</v>
       </c>
       <c r="S16" t="s">
-        <v>248</v>
+        <v>40</v>
       </c>
       <c r="T16" t="s">
-        <v>270</v>
+        <v>40</v>
       </c>
       <c r="U16" t="s">
-        <v>248</v>
+        <v>40</v>
       </c>
       <c r="V16" t="s">
-        <v>209</v>
+        <v>40</v>
       </c>
       <c r="W16" t="s">
-        <v>299</v>
+        <v>40</v>
       </c>
       <c r="X16" t="s">
-        <v>310</v>
+        <v>40</v>
       </c>
       <c r="Y16" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
       <c r="Z16" t="s">
-        <v>209</v>
+        <v>40</v>
       </c>
       <c r="AA16" t="s">
-        <v>209</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="H17" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="L17" t="s">
-        <v>35</v>
+        <v>180</v>
       </c>
       <c r="M17" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="N17" t="s">
-        <v>87</v>
+        <v>209</v>
       </c>
       <c r="O17" t="s">
-        <v>35</v>
+        <v>224</v>
       </c>
       <c r="P17" t="s">
-        <v>87</v>
+        <v>239</v>
       </c>
       <c r="Q17" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="R17" t="s">
-        <v>87</v>
+        <v>266</v>
       </c>
       <c r="S17" t="s">
-        <v>87</v>
+        <v>266</v>
       </c>
       <c r="T17" t="s">
-        <v>87</v>
+        <v>290</v>
       </c>
       <c r="U17" t="s">
-        <v>87</v>
+        <v>266</v>
       </c>
       <c r="V17" t="s">
-        <v>35</v>
+        <v>224</v>
       </c>
       <c r="W17" t="s">
-        <v>35</v>
+        <v>322</v>
       </c>
       <c r="X17" t="s">
-        <v>35</v>
+        <v>334</v>
       </c>
       <c r="Y17" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="Z17" t="s">
-        <v>35</v>
+        <v>224</v>
       </c>
       <c r="AA17" t="s">
-        <v>339</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:27">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="H18" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="I18" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="J18" t="s">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="K18" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>169</v>
+        <v>36</v>
       </c>
       <c r="M18" t="s">
-        <v>184</v>
+        <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>196</v>
+        <v>92</v>
       </c>
       <c r="O18" t="s">
-        <v>210</v>
+        <v>36</v>
       </c>
       <c r="P18" t="s">
-        <v>224</v>
+        <v>92</v>
       </c>
       <c r="Q18" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="R18" t="s">
-        <v>249</v>
+        <v>92</v>
       </c>
       <c r="S18" t="s">
-        <v>249</v>
+        <v>92</v>
       </c>
       <c r="T18" t="s">
-        <v>271</v>
+        <v>92</v>
       </c>
       <c r="U18" t="s">
-        <v>280</v>
+        <v>92</v>
       </c>
       <c r="V18" t="s">
-        <v>287</v>
+        <v>36</v>
       </c>
       <c r="W18" t="s">
-        <v>300</v>
+        <v>36</v>
       </c>
       <c r="X18" t="s">
-        <v>311</v>
+        <v>36</v>
       </c>
       <c r="Y18" t="s">
-        <v>319</v>
+        <v>36</v>
       </c>
       <c r="Z18" t="s">
-        <v>329</v>
+        <v>36</v>
       </c>
       <c r="AA18" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -3967,82 +4048,82 @@
         <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="H19" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="I19" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="J19" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="K19" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="L19" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="M19" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="N19" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="O19" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="P19" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="Q19" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="R19" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="S19" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="T19" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="U19" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="V19" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="W19" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="X19" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="Y19" t="s">
-        <v>320</v>
+        <v>344</v>
       </c>
       <c r="Z19" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="AA19" t="s">
-        <v>341</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -4050,82 +4131,82 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G20" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H20" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="I20" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="J20" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="K20" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="L20" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="M20" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="N20" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="O20" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="P20" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="Q20" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="R20" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="S20" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="T20" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="U20" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="V20" t="s">
-        <v>289</v>
+        <v>310</v>
       </c>
       <c r="W20" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="X20" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="Y20" t="s">
-        <v>321</v>
+        <v>345</v>
       </c>
       <c r="Z20" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="AA20" t="s">
-        <v>342</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -4133,82 +4214,82 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="I21" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="J21" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="K21" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="L21" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
       <c r="M21" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
       <c r="N21" t="s">
-        <v>117</v>
+        <v>212</v>
       </c>
       <c r="O21" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="P21" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="Q21" t="s">
-        <v>117</v>
+        <v>255</v>
       </c>
       <c r="R21" t="s">
-        <v>117</v>
+        <v>269</v>
       </c>
       <c r="S21" t="s">
-        <v>117</v>
+        <v>278</v>
       </c>
       <c r="T21" t="s">
-        <v>117</v>
+        <v>293</v>
       </c>
       <c r="U21" t="s">
-        <v>117</v>
+        <v>303</v>
       </c>
       <c r="V21" t="s">
-        <v>117</v>
+        <v>311</v>
       </c>
       <c r="W21" t="s">
-        <v>117</v>
+        <v>325</v>
       </c>
       <c r="X21" t="s">
-        <v>117</v>
+        <v>337</v>
       </c>
       <c r="Y21" t="s">
-        <v>117</v>
+        <v>346</v>
       </c>
       <c r="Z21" t="s">
-        <v>117</v>
+        <v>357</v>
       </c>
       <c r="AA21" t="s">
-        <v>117</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -4216,82 +4297,82 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="I22" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="J22" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="K22" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="L22" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="M22" t="s">
-        <v>187</v>
+        <v>124</v>
       </c>
       <c r="N22" t="s">
-        <v>199</v>
+        <v>124</v>
       </c>
       <c r="O22" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
       <c r="P22" t="s">
-        <v>227</v>
+        <v>124</v>
       </c>
       <c r="Q22" t="s">
-        <v>239</v>
+        <v>124</v>
       </c>
       <c r="R22" t="s">
-        <v>252</v>
+        <v>124</v>
       </c>
       <c r="S22" t="s">
-        <v>260</v>
+        <v>124</v>
       </c>
       <c r="T22" t="s">
-        <v>274</v>
+        <v>124</v>
       </c>
       <c r="U22" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="V22" t="s">
-        <v>290</v>
+        <v>124</v>
       </c>
       <c r="W22" t="s">
-        <v>303</v>
+        <v>124</v>
       </c>
       <c r="X22" t="s">
-        <v>314</v>
+        <v>124</v>
       </c>
       <c r="Y22" t="s">
-        <v>322</v>
+        <v>124</v>
       </c>
       <c r="Z22" t="s">
-        <v>332</v>
+        <v>124</v>
       </c>
       <c r="AA22" t="s">
-        <v>343</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -4299,82 +4380,82 @@
         <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F23" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H23" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="I23" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="J23" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="K23" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="L23" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="M23" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="N23" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="O23" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="P23" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="Q23" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="R23" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="S23" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="T23" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="U23" t="s">
-        <v>283</v>
+        <v>164</v>
       </c>
       <c r="V23" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="W23" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="X23" t="s">
-        <v>315</v>
+        <v>338</v>
       </c>
       <c r="Y23" t="s">
-        <v>323</v>
+        <v>347</v>
       </c>
       <c r="Z23" t="s">
-        <v>333</v>
+        <v>358</v>
       </c>
       <c r="AA23" t="s">
-        <v>344</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -4382,82 +4463,165 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G24" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="H24" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="I24" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="J24" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="K24" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="L24" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="M24" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="N24" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="O24" t="s">
+        <v>229</v>
+      </c>
+      <c r="P24" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>257</v>
+      </c>
+      <c r="R24" t="s">
+        <v>271</v>
+      </c>
+      <c r="S24" t="s">
+        <v>280</v>
+      </c>
+      <c r="T24" t="s">
+        <v>295</v>
+      </c>
+      <c r="U24" t="s">
+        <v>304</v>
+      </c>
+      <c r="V24" t="s">
+        <v>313</v>
+      </c>
+      <c r="W24" t="s">
+        <v>327</v>
+      </c>
+      <c r="X24" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>348</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" t="s">
+        <v>127</v>
+      </c>
+      <c r="H25" t="s">
+        <v>143</v>
+      </c>
+      <c r="I25" t="s">
+        <v>153</v>
+      </c>
+      <c r="J25" t="s">
+        <v>165</v>
+      </c>
+      <c r="K25" t="s">
+        <v>173</v>
+      </c>
+      <c r="L25" t="s">
+        <v>186</v>
+      </c>
+      <c r="M25" t="s">
+        <v>202</v>
+      </c>
+      <c r="N25" t="s">
         <v>215</v>
       </c>
-      <c r="P24" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>241</v>
-      </c>
-      <c r="R24" t="s">
-        <v>254</v>
-      </c>
-      <c r="S24" t="s">
-        <v>262</v>
-      </c>
-      <c r="T24" t="s">
-        <v>276</v>
-      </c>
-      <c r="U24" t="s">
-        <v>284</v>
-      </c>
-      <c r="V24" t="s">
-        <v>292</v>
-      </c>
-      <c r="W24" t="s">
+      <c r="O25" t="s">
+        <v>230</v>
+      </c>
+      <c r="P25" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>258</v>
+      </c>
+      <c r="R25" t="s">
+        <v>272</v>
+      </c>
+      <c r="S25" t="s">
+        <v>281</v>
+      </c>
+      <c r="T25" t="s">
+        <v>296</v>
+      </c>
+      <c r="U25" t="s">
         <v>305</v>
       </c>
-      <c r="X24" t="s">
-        <v>316</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>324</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>334</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>144</v>
+      <c r="V25" t="s">
+        <v>314</v>
+      </c>
+      <c r="W25" t="s">
+        <v>328</v>
+      </c>
+      <c r="X25" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>360</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited ClassTesterFile.py. now it creates folders and subfolders with test results in docx-format
</commit_message>
<xml_diff>
--- a/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
+++ b/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
@@ -16,85 +16,85 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="372">
   <si>
-    <t>22.09.2021 13:28:19{-}А кто кто кто</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:29:13{-}Фамилия Имя</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:47:58{-}джлдлоогридл</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:48:39{-}орпрдло</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:49:01{-}Петя</t>
-  </si>
-  <si>
-    <t>22.09.2021 13:50:34{-}Вася</t>
-  </si>
-  <si>
-    <t>28.09.2021 10:43:58{-}оыважыва</t>
-  </si>
-  <si>
-    <t>28.09.2021 14:57:51{-}sdfjds</t>
-  </si>
-  <si>
-    <t>28.09.2021 14:59:57{-}kdfjgdfhgfghjf</t>
-  </si>
-  <si>
-    <t>05.10.2021 09:12:37{-}я</t>
-  </si>
-  <si>
-    <t>05.10.2021 09:13:01{-}sdfklsdfsdgsd</t>
-  </si>
-  <si>
-    <t>06.10.2021 15:01:45{-}Фамилия Имя</t>
-  </si>
-  <si>
-    <t>12.10.2021 17:10:17{-}lkjg;ldfjgiljg</t>
-  </si>
-  <si>
-    <t>12.10.2021 17:10:46{-}lkjg;ldfjgiljg</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:21:40{-}озерова елизавета денисовна</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:28:48{-}Лоскутова</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:34:31{-}Туманова Ирина Леонидовна</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:39:34{-}Романцов Дмитрий Ильич</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:39:40{-}Андреева Снежана Генадьевна</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:44:54{-}Белоусова Наталья</t>
-  </si>
-  <si>
-    <t>13.10.2021 09:51:08{-}Петрова Марина Алексеевна</t>
-  </si>
-  <si>
-    <t>20.10.2021 09:09:04{-}озерова елизавета денисовна</t>
-  </si>
-  <si>
-    <t>20.10.2021 09:17:40{-}кекина людмила федоровна</t>
-  </si>
-  <si>
-    <t>20.10.2021 09:48:00{-}Романцов Дмитрий Ильич</t>
-  </si>
-  <si>
-    <t>10.01.2022 17:28:01{-}Фамилия Имя</t>
-  </si>
-  <si>
-    <t>19.01.2022 10:22:18{-}Важенина</t>
-  </si>
-  <si>
-    <t>19.01.2022 14:00:29{-}Фамилия Имя Тестируем 19.01.2022</t>
+    <t>22.09.2021 13:28:19{-}А КТО КТО КТО</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:29:13{-}ФАМИЛИЯ ИМЯ</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:47:58{-}ДЖЛДЛООГРИДЛ</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:48:39{-}ОРПРДЛО</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:49:01{-}ПЕТЯ</t>
+  </si>
+  <si>
+    <t>22.09.2021 13:50:34{-}ВАСЯ</t>
+  </si>
+  <si>
+    <t>28.09.2021 10:43:58{-}ОЫВАЖЫВА</t>
+  </si>
+  <si>
+    <t>28.09.2021 14:57:51{-}SDFJDS</t>
+  </si>
+  <si>
+    <t>28.09.2021 14:59:57{-}KDFJGDFHGFGHJF</t>
+  </si>
+  <si>
+    <t>05.10.2021 09:12:37{-}Я</t>
+  </si>
+  <si>
+    <t>05.10.2021 09:13:01{-}SDFKLSDFSDGSD</t>
+  </si>
+  <si>
+    <t>06.10.2021 15:01:45{-}ФАМИЛИЯ ИМЯ</t>
+  </si>
+  <si>
+    <t>12.10.2021 17:10:17{-}LKJG;LDFJGILJG</t>
+  </si>
+  <si>
+    <t>12.10.2021 17:10:46{-}LKJG;LDFJGILJG</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:21:40{-}ОЗЕРОВА ЕЛИЗАВЕТА ДЕНИСОВНА</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:28:48{-}ЛОСКУТОВА</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:34:31{-}ТУМАНОВА ИРИНА ЛЕОНИДОВНА</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:39:34{-}РОМАНЦОВ ДМИТРИЙ ИЛЬИЧ</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:39:40{-}АНДРЕЕВА СНЕЖАНА ГЕНАДЬЕВНА</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:44:54{-}БЕЛОУСОВА НАТАЛЬЯ</t>
+  </si>
+  <si>
+    <t>13.10.2021 09:51:08{-}ПЕТРОВА МАРИНА АЛЕКСЕЕВНА</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:09:04{-}ОЗЕРОВА ЕЛИЗАВЕТА ДЕНИСОВНА</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:17:40{-}КЕКИНА ЛЮДМИЛА ФЕДОРОВНА</t>
+  </si>
+  <si>
+    <t>20.10.2021 09:48:00{-}РОМАНЦОВ ДМИТРИЙ ИЛЬИЧ</t>
+  </si>
+  <si>
+    <t>10.01.2022 17:28:01{-}ФАМИЛИЯ ИМЯ</t>
+  </si>
+  <si>
+    <t>19.01.2022 10:22:18{-}ВАЖЕНИНА</t>
+  </si>
+  <si>
+    <t>19.01.2022 14:00:29{-}ФАМИЛИЯ ИМЯ ТЕСТИРУЕМ 19.01.2022</t>
   </si>
   <si>
     <t>---------- 22.09.2021 13:28:19 ----------
@@ -154,7 +154,7 @@
     <t>tabakaev_mv</t>
   </si>
   <si>
-    <t>А кто кто кто</t>
+    <t>А КТО КТО КТО</t>
   </si>
   <si>
     <t>название теста</t>
@@ -256,7 +256,7 @@
     <t>22.09.2021 13:29:13</t>
   </si>
   <si>
-    <t>Фамилия Имя</t>
+    <t>ФАМИЛИЯ ИМЯ</t>
   </si>
   <si>
     <t>2598F9AC</t>
@@ -346,7 +346,7 @@
     <t>brailovskiy_vv</t>
   </si>
   <si>
-    <t>джлдлоогридл</t>
+    <t>ДЖЛДЛООГРИДЛ</t>
   </si>
   <si>
     <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Безымянный.mtf</t>
@@ -418,7 +418,7 @@
     <t>SHA-K205-X02</t>
   </si>
   <si>
-    <t>орпрдло</t>
+    <t>ОРПРДЛО</t>
   </si>
   <si>
     <t xml:space="preserve">1) 85 2) 1 </t>
@@ -490,7 +490,7 @@
     <t>SHA-K205-X01</t>
   </si>
   <si>
-    <t>Петя</t>
+    <t>ПЕТЯ</t>
   </si>
   <si>
     <t>1 (50,0% выполненых заданий).</t>
@@ -577,7 +577,7 @@
     <t>SHA-K205-X09</t>
   </si>
   <si>
-    <t>Вася</t>
+    <t>ВАСЯ</t>
   </si>
   <si>
     <t>1</t>
@@ -649,7 +649,7 @@
     <t>28.09.2021 10:43:58</t>
   </si>
   <si>
-    <t>оыважыва</t>
+    <t>ОЫВАЖЫВА</t>
   </si>
   <si>
     <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 2 вариант.mtf</t>
@@ -745,7 +745,7 @@
     <t>28.09.2021 14:57:51</t>
   </si>
   <si>
-    <t>sdfjds</t>
+    <t>SDFJDS</t>
   </si>
   <si>
     <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников ДОО 1 вариант.mtf</t>
@@ -835,7 +835,7 @@
     <t>28.09.2021 14:59:57</t>
   </si>
   <si>
-    <t>kdfjgdfhgfghjf</t>
+    <t>KDFJGDFHGFGHJF</t>
   </si>
   <si>
     <t>0,0 из 30 возможных. Ваш результат: 0,0%</t>
@@ -913,7 +913,7 @@
     <t>pucilo_ev</t>
   </si>
   <si>
-    <t>я</t>
+    <t>Я</t>
   </si>
   <si>
     <t xml:space="preserve">1) - 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
@@ -985,7 +985,7 @@
     <t>05.10.2021 09:13:01</t>
   </si>
   <si>
-    <t>sdfklsdfsdgsd</t>
+    <t>SDFKLSDFSDGSD</t>
   </si>
   <si>
     <t xml:space="preserve">1) 48 2) * 3) * 4) * 5) * 6) * 7) * 8) * 9) * 10) * 11) * 12) * 13) * 14) * 15) * 16) * 17) * 18) * 19) * 20) * 21) * 22) * 23) * 24) * 25) * 26) * 27) * 28) * 29) * 30) * </t>
@@ -1132,7 +1132,7 @@
     <t>12.10.2021 17:10:17</t>
   </si>
   <si>
-    <t>lkjg;ldfjgiljg</t>
+    <t>LKJG;LDFJGILJG</t>
   </si>
   <si>
     <t>\\192.168.201.38\общая папка\06 ООДЦ\ТЕСТЫ\MyTest\Для работников общепита.mtf</t>
@@ -1306,7 +1306,7 @@
     <t>SHA-K205-X06</t>
   </si>
   <si>
-    <t>озерова елизавета денисовна</t>
+    <t>ОЗЕРОВА ЕЛИЗАВЕТА ДЕНИСОВНА</t>
   </si>
   <si>
     <t>9 (30,0% выполненых заданий).</t>
@@ -1393,7 +1393,7 @@
     <t>SHA-K205-X08</t>
   </si>
   <si>
-    <t>Лоскутова</t>
+    <t>ЛОСКУТОВА</t>
   </si>
   <si>
     <t>17 (56,7% выполненых заданий).</t>
@@ -1477,7 +1477,7 @@
     <t>13.10.2021 09:34:31</t>
   </si>
   <si>
-    <t>Туманова Ирина Леонидовна</t>
+    <t>ТУМАНОВА ИРИНА ЛЕОНИДОВНА</t>
   </si>
   <si>
     <t>76,7%</t>
@@ -1558,7 +1558,7 @@
     <t>13.10.2021 09:39:34</t>
   </si>
   <si>
-    <t>Романцов Дмитрий Ильич</t>
+    <t>РОМАНЦОВ ДМИТРИЙ ИЛЬИЧ</t>
   </si>
   <si>
     <t>20 (66,7% выполненых заданий).</t>
@@ -1642,7 +1642,7 @@
     <t>13.10.2021 09:39:40</t>
   </si>
   <si>
-    <t>Андреева Снежана Генадьевна</t>
+    <t>АНДРЕЕВА СНЕЖАНА ГЕНАДЬЕВНА</t>
   </si>
   <si>
     <t xml:space="preserve">1) 72 2) 33 3) 30 4) 22 5) 54 6) 27 7) 17 8) 19 9) 41 10) 24 11) 21 12) 134 13) 16 14) 85 15) 26 16) 23 17) 28 18) 17 19) 37 20) 30 21) 39 22) 49 23) 70 24) 196 25) 23 26) 42 27) 52 28) 93 29) 75 30) 72 </t>
@@ -1714,7 +1714,7 @@
     <t>SHA-K205-X07</t>
   </si>
   <si>
-    <t>Белоусова Наталья</t>
+    <t>БЕЛОУСОВА НАТАЛЬЯ</t>
   </si>
   <si>
     <t>18 (60,0% выполненых заданий).</t>
@@ -1798,7 +1798,7 @@
     <t>13.10.2021 09:51:08</t>
   </si>
   <si>
-    <t>Петрова Марина Алексеевна</t>
+    <t>ПЕТРОВА МАРИНА АЛЕКСЕЕВНА</t>
   </si>
   <si>
     <t xml:space="preserve">1) + 2) + 3) - 4) + 5) + 6) + 7) + 8) - 9) + 10) + 11) + 12) + 13) + 14) + 15) + 16) + 17) + 18) - 19) - 20) + 21) - 22) + 23) + 24) - 25) - 26) - 27) - 28) + 29) + 30) - </t>
@@ -1936,7 +1936,7 @@
     <t>20.10.2021 09:17:40</t>
   </si>
   <si>
-    <t>кекина людмила федоровна</t>
+    <t>КЕКИНА ЛЮДМИЛА ФЕДОРОВНА</t>
   </si>
   <si>
     <t>14 (46,7% выполненых заданий).</t>
@@ -2167,7 +2167,7 @@
     <t>19.01.2022 10:22:18</t>
   </si>
   <si>
-    <t>Важенина</t>
+    <t>ВАЖЕНИНА</t>
   </si>
   <si>
     <t>1D498E48</t>
@@ -2242,7 +2242,7 @@
     <t>19.01.2022 14:00:29</t>
   </si>
   <si>
-    <t>Фамилия Имя Тестируем 19.01.2022</t>
+    <t>ФАМИЛИЯ ИМЯ ТЕСТИРУЕМ 19.01.2022</t>
   </si>
   <si>
     <t>A3C16E8A</t>

</xml_diff>

<commit_message>
some fixes primarly in classtesterfile.py module. now txt-file to parse should be placed in the current working direktory of the project!!!
</commit_message>
<xml_diff>
--- a/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
+++ b/Parse Test Results into Word files/test_output_MyTestProgramSliced.xlsx
@@ -107,8 +107,8 @@
 CRC Файла с тестом: "57C3A660"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 2 (100,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 2 (100,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
@@ -131,8 +131,8 @@
 Название теста: "название теста"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 2 (100,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 2 (100,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
@@ -169,10 +169,10 @@
     <t>2</t>
   </si>
   <si>
-    <t>0 (0,0% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>2 (100,0% выполненых заданий).</t>
+    <t>0 (0,0% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>2 (100,0% выполненных заданий).</t>
   </si>
   <si>
     <t>0,0%</t>
@@ -215,8 +215,8 @@
 CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 2 (100,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 2 (100,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 100,0%.
 Использовано подсказок: 0.
 Набрано баллов: 2,0 из 2 возможных. Ваш результат: 100,0%.
@@ -239,8 +239,8 @@
 Название теста: ""
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 2 (100,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 2 (100,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 100,0%.
 Использовано подсказок: 0.
 Набрано баллов: 2,0 из 2 возможных. Ваш результат: 100,0%.
@@ -299,8 +299,8 @@
 CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 2 (100,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 2 (100,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 100,0%.
 Использовано подсказок: 0.
 Набрано баллов: 2,0 из 2 возможных. Ваш результат: 100,0%.
@@ -323,8 +323,8 @@
 Название теста: ""
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 2 (100,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 2 (100,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 100,0%.
 Использовано подсказок: 0.
 Набрано баллов: 2,0 из 2 возможных. Ваш результат: 100,0%.
@@ -374,8 +374,8 @@
 CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 2 (100,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 2 (100,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
@@ -398,8 +398,8 @@
 Название теста: ""
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 2 (100,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 2 (100,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
@@ -446,8 +446,8 @@
 CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 1 (50,0% выполненых заданий).
-Из них ошибок: 1 (50,0% выполненых заданий).
+Из них правильно: 1 (50,0% выполненных заданий).
+Из них ошибок: 1 (50,0% выполненных заданий).
 Результативность: 50,0%.
 Использовано подсказок: 0.
 Набрано баллов: 1,0 из 2 возможных. Ваш результат: 50,0%.
@@ -470,8 +470,8 @@
 Название теста: ""
 Всего заданий в тесте: 2.
 Выполнено заданий: 2.
-Из них правильно: 1 (50,0% выполненых заданий).
-Из них ошибок: 1 (50,0% выполненых заданий).
+Из них правильно: 1 (50,0% выполненных заданий).
+Из них ошибок: 1 (50,0% выполненных заданий).
 Результативность: 50,0%.
 Использовано подсказок: 0.
 Набрано баллов: 1,0 из 2 возможных. Ваш результат: 50,0%.
@@ -493,7 +493,7 @@
     <t>ПЕТЯ</t>
   </si>
   <si>
-    <t>1 (50,0% выполненых заданий).</t>
+    <t>1 (50,0% выполненных заданий).</t>
   </si>
   <si>
     <t>50,0%</t>
@@ -533,8 +533,8 @@
 CRC Файла с тестом: "2598F9AC"
 Всего заданий в тесте: 2.
 Выполнено заданий: 1.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
@@ -557,8 +557,8 @@
 Название теста: ""
 Всего заданий в тесте: 2.
 Выполнено заданий: 1.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 2 возможных. Ваш результат: 0,0%.
@@ -608,8 +608,8 @@
 CRC Файла с тестом: "4F621F46"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 5 (16,7% выполненых заданий).
-Из них ошибок: 25 (83,3% выполненых заданий).
+Из них правильно: 5 (16,7% выполненных заданий).
+Из них ошибок: 25 (83,3% выполненных заданий).
 Результативность: 16,7%.
 Использовано подсказок: 0.
 Набрано баллов: 5,0 из 30 возможных. Ваш результат: 16,7%.
@@ -632,8 +632,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 5 (16,7% выполненых заданий).
-Из них ошибок: 25 (83,3% выполненых заданий).
+Из них правильно: 5 (16,7% выполненных заданий).
+Из них ошибок: 25 (83,3% выполненных заданий).
 Результативность: 16,7%.
 Использовано подсказок: 0.
 Набрано баллов: 5,0 из 30 возможных. Ваш результат: 16,7%.
@@ -661,10 +661,10 @@
     <t>30</t>
   </si>
   <si>
-    <t>5 (16,7% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>25 (83,3% выполненых заданий).</t>
+    <t>5 (16,7% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>25 (83,3% выполненных заданий).</t>
   </si>
   <si>
     <t>16,7%</t>
@@ -704,8 +704,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 7 (23,3% выполненых заданий).
-Из них ошибок: 23 (76,7% выполненых заданий).
+Из них правильно: 7 (23,3% выполненных заданий).
+Из них ошибок: 23 (76,7% выполненных заданий).
 Результативность: 23,3%.
 Использовано подсказок: 0.
 Набрано баллов: 7,0 из 30 возможных. Ваш результат: 23,3%.
@@ -728,8 +728,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 7 (23,3% выполненых заданий).
-Из них ошибок: 23 (76,7% выполненых заданий).
+Из них правильно: 7 (23,3% выполненных заданий).
+Из них ошибок: 23 (76,7% выполненных заданий).
 Результативность: 23,3%.
 Использовано подсказок: 0.
 Набрано баллов: 7,0 из 30 возможных. Ваш результат: 23,3%.
@@ -754,10 +754,10 @@
     <t>554B1E8C</t>
   </si>
   <si>
-    <t>7 (23,3% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>23 (76,7% выполненых заданий).</t>
+    <t>7 (23,3% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>23 (76,7% выполненных заданий).</t>
   </si>
   <si>
     <t>23,3%</t>
@@ -794,8 +794,8 @@
 CRC Файла с тестом: "4F621F46"
 Всего заданий в тесте: 30.
 Выполнено заданий: 1.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
@@ -818,8 +818,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 1.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
@@ -866,8 +866,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 2.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 1 (50,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 1 (50,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
@@ -890,8 +890,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 2.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 1 (50,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 1 (50,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
@@ -944,8 +944,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 1.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
@@ -968,8 +968,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 1.
-Из них правильно: 0 (0,0% выполненых заданий).
-Из них ошибок: 0 (0,0% выполненых заданий).
+Из них правильно: 0 (0,0% выполненных заданий).
+Из них ошибок: 0 (0,0% выполненных заданий).
 Результативность: 0,0%.
 Использовано подсказок: 0.
 Набрано баллов: 0,0 из 30 возможных. Ваш результат: 0,0%.
@@ -1010,8 +1010,8 @@
 CRC Файла с тестом: "4F621F46"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 8 (26,7% выполненых заданий).
-Из них ошибок: 22 (73,3% выполненых заданий).
+Из них правильно: 8 (26,7% выполненных заданий).
+Из них ошибок: 22 (73,3% выполненных заданий).
 Результативность: 26,7%.
 Использовано подсказок: 0.
 Набрано баллов: 8,0 из 30 возможных. Ваш результат: 26,7%.
@@ -1034,8 +1034,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 8 (26,7% выполненых заданий).
-Из них ошибок: 22 (73,3% выполненых заданий).
+Из них правильно: 8 (26,7% выполненных заданий).
+Из них ошибок: 22 (73,3% выполненных заданий).
 Результативность: 26,7%.
 Использовано подсказок: 0.
 Набрано баллов: 8,0 из 30 возможных. Ваш результат: 26,7%.
@@ -1051,10 +1051,10 @@
     <t>06.10.2021 15:01:45</t>
   </si>
   <si>
-    <t>8 (26,7% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>22 (73,3% выполненых заданий).</t>
+    <t>8 (26,7% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>22 (73,3% выполненных заданий).</t>
   </si>
   <si>
     <t>26,7%</t>
@@ -1091,8 +1091,8 @@
 CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 4 (13,3% выполненых заданий).
-Из них ошибок: 26 (86,7% выполненых заданий).
+Из них правильно: 4 (13,3% выполненных заданий).
+Из них ошибок: 26 (86,7% выполненных заданий).
 Результативность: 13,3%.
 Использовано подсказок: 0.
 Набрано баллов: 4,0 из 30 возможных. Ваш результат: 13,3%.
@@ -1115,8 +1115,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 4 (13,3% выполненых заданий).
-Из них ошибок: 26 (86,7% выполненых заданий).
+Из них правильно: 4 (13,3% выполненных заданий).
+Из них ошибок: 26 (86,7% выполненных заданий).
 Результативность: 13,3%.
 Использовано подсказок: 0.
 Набрано баллов: 4,0 из 30 возможных. Ваш результат: 13,3%.
@@ -1141,10 +1141,10 @@
     <t>5A416D2A</t>
   </si>
   <si>
-    <t>4 (13,3% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>26 (86,7% выполненых заданий).</t>
+    <t>4 (13,3% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>26 (86,7% выполненных заданий).</t>
   </si>
   <si>
     <t>13,3%</t>
@@ -1181,8 +1181,8 @@
 CRC Файла с тестом: "7AC88467"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 15 (50,0% выполненых заданий).
-Из них ошибок: 15 (50,0% выполненых заданий).
+Из них правильно: 15 (50,0% выполненных заданий).
+Из них ошибок: 15 (50,0% выполненных заданий).
 Результативность: 50,0%.
 Использовано подсказок: 0.
 Набрано баллов: 15,0 из 30 возможных. Ваш результат: 50,0%.
@@ -1205,8 +1205,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 15 (50,0% выполненых заданий).
-Из них ошибок: 15 (50,0% выполненых заданий).
+Из них правильно: 15 (50,0% выполненных заданий).
+Из них ошибок: 15 (50,0% выполненных заданий).
 Результативность: 50,0%.
 Использовано подсказок: 0.
 Набрано баллов: 15,0 из 30 возможных. Ваш результат: 50,0%.
@@ -1228,7 +1228,7 @@
     <t>7AC88467</t>
   </si>
   <si>
-    <t>15 (50,0% выполненых заданий).</t>
+    <t>15 (50,0% выполненных заданий).</t>
   </si>
   <si>
     <t>15,0 из 30 возможных. Ваш результат: 50,0%</t>
@@ -1262,8 +1262,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
@@ -1286,8 +1286,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
@@ -1309,10 +1309,10 @@
     <t>ОЗЕРОВА ЕЛИЗАВЕТА ДЕНИСОВНА</t>
   </si>
   <si>
-    <t>9 (30,0% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>21 (70,0% выполненых заданий).</t>
+    <t>9 (30,0% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>21 (70,0% выполненных заданий).</t>
   </si>
   <si>
     <t>30,0%</t>
@@ -1349,8 +1349,8 @@
 CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 17 (56,7% выполненых заданий).
-Из них ошибок: 13 (43,3% выполненых заданий).
+Из них правильно: 17 (56,7% выполненных заданий).
+Из них ошибок: 13 (43,3% выполненных заданий).
 Результативность: 56,7%.
 Использовано подсказок: 0.
 Набрано баллов: 17,0 из 30 возможных. Ваш результат: 56,7%.
@@ -1373,8 +1373,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 17 (56,7% выполненых заданий).
-Из них ошибок: 13 (43,3% выполненых заданий).
+Из них правильно: 17 (56,7% выполненных заданий).
+Из них ошибок: 13 (43,3% выполненных заданий).
 Результативность: 56,7%.
 Использовано подсказок: 0.
 Набрано баллов: 17,0 из 30 возможных. Ваш результат: 56,7%.
@@ -1396,10 +1396,10 @@
     <t>ЛОСКУТОВА</t>
   </si>
   <si>
-    <t>17 (56,7% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>13 (43,3% выполненых заданий).</t>
+    <t>17 (56,7% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>13 (43,3% выполненных заданий).</t>
   </si>
   <si>
     <t>56,7%</t>
@@ -1436,8 +1436,8 @@
 CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 23 (76,7% выполненых заданий).
-Из них ошибок: 7 (23,3% выполненых заданий).
+Из них правильно: 23 (76,7% выполненных заданий).
+Из них ошибок: 7 (23,3% выполненных заданий).
 Результативность: 76,7%.
 Использовано подсказок: 0.
 Набрано баллов: 23,0 из 30 возможных. Ваш результат: 76,7%.
@@ -1460,8 +1460,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 23 (76,7% выполненых заданий).
-Из них ошибок: 7 (23,3% выполненых заданий).
+Из них правильно: 23 (76,7% выполненных заданий).
+Из них ошибок: 7 (23,3% выполненных заданий).
 Результативность: 76,7%.
 Использовано подсказок: 0.
 Набрано баллов: 23,0 из 30 возможных. Ваш результат: 76,7%.
@@ -1517,8 +1517,8 @@
 CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 20 (66,7% выполненых заданий).
-Из них ошибок: 10 (33,3% выполненых заданий).
+Из них правильно: 20 (66,7% выполненных заданий).
+Из них ошибок: 10 (33,3% выполненных заданий).
 Результативность: 66,7%.
 Использовано подсказок: 0.
 Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
@@ -1541,8 +1541,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 20 (66,7% выполненых заданий).
-Из них ошибок: 10 (33,3% выполненых заданий).
+Из них правильно: 20 (66,7% выполненных заданий).
+Из них ошибок: 10 (33,3% выполненных заданий).
 Результативность: 66,7%.
 Использовано подсказок: 0.
 Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
@@ -1561,10 +1561,10 @@
     <t>РОМАНЦОВ ДМИТРИЙ ИЛЬИЧ</t>
   </si>
   <si>
-    <t>20 (66,7% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>10 (33,3% выполненых заданий).</t>
+    <t>20 (66,7% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>10 (33,3% выполненных заданий).</t>
   </si>
   <si>
     <t>66,7%</t>
@@ -1601,8 +1601,8 @@
 CRC Файла с тестом: "5A416D2A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 20 (66,7% выполненых заданий).
-Из них ошибок: 10 (33,3% выполненых заданий).
+Из них правильно: 20 (66,7% выполненных заданий).
+Из них ошибок: 10 (33,3% выполненных заданий).
 Результативность: 66,7%.
 Использовано подсказок: 0.
 Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
@@ -1625,8 +1625,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 20 (66,7% выполненых заданий).
-Из них ошибок: 10 (33,3% выполненых заданий).
+Из них правильно: 20 (66,7% выполненных заданий).
+Из них ошибок: 10 (33,3% выполненных заданий).
 Результативность: 66,7%.
 Использовано подсказок: 0.
 Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
@@ -1670,8 +1670,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 18 (60,0% выполненых заданий).
-Из них ошибок: 12 (40,0% выполненых заданий).
+Из них правильно: 18 (60,0% выполненных заданий).
+Из них ошибок: 12 (40,0% выполненных заданий).
 Результативность: 60,0%.
 Использовано подсказок: 0.
 Набрано баллов: 18,0 из 30 возможных. Ваш результат: 60,0%.
@@ -1694,8 +1694,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 18 (60,0% выполненых заданий).
-Из них ошибок: 12 (40,0% выполненых заданий).
+Из них правильно: 18 (60,0% выполненных заданий).
+Из них ошибок: 12 (40,0% выполненных заданий).
 Результативность: 60,0%.
 Использовано подсказок: 0.
 Набрано баллов: 18,0 из 30 возможных. Ваш результат: 60,0%.
@@ -1717,10 +1717,10 @@
     <t>БЕЛОУСОВА НАТАЛЬЯ</t>
   </si>
   <si>
-    <t>18 (60,0% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>12 (40,0% выполненых заданий).</t>
+    <t>18 (60,0% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>12 (40,0% выполненных заданий).</t>
   </si>
   <si>
     <t>60,0%</t>
@@ -1757,8 +1757,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 20 (66,7% выполненых заданий).
-Из них ошибок: 10 (33,3% выполненых заданий).
+Из них правильно: 20 (66,7% выполненных заданий).
+Из них ошибок: 10 (33,3% выполненных заданий).
 Результативность: 66,7%.
 Использовано подсказок: 0.
 Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
@@ -1781,8 +1781,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 20 (66,7% выполненых заданий).
-Из них ошибок: 10 (33,3% выполненых заданий).
+Из них правильно: 20 (66,7% выполненных заданий).
+Из них ошибок: 10 (33,3% выполненных заданий).
 Результативность: 66,7%.
 Использовано подсказок: 0.
 Набрано баллов: 20,0 из 30 возможных. Ваш результат: 66,7%.
@@ -1826,8 +1826,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
@@ -1850,8 +1850,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
@@ -1895,8 +1895,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 14 (46,7% выполненых заданий).
-Из них ошибок: 16 (53,3% выполненых заданий).
+Из них правильно: 14 (46,7% выполненных заданий).
+Из них ошибок: 16 (53,3% выполненных заданий).
 Результативность: 46,7%.
 Использовано подсказок: 0.
 Набрано баллов: 14,0 из 30 возможных. Ваш результат: 46,7%.
@@ -1919,8 +1919,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 14 (46,7% выполненых заданий).
-Из них ошибок: 16 (53,3% выполненых заданий).
+Из них правильно: 14 (46,7% выполненных заданий).
+Из них ошибок: 16 (53,3% выполненных заданий).
 Результативность: 46,7%.
 Использовано подсказок: 0.
 Набрано баллов: 14,0 из 30 возможных. Ваш результат: 46,7%.
@@ -1939,10 +1939,10 @@
     <t>КЕКИНА ЛЮДМИЛА ФЕДОРОВНА</t>
   </si>
   <si>
-    <t>14 (46,7% выполненых заданий).</t>
-  </si>
-  <si>
-    <t>16 (53,3% выполненых заданий).</t>
+    <t>14 (46,7% выполненных заданий).</t>
+  </si>
+  <si>
+    <t>16 (53,3% выполненных заданий).</t>
   </si>
   <si>
     <t>46,7%</t>
@@ -1979,8 +1979,8 @@
 CRC Файла с тестом: "2C7EB1D6"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 21 (70,0% выполненых заданий).
-Из них ошибок: 9 (30,0% выполненых заданий).
+Из них правильно: 21 (70,0% выполненных заданий).
+Из них ошибок: 9 (30,0% выполненных заданий).
 Результативность: 70,0%.
 Использовано подсказок: 0.
 Набрано баллов: 21,0 из 30 возможных. Ваш результат: 70,0%.
@@ -2003,8 +2003,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 21 (70,0% выполненых заданий).
-Из них ошибок: 9 (30,0% выполненых заданий).
+Из них правильно: 21 (70,0% выполненных заданий).
+Из них ошибок: 9 (30,0% выполненных заданий).
 Результативность: 70,0%.
 Использовано подсказок: 0.
 Набрано баллов: 21,0 из 30 возможных. Ваш результат: 70,0%.
@@ -2057,8 +2057,8 @@
 CRC Файла с тестом: "554B1E8C"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 7 (23,3% выполненых заданий).
-Из них ошибок: 23 (76,7% выполненых заданий).
+Из них правильно: 7 (23,3% выполненных заданий).
+Из них ошибок: 23 (76,7% выполненных заданий).
 Результативность: 23,3%.
 Использовано подсказок: 0.
 Набрано баллов: 7,0 из 30 возможных. Ваш результат: 23,3%.
@@ -2081,8 +2081,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 7 (23,3% выполненых заданий).
-Из них ошибок: 23 (76,7% выполненых заданий).
+Из них правильно: 7 (23,3% выполненных заданий).
+Из них ошибок: 23 (76,7% выполненных заданий).
 Результативность: 23,3%.
 Использовано подсказок: 0.
 Набрано баллов: 7,0 из 30 возможных. Ваш результат: 23,3%.
@@ -2126,8 +2126,8 @@
 CRC Файла с тестом: "1D498E48"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
@@ -2150,8 +2150,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
@@ -2201,8 +2201,8 @@
 CRC Файла с тестом: "A3C16E8A"
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.
@@ -2225,8 +2225,8 @@
 Название теста: ""
 Всего заданий в тесте: 30.
 Выполнено заданий: 30.
-Из них правильно: 9 (30,0% выполненых заданий).
-Из них ошибок: 21 (70,0% выполненых заданий).
+Из них правильно: 9 (30,0% выполненных заданий).
+Из них ошибок: 21 (70,0% выполненных заданий).
 Результативность: 30,0%.
 Использовано подсказок: 0.
 Набрано баллов: 9,0 из 30 возможных. Ваш результат: 30,0%.

</xml_diff>